<commit_message>
my picks locked page complete
</commit_message>
<xml_diff>
--- a/excel docs/java testing-audit info.xlsx
+++ b/excel docs/java testing-audit info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joecollins/Desktop/documents/personal-projects/world-cup-heroku/excel docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4229317-0112-7E4B-94A9-59A129A33562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955E9E9C-5152-CC49-861B-159195326AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15860" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -2616,7 +2616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86316F4E-9A6C-492E-9EDB-018A26A821E8}">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="P31" sqref="P31:P41"/>
     </sheetView>
   </sheetViews>
@@ -8190,7 +8190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61C1E5FA-F91B-4A41-A4C1-97D69E012813}">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="N41" sqref="N41"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
test specs updated with actual 2022 world cup info, css on knockout stage complete too
</commit_message>
<xml_diff>
--- a/excel docs/java testing-audit info.xlsx
+++ b/excel docs/java testing-audit info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joecollins/Desktop/documents/personal-projects/world-cup-heroku/excel docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955E9E9C-5152-CC49-861B-159195326AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3C4F44-B0A0-7141-B9F2-364CD5C25541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -21,10 +21,11 @@
     <sheet name="Kelly" sheetId="9" r:id="rId6"/>
     <sheet name="rules" sheetId="7" r:id="rId7"/>
     <sheet name="testing" sheetId="11" r:id="rId8"/>
-    <sheet name="tiebreaker testing" sheetId="12" r:id="rId9"/>
+    <sheet name="part tiebreaker testing" sheetId="12" r:id="rId9"/>
+    <sheet name="group tiebreaker testing" sheetId="14" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'tiebreaker testing'!$A$1:$G$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'part tiebreaker testing'!$A$1:$G$25</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="148">
   <si>
     <t>A1</t>
   </si>
@@ -642,12 +643,24 @@
   <si>
     <t>Stan</t>
   </si>
+  <si>
+    <t>Greatest number of points obtained in all of the group matches.</t>
+  </si>
+  <si>
+    <t>Goal Difference in all of the group matches.</t>
+  </si>
+  <si>
+    <t>Greatest number of goals scored in all group matches.</t>
+  </si>
+  <si>
+    <t>Points obtained in the group matches between teams concerned.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -708,6 +721,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1200,7 +1218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1447,24 +1465,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1474,6 +1492,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1498,18 +1528,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1534,15 +1552,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1581,6 +1599,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1900,11 +1922,11 @@
       <c r="F1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="87" t="s">
+      <c r="J1" s="84" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="88"/>
-      <c r="L1" s="89"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="86"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B2" s="14" t="s">
@@ -2224,7 +2246,7 @@
         <v>Ecuador</v>
       </c>
       <c r="C27" s="7"/>
-      <c r="D27" s="84" t="s">
+      <c r="D27" s="87" t="s">
         <v>134</v>
       </c>
       <c r="E27" s="7"/>
@@ -2238,7 +2260,7 @@
       <c r="M27" s="7"/>
       <c r="N27" s="7"/>
       <c r="O27" s="7"/>
-      <c r="P27" s="84" t="s">
+      <c r="P27" s="87" t="s">
         <v>41</v>
       </c>
       <c r="Q27" s="7"/>
@@ -2260,9 +2282,9 @@
         <v>Iran</v>
       </c>
       <c r="C28" s="7"/>
-      <c r="D28" s="86"/>
+      <c r="D28" s="88"/>
       <c r="E28" s="7"/>
-      <c r="F28" s="84" t="s">
+      <c r="F28" s="87" t="s">
         <v>25</v>
       </c>
       <c r="G28" s="7"/>
@@ -2272,11 +2294,11 @@
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
       <c r="M28" s="7"/>
-      <c r="N28" s="84" t="s">
+      <c r="N28" s="87" t="s">
         <v>34</v>
       </c>
       <c r="O28" s="7"/>
-      <c r="P28" s="86"/>
+      <c r="P28" s="88"/>
       <c r="Q28" s="7"/>
       <c r="R28" s="15" t="str">
         <f>B3</f>
@@ -2293,7 +2315,7 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
-      <c r="F29" s="85"/>
+      <c r="F29" s="89"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
@@ -2301,7 +2323,7 @@
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
-      <c r="N29" s="85"/>
+      <c r="N29" s="89"/>
       <c r="O29" s="7"/>
       <c r="P29" s="7"/>
       <c r="Q29" s="7"/>
@@ -2318,11 +2340,11 @@
         <v>Argentina</v>
       </c>
       <c r="C30" s="7"/>
-      <c r="D30" s="84" t="s">
+      <c r="D30" s="87" t="s">
         <v>25</v>
       </c>
       <c r="E30" s="7"/>
-      <c r="F30" s="86"/>
+      <c r="F30" s="88"/>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
@@ -2330,9 +2352,9 @@
       <c r="K30" s="7"/>
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
-      <c r="N30" s="86"/>
+      <c r="N30" s="88"/>
       <c r="O30" s="7"/>
-      <c r="P30" s="84" t="s">
+      <c r="P30" s="87" t="s">
         <v>34</v>
       </c>
       <c r="Q30" s="7"/>
@@ -2354,7 +2376,7 @@
         <v>France</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="86"/>
+      <c r="D31" s="88"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
@@ -2370,7 +2392,7 @@
       <c r="M31" s="7"/>
       <c r="N31" s="7"/>
       <c r="O31" s="7"/>
-      <c r="P31" s="86"/>
+      <c r="P31" s="88"/>
       <c r="Q31" s="7"/>
       <c r="R31" s="15" t="str">
         <f>B9</f>
@@ -2414,7 +2436,7 @@
         <v>Italy</v>
       </c>
       <c r="C33" s="7"/>
-      <c r="D33" s="84" t="s">
+      <c r="D33" s="87" t="s">
         <v>139</v>
       </c>
       <c r="E33" s="7"/>
@@ -2428,7 +2450,7 @@
       <c r="M33" s="7"/>
       <c r="N33" s="7"/>
       <c r="O33" s="7"/>
-      <c r="P33" s="84" t="s">
+      <c r="P33" s="87" t="s">
         <v>14</v>
       </c>
       <c r="Q33" s="7"/>
@@ -2450,9 +2472,9 @@
         <v>Canada</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="86"/>
+      <c r="D34" s="88"/>
       <c r="E34" s="7"/>
-      <c r="F34" s="84" t="s">
+      <c r="F34" s="87" t="s">
         <v>12</v>
       </c>
       <c r="G34" s="7"/>
@@ -2462,11 +2484,11 @@
       <c r="K34" s="7"/>
       <c r="L34" s="7"/>
       <c r="M34" s="7"/>
-      <c r="N34" s="84" t="s">
+      <c r="N34" s="87" t="s">
         <v>14</v>
       </c>
       <c r="O34" s="7"/>
-      <c r="P34" s="86"/>
+      <c r="P34" s="88"/>
       <c r="Q34" s="7"/>
       <c r="R34" s="15" t="str">
         <f>B15</f>
@@ -2483,7 +2505,7 @@
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
-      <c r="F35" s="85"/>
+      <c r="F35" s="89"/>
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
@@ -2491,7 +2513,7 @@
       <c r="K35" s="7"/>
       <c r="L35" s="7"/>
       <c r="M35" s="7"/>
-      <c r="N35" s="85"/>
+      <c r="N35" s="89"/>
       <c r="O35" s="7"/>
       <c r="P35" s="7"/>
       <c r="Q35" s="7"/>
@@ -2508,11 +2530,11 @@
         <v>Brasil</v>
       </c>
       <c r="C36" s="7"/>
-      <c r="D36" s="84" t="s">
+      <c r="D36" s="87" t="s">
         <v>12</v>
       </c>
       <c r="E36" s="7"/>
-      <c r="F36" s="86"/>
+      <c r="F36" s="88"/>
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
       <c r="I36" s="7"/>
@@ -2520,9 +2542,9 @@
       <c r="K36" s="7"/>
       <c r="L36" s="7"/>
       <c r="M36" s="7"/>
-      <c r="N36" s="86"/>
+      <c r="N36" s="88"/>
       <c r="O36" s="7"/>
-      <c r="P36" s="84" t="s">
+      <c r="P36" s="87" t="s">
         <v>137</v>
       </c>
       <c r="Q36" s="7"/>
@@ -2544,7 +2566,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="86"/>
+      <c r="D37" s="88"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
@@ -2556,7 +2578,7 @@
       <c r="M37" s="7"/>
       <c r="N37" s="7"/>
       <c r="O37" s="7"/>
-      <c r="P37" s="86"/>
+      <c r="P37" s="88"/>
       <c r="Q37" s="7"/>
       <c r="R37" s="15" t="str">
         <f>B21</f>
@@ -2591,6 +2613,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="N28:N30"/>
+    <mergeCell ref="N34:N36"/>
+    <mergeCell ref="P27:P28"/>
+    <mergeCell ref="P30:P31"/>
+    <mergeCell ref="P33:P34"/>
+    <mergeCell ref="P36:P37"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="D27:D28"/>
     <mergeCell ref="D30:D31"/>
@@ -2600,15 +2628,53 @@
     <mergeCell ref="F34:F36"/>
     <mergeCell ref="H31:H33"/>
     <mergeCell ref="L31:L33"/>
-    <mergeCell ref="N28:N30"/>
-    <mergeCell ref="N34:N36"/>
-    <mergeCell ref="P27:P28"/>
-    <mergeCell ref="P30:P31"/>
-    <mergeCell ref="P33:P34"/>
-    <mergeCell ref="P36:P37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A13F6EC-BC2A-504C-A071-8460572D194C}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="189" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="63" x14ac:dyDescent="0.2">
+      <c r="A1" s="130" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="42" x14ac:dyDescent="0.2">
+      <c r="A2" s="130" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="63" x14ac:dyDescent="0.2">
+      <c r="A3" s="130" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="63" x14ac:dyDescent="0.2">
+      <c r="A4" s="130" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="129"/>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="129"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2616,8 +2682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86316F4E-9A6C-492E-9EDB-018A26A821E8}">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31:P41"/>
+    <sheetView topLeftCell="O1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2648,26 +2714,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="89"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="86"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="87" t="s">
+      <c r="J1" s="84" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="88"/>
-      <c r="N1" s="89"/>
-      <c r="P1" s="87" t="s">
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="86"/>
+      <c r="P1" s="84" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="88"/>
-      <c r="R1" s="89"/>
+      <c r="Q1" s="85"/>
+      <c r="R1" s="86"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -2870,23 +2936,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="101" t="s">
+      <c r="B8" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="102"/>
-      <c r="D8" s="102"/>
-      <c r="E8" s="102"/>
-      <c r="F8" s="103"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="94"/>
+      <c r="E8" s="94"/>
+      <c r="F8" s="95"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="101" t="s">
+      <c r="J8" s="93" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="102"/>
-      <c r="L8" s="102"/>
-      <c r="M8" s="102"/>
-      <c r="N8" s="103"/>
+      <c r="K8" s="94"/>
+      <c r="L8" s="94"/>
+      <c r="M8" s="94"/>
+      <c r="N8" s="95"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -3076,23 +3142,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="101" t="s">
+      <c r="B15" s="93" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="102"/>
-      <c r="D15" s="102"/>
-      <c r="E15" s="102"/>
-      <c r="F15" s="103"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="95"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="101" t="s">
+      <c r="J15" s="93" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="102"/>
-      <c r="L15" s="102"/>
-      <c r="M15" s="102"/>
-      <c r="N15" s="103"/>
+      <c r="K15" s="94"/>
+      <c r="L15" s="94"/>
+      <c r="M15" s="94"/>
+      <c r="N15" s="95"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -3213,10 +3279,10 @@
         <f t="shared" ref="N19:N20" si="5">IF(J19=L19,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Q19" s="104" t="s">
+      <c r="Q19" s="96" t="s">
         <v>82</v>
       </c>
-      <c r="R19" s="104"/>
+      <c r="R19" s="96"/>
     </row>
     <row r="20" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="27" t="s">
@@ -3271,23 +3337,23 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="101" t="s">
+      <c r="B22" s="93" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="102"/>
-      <c r="D22" s="102"/>
-      <c r="E22" s="102"/>
-      <c r="F22" s="103"/>
+      <c r="C22" s="94"/>
+      <c r="D22" s="94"/>
+      <c r="E22" s="94"/>
+      <c r="F22" s="95"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="101" t="s">
+      <c r="J22" s="93" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="102"/>
-      <c r="L22" s="102"/>
-      <c r="M22" s="102"/>
-      <c r="N22" s="103"/>
+      <c r="K22" s="94"/>
+      <c r="L22" s="94"/>
+      <c r="M22" s="94"/>
+      <c r="N22" s="95"/>
       <c r="Q22" s="49"/>
       <c r="R22" s="32" t="s">
         <v>85</v>
@@ -3518,7 +3584,7 @@
         <v>Ecuador</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="96" t="s">
+      <c r="D31" s="100" t="s">
         <v>134</v>
       </c>
       <c r="E31" s="7"/>
@@ -3536,7 +3602,7 @@
         <v>79</v>
       </c>
       <c r="O31" s="7"/>
-      <c r="P31" s="96" t="s">
+      <c r="P31" s="100" t="s">
         <v>41</v>
       </c>
       <c r="Q31" s="7"/>
@@ -3558,12 +3624,12 @@
         <v>Iran</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="97"/>
+      <c r="D32" s="101"/>
       <c r="E32" s="23">
         <f>IF(D31=Master!D27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F32" s="96" t="s">
+      <c r="F32" s="100" t="s">
         <v>25</v>
       </c>
       <c r="G32" s="7"/>
@@ -3573,14 +3639,14 @@
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
-      <c r="N32" s="96" t="s">
+      <c r="N32" s="100" t="s">
         <v>34</v>
       </c>
       <c r="O32" s="23">
         <f>IF(P31=Master!P27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P32" s="97"/>
+      <c r="P32" s="101"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="39" t="str">
         <f>D4</f>
@@ -3599,7 +3665,7 @@
         <v>70</v>
       </c>
       <c r="E33" s="7"/>
-      <c r="F33" s="98"/>
+      <c r="F33" s="102"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
@@ -3607,7 +3673,7 @@
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
-      <c r="N33" s="98"/>
+      <c r="N33" s="102"/>
       <c r="O33" s="7"/>
       <c r="P33" s="35"/>
       <c r="Q33" s="7"/>
@@ -3624,14 +3690,14 @@
         <v>Argentina</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="96" t="s">
+      <c r="D34" s="100" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="23">
         <f>IF(D34=Master!D30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F34" s="97"/>
+      <c r="F34" s="101"/>
       <c r="G34" s="23">
         <f>IF(F32=Master!F28,4,0)</f>
         <v>4</v>
@@ -3649,12 +3715,12 @@
         <f>IF(N32=Master!N28,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N34" s="97"/>
+      <c r="N34" s="101"/>
       <c r="O34" s="23">
         <f>IF(P34=Master!P30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P34" s="96" t="s">
+      <c r="P34" s="100" t="s">
         <v>34</v>
       </c>
       <c r="Q34" s="7"/>
@@ -3676,11 +3742,11 @@
         <v>France</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="97"/>
+      <c r="D35" s="101"/>
       <c r="E35" s="7"/>
       <c r="F35" s="35"/>
       <c r="G35" s="7"/>
-      <c r="H35" s="96" t="s">
+      <c r="H35" s="100" t="s">
         <v>25</v>
       </c>
       <c r="I35" s="7"/>
@@ -3688,13 +3754,13 @@
         <v>81</v>
       </c>
       <c r="K35" s="7"/>
-      <c r="L35" s="96" t="s">
+      <c r="L35" s="100" t="s">
         <v>14</v>
       </c>
       <c r="M35" s="7"/>
       <c r="N35" s="35"/>
       <c r="O35" s="7"/>
-      <c r="P35" s="97"/>
+      <c r="P35" s="101"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="39" t="str">
         <f>D11</f>
@@ -3715,7 +3781,7 @@
       <c r="E36" s="7"/>
       <c r="F36" s="35"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="98"/>
+      <c r="H36" s="102"/>
       <c r="I36" s="24">
         <f>IF(H35=Master!H31,6,0)</f>
         <v>6</v>
@@ -3727,7 +3793,7 @@
         <f>IF(L35=Master!L31,6,0)</f>
         <v>6</v>
       </c>
-      <c r="L36" s="98"/>
+      <c r="L36" s="102"/>
       <c r="M36" s="7"/>
       <c r="N36" s="35"/>
       <c r="O36" s="7"/>
@@ -3748,7 +3814,7 @@
         <v>Italy</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="99" t="s">
+      <c r="D37" s="103" t="s">
         <v>139</v>
       </c>
       <c r="E37" s="7"/>
@@ -3756,17 +3822,17 @@
         <v>78</v>
       </c>
       <c r="G37" s="7"/>
-      <c r="H37" s="97"/>
+      <c r="H37" s="101"/>
       <c r="I37" s="7"/>
       <c r="J37" s="35"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="97"/>
+      <c r="L37" s="101"/>
       <c r="M37" s="7"/>
       <c r="N37" s="35" t="s">
         <v>80</v>
       </c>
       <c r="O37" s="7"/>
-      <c r="P37" s="96" t="s">
+      <c r="P37" s="100" t="s">
         <v>14</v>
       </c>
       <c r="Q37" s="7"/>
@@ -3788,12 +3854,12 @@
         <v>Canada</v>
       </c>
       <c r="C38" s="7"/>
-      <c r="D38" s="100"/>
+      <c r="D38" s="104"/>
       <c r="E38" s="23">
         <f>IF(D37=Master!D33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F38" s="93" t="s">
+      <c r="F38" s="97" t="s">
         <v>12</v>
       </c>
       <c r="G38" s="23">
@@ -3812,14 +3878,14 @@
         <f>IF(N38=Master!N34,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N38" s="96" t="s">
+      <c r="N38" s="100" t="s">
         <v>14</v>
       </c>
       <c r="O38" s="23">
         <f>IF(P37=Master!P33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P38" s="97"/>
+      <c r="P38" s="101"/>
       <c r="Q38" s="7"/>
       <c r="R38" s="39" t="str">
         <f>D18</f>
@@ -3838,7 +3904,7 @@
         <v>72</v>
       </c>
       <c r="E39" s="7"/>
-      <c r="F39" s="94"/>
+      <c r="F39" s="98"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
@@ -3846,7 +3912,7 @@
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
-      <c r="N39" s="98"/>
+      <c r="N39" s="102"/>
       <c r="O39" s="7"/>
       <c r="P39" s="35" t="s">
         <v>76</v>
@@ -3865,14 +3931,14 @@
         <v>Brasil</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="96" t="s">
+      <c r="D40" s="100" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="23">
         <f>IF(D40=Master!D36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F40" s="95"/>
+      <c r="F40" s="99"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
@@ -3880,12 +3946,12 @@
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
-      <c r="N40" s="97"/>
+      <c r="N40" s="101"/>
       <c r="O40" s="23">
         <f>IF(P40=Master!P36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P40" s="96" t="s">
+      <c r="P40" s="100" t="s">
         <v>137</v>
       </c>
       <c r="Q40" s="7"/>
@@ -3907,7 +3973,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="97"/>
+      <c r="D41" s="101"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -3919,7 +3985,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="97"/>
+      <c r="P41" s="101"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="39" t="str">
         <f>D25</f>
@@ -3987,16 +4053,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J22:N22"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="J8:N8"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="Q19:R19"/>
     <mergeCell ref="F38:F40"/>
     <mergeCell ref="P37:P38"/>
     <mergeCell ref="P40:P41"/>
@@ -4011,6 +4067,16 @@
     <mergeCell ref="D37:D38"/>
     <mergeCell ref="H35:H37"/>
     <mergeCell ref="L35:L37"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J22:N22"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="Q19:R19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -4053,26 +4119,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="89"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="86"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="87" t="s">
+      <c r="J1" s="84" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="88"/>
-      <c r="N1" s="89"/>
-      <c r="P1" s="87" t="s">
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="86"/>
+      <c r="P1" s="84" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="88"/>
-      <c r="R1" s="89"/>
+      <c r="Q1" s="85"/>
+      <c r="R1" s="86"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -4275,23 +4341,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="101" t="s">
+      <c r="B8" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="102"/>
-      <c r="D8" s="102"/>
-      <c r="E8" s="102"/>
-      <c r="F8" s="103"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="94"/>
+      <c r="E8" s="94"/>
+      <c r="F8" s="95"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="101" t="s">
+      <c r="J8" s="93" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="102"/>
-      <c r="L8" s="102"/>
-      <c r="M8" s="102"/>
-      <c r="N8" s="103"/>
+      <c r="K8" s="94"/>
+      <c r="L8" s="94"/>
+      <c r="M8" s="94"/>
+      <c r="N8" s="95"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -4481,23 +4547,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="101" t="s">
+      <c r="B15" s="93" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="102"/>
-      <c r="D15" s="102"/>
-      <c r="E15" s="102"/>
-      <c r="F15" s="103"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="95"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="101" t="s">
+      <c r="J15" s="93" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="102"/>
-      <c r="L15" s="102"/>
-      <c r="M15" s="102"/>
-      <c r="N15" s="103"/>
+      <c r="K15" s="94"/>
+      <c r="L15" s="94"/>
+      <c r="M15" s="94"/>
+      <c r="N15" s="95"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -4618,10 +4684,10 @@
         <f t="shared" ref="N19:N20" si="5">IF(J19=L19,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Q19" s="104" t="s">
+      <c r="Q19" s="96" t="s">
         <v>82</v>
       </c>
-      <c r="R19" s="104"/>
+      <c r="R19" s="96"/>
     </row>
     <row r="20" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="27" t="s">
@@ -4676,23 +4742,23 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="101" t="s">
+      <c r="B22" s="93" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="102"/>
-      <c r="D22" s="102"/>
-      <c r="E22" s="102"/>
-      <c r="F22" s="103"/>
+      <c r="C22" s="94"/>
+      <c r="D22" s="94"/>
+      <c r="E22" s="94"/>
+      <c r="F22" s="95"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="101" t="s">
+      <c r="J22" s="93" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="102"/>
-      <c r="L22" s="102"/>
-      <c r="M22" s="102"/>
-      <c r="N22" s="103"/>
+      <c r="K22" s="94"/>
+      <c r="L22" s="94"/>
+      <c r="M22" s="94"/>
+      <c r="N22" s="95"/>
       <c r="Q22" s="49"/>
       <c r="R22" s="32" t="s">
         <v>85</v>
@@ -4923,7 +4989,7 @@
         <v>Ecuador</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="96" t="s">
+      <c r="D31" s="100" t="s">
         <v>134</v>
       </c>
       <c r="E31" s="7"/>
@@ -4941,7 +5007,7 @@
         <v>79</v>
       </c>
       <c r="O31" s="7"/>
-      <c r="P31" s="96" t="s">
+      <c r="P31" s="100" t="s">
         <v>41</v>
       </c>
       <c r="Q31" s="7"/>
@@ -4963,12 +5029,12 @@
         <v>Iran</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="97"/>
+      <c r="D32" s="101"/>
       <c r="E32" s="23">
         <f>IF(D31=Master!D27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F32" s="96" t="s">
+      <c r="F32" s="100" t="s">
         <v>25</v>
       </c>
       <c r="G32" s="7"/>
@@ -4978,14 +5044,14 @@
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
-      <c r="N32" s="96" t="s">
+      <c r="N32" s="100" t="s">
         <v>34</v>
       </c>
       <c r="O32" s="23">
         <f>IF(P31=Master!P27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P32" s="97"/>
+      <c r="P32" s="101"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="81" t="str">
         <f>D4</f>
@@ -5004,7 +5070,7 @@
         <v>70</v>
       </c>
       <c r="E33" s="7"/>
-      <c r="F33" s="98"/>
+      <c r="F33" s="102"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
@@ -5012,7 +5078,7 @@
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
-      <c r="N33" s="98"/>
+      <c r="N33" s="102"/>
       <c r="O33" s="7"/>
       <c r="P33" s="35"/>
       <c r="Q33" s="7"/>
@@ -5029,14 +5095,14 @@
         <v>Argentina</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="96" t="s">
+      <c r="D34" s="100" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="23">
         <f>IF(D34=Master!D30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F34" s="97"/>
+      <c r="F34" s="101"/>
       <c r="G34" s="23">
         <f>IF(F32=Master!F28,4,0)</f>
         <v>4</v>
@@ -5054,12 +5120,12 @@
         <f>IF(N32=Master!N28,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N34" s="97"/>
+      <c r="N34" s="101"/>
       <c r="O34" s="23">
         <f>IF(P34=Master!P30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P34" s="96" t="s">
+      <c r="P34" s="100" t="s">
         <v>34</v>
       </c>
       <c r="Q34" s="7"/>
@@ -5081,11 +5147,11 @@
         <v>France</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="97"/>
+      <c r="D35" s="101"/>
       <c r="E35" s="7"/>
       <c r="F35" s="35"/>
       <c r="G35" s="7"/>
-      <c r="H35" s="96" t="s">
+      <c r="H35" s="100" t="s">
         <v>25</v>
       </c>
       <c r="I35" s="7"/>
@@ -5093,13 +5159,13 @@
         <v>81</v>
       </c>
       <c r="K35" s="7"/>
-      <c r="L35" s="96" t="s">
+      <c r="L35" s="100" t="s">
         <v>14</v>
       </c>
       <c r="M35" s="7"/>
       <c r="N35" s="35"/>
       <c r="O35" s="7"/>
-      <c r="P35" s="97"/>
+      <c r="P35" s="101"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="81" t="str">
         <f>D11</f>
@@ -5120,7 +5186,7 @@
       <c r="E36" s="7"/>
       <c r="F36" s="35"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="98"/>
+      <c r="H36" s="102"/>
       <c r="I36" s="24">
         <f>IF(H35=Master!H31,6,0)</f>
         <v>6</v>
@@ -5132,7 +5198,7 @@
         <f>IF(L35=Master!L31,6,0)</f>
         <v>6</v>
       </c>
-      <c r="L36" s="98"/>
+      <c r="L36" s="102"/>
       <c r="M36" s="7"/>
       <c r="N36" s="35"/>
       <c r="O36" s="7"/>
@@ -5153,7 +5219,7 @@
         <v>Italy</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="99" t="s">
+      <c r="D37" s="103" t="s">
         <v>139</v>
       </c>
       <c r="E37" s="7"/>
@@ -5161,17 +5227,17 @@
         <v>78</v>
       </c>
       <c r="G37" s="7"/>
-      <c r="H37" s="97"/>
+      <c r="H37" s="101"/>
       <c r="I37" s="7"/>
       <c r="J37" s="35"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="97"/>
+      <c r="L37" s="101"/>
       <c r="M37" s="7"/>
       <c r="N37" s="35" t="s">
         <v>80</v>
       </c>
       <c r="O37" s="7"/>
-      <c r="P37" s="96" t="s">
+      <c r="P37" s="100" t="s">
         <v>14</v>
       </c>
       <c r="Q37" s="7"/>
@@ -5193,12 +5259,12 @@
         <v>Canada</v>
       </c>
       <c r="C38" s="7"/>
-      <c r="D38" s="100"/>
+      <c r="D38" s="104"/>
       <c r="E38" s="23">
         <f>IF(D37=Master!D33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F38" s="93" t="s">
+      <c r="F38" s="97" t="s">
         <v>12</v>
       </c>
       <c r="G38" s="23">
@@ -5217,14 +5283,14 @@
         <f>IF(N38=Master!N34,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N38" s="96" t="s">
+      <c r="N38" s="100" t="s">
         <v>14</v>
       </c>
       <c r="O38" s="23">
         <f>IF(P37=Master!P33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P38" s="97"/>
+      <c r="P38" s="101"/>
       <c r="Q38" s="7"/>
       <c r="R38" s="81" t="str">
         <f>D18</f>
@@ -5243,7 +5309,7 @@
         <v>72</v>
       </c>
       <c r="E39" s="7"/>
-      <c r="F39" s="94"/>
+      <c r="F39" s="98"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
@@ -5251,7 +5317,7 @@
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
-      <c r="N39" s="98"/>
+      <c r="N39" s="102"/>
       <c r="O39" s="7"/>
       <c r="P39" s="35" t="s">
         <v>76</v>
@@ -5270,14 +5336,14 @@
         <v>Brasil</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="96" t="s">
+      <c r="D40" s="100" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="23">
         <f>IF(D40=Master!D36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F40" s="95"/>
+      <c r="F40" s="99"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
@@ -5285,12 +5351,12 @@
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
-      <c r="N40" s="97"/>
+      <c r="N40" s="101"/>
       <c r="O40" s="23">
         <f>IF(P40=Master!P36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P40" s="96" t="s">
+      <c r="P40" s="100" t="s">
         <v>137</v>
       </c>
       <c r="Q40" s="7"/>
@@ -5312,7 +5378,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="97"/>
+      <c r="D41" s="101"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -5324,7 +5390,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="97"/>
+      <c r="P41" s="101"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="81" t="str">
         <f>D25</f>
@@ -5392,6 +5458,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J1:N1"/>
     <mergeCell ref="P40:P41"/>
     <mergeCell ref="Q19:R19"/>
     <mergeCell ref="B22:F22"/>
@@ -5408,14 +5482,6 @@
     <mergeCell ref="P37:P38"/>
     <mergeCell ref="F38:F40"/>
     <mergeCell ref="N38:N40"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="J8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -5426,8 +5492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C64DF09A-2D3C-4C49-8B16-319C8D3CEDC7}">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+    <sheetView topLeftCell="A23" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3:R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5455,26 +5521,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="89"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="86"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="87" t="s">
+      <c r="J1" s="84" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="88"/>
-      <c r="N1" s="89"/>
-      <c r="P1" s="87" t="s">
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="86"/>
+      <c r="P1" s="84" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="88"/>
-      <c r="R1" s="89"/>
+      <c r="Q1" s="85"/>
+      <c r="R1" s="86"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -5677,23 +5743,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="101" t="s">
+      <c r="B8" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="102"/>
-      <c r="D8" s="102"/>
-      <c r="E8" s="102"/>
-      <c r="F8" s="103"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="94"/>
+      <c r="E8" s="94"/>
+      <c r="F8" s="95"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="101" t="s">
+      <c r="J8" s="93" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="102"/>
-      <c r="L8" s="102"/>
-      <c r="M8" s="102"/>
-      <c r="N8" s="103"/>
+      <c r="K8" s="94"/>
+      <c r="L8" s="94"/>
+      <c r="M8" s="94"/>
+      <c r="N8" s="95"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -5883,23 +5949,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="101" t="s">
+      <c r="B15" s="93" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="102"/>
-      <c r="D15" s="102"/>
-      <c r="E15" s="102"/>
-      <c r="F15" s="103"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="95"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="101" t="s">
+      <c r="J15" s="93" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="102"/>
-      <c r="L15" s="102"/>
-      <c r="M15" s="102"/>
-      <c r="N15" s="103"/>
+      <c r="K15" s="94"/>
+      <c r="L15" s="94"/>
+      <c r="M15" s="94"/>
+      <c r="N15" s="95"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -6064,23 +6130,23 @@
       <c r="N21" s="52"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="101" t="s">
+      <c r="B22" s="93" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="102"/>
-      <c r="D22" s="102"/>
-      <c r="E22" s="102"/>
-      <c r="F22" s="103"/>
+      <c r="C22" s="94"/>
+      <c r="D22" s="94"/>
+      <c r="E22" s="94"/>
+      <c r="F22" s="95"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="101" t="s">
+      <c r="J22" s="93" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="102"/>
-      <c r="L22" s="102"/>
-      <c r="M22" s="102"/>
-      <c r="N22" s="103"/>
+      <c r="K22" s="94"/>
+      <c r="L22" s="94"/>
+      <c r="M22" s="94"/>
+      <c r="N22" s="95"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B23" s="56" t="s">
@@ -6136,8 +6202,7 @@
       </c>
       <c r="M24" s="51"/>
       <c r="N24" s="34">
-        <f>IF(J24=L24,3, IF(J24=L25,1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
@@ -6167,8 +6232,7 @@
       </c>
       <c r="M25" s="51"/>
       <c r="N25" s="34">
-        <f>IF(J25=L25,2, IF(J25=L24,1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
@@ -6321,7 +6385,7 @@
         <v>79</v>
       </c>
       <c r="O31" s="7"/>
-      <c r="P31" s="96" t="s">
+      <c r="P31" s="100" t="s">
         <v>41</v>
       </c>
       <c r="Q31" s="7"/>
@@ -6365,7 +6429,7 @@
         <f>IF(P31=Master!P27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P32" s="97"/>
+      <c r="P32" s="101"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="39" t="str">
         <f>D4</f>
@@ -6411,7 +6475,7 @@
         <v>Argentina</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="96" t="s">
+      <c r="D34" s="100" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="23">
@@ -6441,7 +6505,7 @@
         <f>IF(P34=Master!P30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P34" s="96" t="s">
+      <c r="P34" s="100" t="s">
         <v>34</v>
       </c>
       <c r="Q34" s="7"/>
@@ -6463,7 +6527,7 @@
         <v>France</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="97"/>
+      <c r="D35" s="101"/>
       <c r="E35" s="7"/>
       <c r="F35" s="35"/>
       <c r="G35" s="7"/>
@@ -6481,7 +6545,7 @@
       <c r="M35" s="7"/>
       <c r="N35" s="35"/>
       <c r="O35" s="7"/>
-      <c r="P35" s="97"/>
+      <c r="P35" s="101"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="39" t="str">
         <f>D11</f>
@@ -6535,7 +6599,7 @@
         <v>Italy</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="99" t="s">
+      <c r="D37" s="103" t="s">
         <v>139</v>
       </c>
       <c r="E37" s="7"/>
@@ -6575,7 +6639,7 @@
         <v>Canada</v>
       </c>
       <c r="C38" s="7"/>
-      <c r="D38" s="100"/>
+      <c r="D38" s="104"/>
       <c r="E38" s="23">
         <f>IF(D37=Master!D33,2,0)</f>
         <v>2</v>
@@ -6652,7 +6716,7 @@
         <v>Brasil</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="96" t="s">
+      <c r="D40" s="100" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="23">
@@ -6672,7 +6736,7 @@
         <f>IF(P40=Master!P36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P40" s="96" t="s">
+      <c r="P40" s="100" t="s">
         <v>137</v>
       </c>
       <c r="Q40" s="7"/>
@@ -6694,7 +6758,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="97"/>
+      <c r="D41" s="101"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -6706,7 +6770,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="97"/>
+      <c r="P41" s="101"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="39" t="str">
         <f>D25</f>
@@ -6774,6 +6838,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="J8:N8"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="D31:D32"/>
@@ -6790,13 +6861,6 @@
     <mergeCell ref="N38:N40"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="P40:P41"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="J8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -6807,8 +6871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB731263-BF9E-B94A-B168-4AE30BA7699C}">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="N41" sqref="N41"/>
+    <sheetView topLeftCell="A20" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3:R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6836,26 +6900,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="89"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="86"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="87" t="s">
+      <c r="J1" s="84" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="88"/>
-      <c r="N1" s="89"/>
-      <c r="P1" s="87" t="s">
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="86"/>
+      <c r="P1" s="84" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="88"/>
-      <c r="R1" s="89"/>
+      <c r="Q1" s="85"/>
+      <c r="R1" s="86"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -7058,23 +7122,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="101" t="s">
+      <c r="B8" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="102"/>
-      <c r="D8" s="102"/>
-      <c r="E8" s="102"/>
-      <c r="F8" s="103"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="94"/>
+      <c r="E8" s="94"/>
+      <c r="F8" s="95"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="101" t="s">
+      <c r="J8" s="93" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="102"/>
-      <c r="L8" s="102"/>
-      <c r="M8" s="102"/>
-      <c r="N8" s="103"/>
+      <c r="K8" s="94"/>
+      <c r="L8" s="94"/>
+      <c r="M8" s="94"/>
+      <c r="N8" s="95"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -7264,23 +7328,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="101" t="s">
+      <c r="B15" s="93" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="102"/>
-      <c r="D15" s="102"/>
-      <c r="E15" s="102"/>
-      <c r="F15" s="103"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="95"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="101" t="s">
+      <c r="J15" s="93" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="102"/>
-      <c r="L15" s="102"/>
-      <c r="M15" s="102"/>
-      <c r="N15" s="103"/>
+      <c r="K15" s="94"/>
+      <c r="L15" s="94"/>
+      <c r="M15" s="94"/>
+      <c r="N15" s="95"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -7447,23 +7511,23 @@
       <c r="N21" s="52"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="101" t="s">
+      <c r="B22" s="93" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="102"/>
-      <c r="D22" s="102"/>
-      <c r="E22" s="102"/>
-      <c r="F22" s="103"/>
+      <c r="C22" s="94"/>
+      <c r="D22" s="94"/>
+      <c r="E22" s="94"/>
+      <c r="F22" s="95"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="101" t="s">
+      <c r="J22" s="93" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="102"/>
-      <c r="L22" s="102"/>
-      <c r="M22" s="102"/>
-      <c r="N22" s="103"/>
+      <c r="K22" s="94"/>
+      <c r="L22" s="94"/>
+      <c r="M22" s="94"/>
+      <c r="N22" s="95"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B23" s="56" t="s">
@@ -7918,7 +7982,7 @@
         <v>Italy</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="114" t="s">
+      <c r="D37" s="113" t="s">
         <v>136</v>
       </c>
       <c r="E37" s="7"/>
@@ -7958,7 +8022,7 @@
         <v>Canada</v>
       </c>
       <c r="C38" s="7"/>
-      <c r="D38" s="115"/>
+      <c r="D38" s="114"/>
       <c r="E38" s="23">
         <f>IF(D37=Master!D33,2,0)</f>
         <v>0</v>
@@ -8008,7 +8072,7 @@
         <v>72</v>
       </c>
       <c r="E39" s="7"/>
-      <c r="F39" s="113"/>
+      <c r="F39" s="115"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
@@ -8016,7 +8080,7 @@
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
-      <c r="N39" s="113"/>
+      <c r="N39" s="115"/>
       <c r="O39" s="7"/>
       <c r="P39" s="35" t="s">
         <v>76</v>
@@ -8035,7 +8099,7 @@
         <v>Brasil</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="96" t="s">
+      <c r="D40" s="100" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="23">
@@ -8077,7 +8141,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="97"/>
+      <c r="D41" s="101"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -8157,6 +8221,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="J8:N8"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="D31:D32"/>
@@ -8173,13 +8244,6 @@
     <mergeCell ref="N38:N40"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="P40:P41"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="J8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -8190,8 +8254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61C1E5FA-F91B-4A41-A4C1-97D69E012813}">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="N41" sqref="N41"/>
+    <sheetView topLeftCell="A26" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3:R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8219,26 +8283,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="89"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="86"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="87" t="s">
+      <c r="J1" s="84" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="88"/>
-      <c r="N1" s="89"/>
-      <c r="P1" s="87" t="s">
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="86"/>
+      <c r="P1" s="84" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="88"/>
-      <c r="R1" s="89"/>
+      <c r="Q1" s="85"/>
+      <c r="R1" s="86"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -8441,23 +8505,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="101" t="s">
+      <c r="B8" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="102"/>
-      <c r="D8" s="102"/>
-      <c r="E8" s="102"/>
-      <c r="F8" s="103"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="94"/>
+      <c r="E8" s="94"/>
+      <c r="F8" s="95"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="101" t="s">
+      <c r="J8" s="93" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="102"/>
-      <c r="L8" s="102"/>
-      <c r="M8" s="102"/>
-      <c r="N8" s="103"/>
+      <c r="K8" s="94"/>
+      <c r="L8" s="94"/>
+      <c r="M8" s="94"/>
+      <c r="N8" s="95"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -8647,23 +8711,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="101" t="s">
+      <c r="B15" s="93" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="102"/>
-      <c r="D15" s="102"/>
-      <c r="E15" s="102"/>
-      <c r="F15" s="103"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="95"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="101" t="s">
+      <c r="J15" s="93" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="102"/>
-      <c r="L15" s="102"/>
-      <c r="M15" s="102"/>
-      <c r="N15" s="103"/>
+      <c r="K15" s="94"/>
+      <c r="L15" s="94"/>
+      <c r="M15" s="94"/>
+      <c r="N15" s="95"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -8830,23 +8894,23 @@
       <c r="N21" s="52"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="101" t="s">
+      <c r="B22" s="93" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="102"/>
-      <c r="D22" s="102"/>
-      <c r="E22" s="102"/>
-      <c r="F22" s="103"/>
+      <c r="C22" s="94"/>
+      <c r="D22" s="94"/>
+      <c r="E22" s="94"/>
+      <c r="F22" s="95"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="101" t="s">
+      <c r="J22" s="93" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="102"/>
-      <c r="L22" s="102"/>
-      <c r="M22" s="102"/>
-      <c r="N22" s="103"/>
+      <c r="K22" s="94"/>
+      <c r="L22" s="94"/>
+      <c r="M22" s="94"/>
+      <c r="N22" s="95"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B23" s="56" t="s">
@@ -9156,7 +9220,7 @@
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
-      <c r="N33" s="113"/>
+      <c r="N33" s="115"/>
       <c r="O33" s="7"/>
       <c r="P33" s="35" t="s">
         <v>74</v>
@@ -9538,6 +9602,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="J8:N8"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="D31:D32"/>
@@ -9554,13 +9625,6 @@
     <mergeCell ref="N38:N40"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="P40:P41"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="J8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -9642,7 +9706,7 @@
   <dimension ref="A1:AC43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AC24" sqref="AC24:AC27"/>
+      <selection activeCell="W41" sqref="W41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9678,26 +9742,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="89"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="86"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="87" t="s">
+      <c r="J1" s="84" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="88"/>
-      <c r="N1" s="89"/>
-      <c r="P1" s="87" t="s">
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="86"/>
+      <c r="P1" s="84" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="88"/>
-      <c r="R1" s="89"/>
+      <c r="Q1" s="85"/>
+      <c r="R1" s="86"/>
       <c r="W1" s="1" t="s">
         <v>92</v>
       </c>
@@ -10005,23 +10069,23 @@
       </c>
     </row>
     <row r="8" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B8" s="101" t="s">
+      <c r="B8" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="102"/>
-      <c r="D8" s="102"/>
-      <c r="E8" s="102"/>
-      <c r="F8" s="103"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="94"/>
+      <c r="E8" s="94"/>
+      <c r="F8" s="95"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="101" t="s">
+      <c r="J8" s="93" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="102"/>
-      <c r="L8" s="102"/>
-      <c r="M8" s="102"/>
-      <c r="N8" s="103"/>
+      <c r="K8" s="94"/>
+      <c r="L8" s="94"/>
+      <c r="M8" s="94"/>
+      <c r="N8" s="95"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -10309,23 +10373,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B15" s="101" t="s">
+      <c r="B15" s="93" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="102"/>
-      <c r="D15" s="102"/>
-      <c r="E15" s="102"/>
-      <c r="F15" s="103"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="95"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="101" t="s">
+      <c r="J15" s="93" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="102"/>
-      <c r="L15" s="102"/>
-      <c r="M15" s="102"/>
-      <c r="N15" s="103"/>
+      <c r="K15" s="94"/>
+      <c r="L15" s="94"/>
+      <c r="M15" s="94"/>
+      <c r="N15" s="95"/>
     </row>
     <row r="16" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -10590,23 +10654,23 @@
       <c r="N21" s="52"/>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B22" s="101" t="s">
+      <c r="B22" s="93" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="102"/>
-      <c r="D22" s="102"/>
-      <c r="E22" s="102"/>
-      <c r="F22" s="103"/>
+      <c r="C22" s="94"/>
+      <c r="D22" s="94"/>
+      <c r="E22" s="94"/>
+      <c r="F22" s="95"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="101" t="s">
+      <c r="J22" s="93" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="102"/>
-      <c r="L22" s="102"/>
-      <c r="M22" s="102"/>
-      <c r="N22" s="103"/>
+      <c r="K22" s="94"/>
+      <c r="L22" s="94"/>
+      <c r="M22" s="94"/>
+      <c r="N22" s="95"/>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B23" s="56" t="s">
@@ -11380,13 +11444,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="J8:N8"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="D31:D32"/>
@@ -11403,6 +11460,13 @@
     <mergeCell ref="N38:N40"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="P40:P41"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="J8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -11414,7 +11478,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView zoomScale="132" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:I20"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updates in ko stage edit page before making input changes
</commit_message>
<xml_diff>
--- a/excel docs/java testing-audit info.xlsx
+++ b/excel docs/java testing-audit info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joecollins/Desktop/documents/personal-projects/world-cup-heroku/excel docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3C4F44-B0A0-7141-B9F2-364CD5C25541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8DC836-0192-9649-BE87-56D3E22C0F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -1465,144 +1465,144 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1922,11 +1922,11 @@
       <c r="F1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="84" t="s">
+      <c r="J1" s="89" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="85"/>
-      <c r="L1" s="86"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="91"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B2" s="14" t="s">
@@ -2246,7 +2246,7 @@
         <v>Ecuador</v>
       </c>
       <c r="C27" s="7"/>
-      <c r="D27" s="87" t="s">
+      <c r="D27" s="86" t="s">
         <v>134</v>
       </c>
       <c r="E27" s="7"/>
@@ -2260,7 +2260,7 @@
       <c r="M27" s="7"/>
       <c r="N27" s="7"/>
       <c r="O27" s="7"/>
-      <c r="P27" s="87" t="s">
+      <c r="P27" s="86" t="s">
         <v>41</v>
       </c>
       <c r="Q27" s="7"/>
@@ -2284,7 +2284,7 @@
       <c r="C28" s="7"/>
       <c r="D28" s="88"/>
       <c r="E28" s="7"/>
-      <c r="F28" s="87" t="s">
+      <c r="F28" s="86" t="s">
         <v>25</v>
       </c>
       <c r="G28" s="7"/>
@@ -2294,7 +2294,7 @@
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
       <c r="M28" s="7"/>
-      <c r="N28" s="87" t="s">
+      <c r="N28" s="86" t="s">
         <v>34</v>
       </c>
       <c r="O28" s="7"/>
@@ -2315,7 +2315,7 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
-      <c r="F29" s="89"/>
+      <c r="F29" s="87"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
@@ -2323,7 +2323,7 @@
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
-      <c r="N29" s="89"/>
+      <c r="N29" s="87"/>
       <c r="O29" s="7"/>
       <c r="P29" s="7"/>
       <c r="Q29" s="7"/>
@@ -2340,7 +2340,7 @@
         <v>Argentina</v>
       </c>
       <c r="C30" s="7"/>
-      <c r="D30" s="87" t="s">
+      <c r="D30" s="86" t="s">
         <v>25</v>
       </c>
       <c r="E30" s="7"/>
@@ -2354,7 +2354,7 @@
       <c r="M30" s="7"/>
       <c r="N30" s="88"/>
       <c r="O30" s="7"/>
-      <c r="P30" s="87" t="s">
+      <c r="P30" s="86" t="s">
         <v>34</v>
       </c>
       <c r="Q30" s="7"/>
@@ -2380,13 +2380,13 @@
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
-      <c r="H31" s="90" t="s">
+      <c r="H31" s="92" t="s">
         <v>25</v>
       </c>
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
-      <c r="L31" s="90" t="s">
+      <c r="L31" s="92" t="s">
         <v>14</v>
       </c>
       <c r="M31" s="7"/>
@@ -2411,13 +2411,13 @@
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
-      <c r="H32" s="91"/>
+      <c r="H32" s="93"/>
       <c r="I32" s="7"/>
       <c r="J32" s="23" t="s">
         <v>25</v>
       </c>
       <c r="K32" s="7"/>
-      <c r="L32" s="91"/>
+      <c r="L32" s="93"/>
       <c r="M32" s="7"/>
       <c r="N32" s="7"/>
       <c r="O32" s="7"/>
@@ -2436,21 +2436,21 @@
         <v>Italy</v>
       </c>
       <c r="C33" s="7"/>
-      <c r="D33" s="87" t="s">
+      <c r="D33" s="86" t="s">
         <v>139</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
-      <c r="H33" s="92"/>
+      <c r="H33" s="94"/>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
-      <c r="L33" s="92"/>
+      <c r="L33" s="94"/>
       <c r="M33" s="7"/>
       <c r="N33" s="7"/>
       <c r="O33" s="7"/>
-      <c r="P33" s="87" t="s">
+      <c r="P33" s="86" t="s">
         <v>14</v>
       </c>
       <c r="Q33" s="7"/>
@@ -2474,7 +2474,7 @@
       <c r="C34" s="7"/>
       <c r="D34" s="88"/>
       <c r="E34" s="7"/>
-      <c r="F34" s="87" t="s">
+      <c r="F34" s="86" t="s">
         <v>12</v>
       </c>
       <c r="G34" s="7"/>
@@ -2484,7 +2484,7 @@
       <c r="K34" s="7"/>
       <c r="L34" s="7"/>
       <c r="M34" s="7"/>
-      <c r="N34" s="87" t="s">
+      <c r="N34" s="86" t="s">
         <v>14</v>
       </c>
       <c r="O34" s="7"/>
@@ -2505,7 +2505,7 @@
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
-      <c r="F35" s="89"/>
+      <c r="F35" s="87"/>
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
@@ -2513,7 +2513,7 @@
       <c r="K35" s="7"/>
       <c r="L35" s="7"/>
       <c r="M35" s="7"/>
-      <c r="N35" s="89"/>
+      <c r="N35" s="87"/>
       <c r="O35" s="7"/>
       <c r="P35" s="7"/>
       <c r="Q35" s="7"/>
@@ -2530,7 +2530,7 @@
         <v>Brasil</v>
       </c>
       <c r="C36" s="7"/>
-      <c r="D36" s="87" t="s">
+      <c r="D36" s="86" t="s">
         <v>12</v>
       </c>
       <c r="E36" s="7"/>
@@ -2544,7 +2544,7 @@
       <c r="M36" s="7"/>
       <c r="N36" s="88"/>
       <c r="O36" s="7"/>
-      <c r="P36" s="87" t="s">
+      <c r="P36" s="86" t="s">
         <v>137</v>
       </c>
       <c r="Q36" s="7"/>
@@ -2613,12 +2613,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="N28:N30"/>
-    <mergeCell ref="N34:N36"/>
-    <mergeCell ref="P27:P28"/>
-    <mergeCell ref="P30:P31"/>
-    <mergeCell ref="P33:P34"/>
-    <mergeCell ref="P36:P37"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="D27:D28"/>
     <mergeCell ref="D30:D31"/>
@@ -2628,6 +2622,12 @@
     <mergeCell ref="F34:F36"/>
     <mergeCell ref="H31:H33"/>
     <mergeCell ref="L31:L33"/>
+    <mergeCell ref="N28:N30"/>
+    <mergeCell ref="N34:N36"/>
+    <mergeCell ref="P27:P28"/>
+    <mergeCell ref="P30:P31"/>
+    <mergeCell ref="P33:P34"/>
+    <mergeCell ref="P36:P37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -2638,7 +2638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A13F6EC-BC2A-504C-A071-8460572D194C}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="189" workbookViewId="0">
+    <sheetView zoomScale="189" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -2648,30 +2648,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="63" x14ac:dyDescent="0.2">
-      <c r="A1" s="130" t="s">
+      <c r="A1" s="85" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="42" x14ac:dyDescent="0.2">
-      <c r="A2" s="130" t="s">
+      <c r="A2" s="85" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="63" x14ac:dyDescent="0.2">
-      <c r="A3" s="130" t="s">
+      <c r="A3" s="85" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="63" x14ac:dyDescent="0.2">
-      <c r="A4" s="130" t="s">
+      <c r="A4" s="85" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="129"/>
+      <c r="A5" s="84"/>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="129"/>
+      <c r="A6" s="84"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2682,8 +2682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86316F4E-9A6C-492E-9EDB-018A26A821E8}">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2714,26 +2714,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="86"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="91"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="84" t="s">
+      <c r="J1" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="85"/>
-      <c r="L1" s="85"/>
-      <c r="M1" s="85"/>
-      <c r="N1" s="86"/>
-      <c r="P1" s="84" t="s">
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="91"/>
+      <c r="P1" s="89" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="85"/>
-      <c r="R1" s="86"/>
+      <c r="Q1" s="90"/>
+      <c r="R1" s="91"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -2936,23 +2936,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="93" t="s">
+      <c r="B8" s="103" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="95"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="104"/>
+      <c r="E8" s="104"/>
+      <c r="F8" s="105"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="93" t="s">
+      <c r="J8" s="103" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="94"/>
-      <c r="L8" s="94"/>
-      <c r="M8" s="94"/>
-      <c r="N8" s="95"/>
+      <c r="K8" s="104"/>
+      <c r="L8" s="104"/>
+      <c r="M8" s="104"/>
+      <c r="N8" s="105"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -3142,23 +3142,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="93" t="s">
+      <c r="B15" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="94"/>
-      <c r="D15" s="94"/>
-      <c r="E15" s="94"/>
-      <c r="F15" s="95"/>
+      <c r="C15" s="104"/>
+      <c r="D15" s="104"/>
+      <c r="E15" s="104"/>
+      <c r="F15" s="105"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="93" t="s">
+      <c r="J15" s="103" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="94"/>
-      <c r="L15" s="94"/>
-      <c r="M15" s="94"/>
-      <c r="N15" s="95"/>
+      <c r="K15" s="104"/>
+      <c r="L15" s="104"/>
+      <c r="M15" s="104"/>
+      <c r="N15" s="105"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -3279,10 +3279,10 @@
         <f t="shared" ref="N19:N20" si="5">IF(J19=L19,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Q19" s="96" t="s">
+      <c r="Q19" s="106" t="s">
         <v>82</v>
       </c>
-      <c r="R19" s="96"/>
+      <c r="R19" s="106"/>
     </row>
     <row r="20" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="27" t="s">
@@ -3337,23 +3337,23 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="93" t="s">
+      <c r="B22" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="94"/>
-      <c r="D22" s="94"/>
-      <c r="E22" s="94"/>
-      <c r="F22" s="95"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="105"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="93" t="s">
+      <c r="J22" s="103" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="94"/>
-      <c r="L22" s="94"/>
-      <c r="M22" s="94"/>
-      <c r="N22" s="95"/>
+      <c r="K22" s="104"/>
+      <c r="L22" s="104"/>
+      <c r="M22" s="104"/>
+      <c r="N22" s="105"/>
       <c r="Q22" s="49"/>
       <c r="R22" s="32" t="s">
         <v>85</v>
@@ -3584,7 +3584,7 @@
         <v>Ecuador</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="100" t="s">
+      <c r="D31" s="98" t="s">
         <v>134</v>
       </c>
       <c r="E31" s="7"/>
@@ -3602,7 +3602,7 @@
         <v>79</v>
       </c>
       <c r="O31" s="7"/>
-      <c r="P31" s="100" t="s">
+      <c r="P31" s="98" t="s">
         <v>41</v>
       </c>
       <c r="Q31" s="7"/>
@@ -3624,12 +3624,12 @@
         <v>Iran</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="101"/>
+      <c r="D32" s="99"/>
       <c r="E32" s="23">
         <f>IF(D31=Master!D27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F32" s="100" t="s">
+      <c r="F32" s="98" t="s">
         <v>25</v>
       </c>
       <c r="G32" s="7"/>
@@ -3639,14 +3639,14 @@
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
-      <c r="N32" s="100" t="s">
+      <c r="N32" s="98" t="s">
         <v>34</v>
       </c>
       <c r="O32" s="23">
         <f>IF(P31=Master!P27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P32" s="101"/>
+      <c r="P32" s="99"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="39" t="str">
         <f>D4</f>
@@ -3665,7 +3665,7 @@
         <v>70</v>
       </c>
       <c r="E33" s="7"/>
-      <c r="F33" s="102"/>
+      <c r="F33" s="100"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
@@ -3673,7 +3673,7 @@
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
-      <c r="N33" s="102"/>
+      <c r="N33" s="100"/>
       <c r="O33" s="7"/>
       <c r="P33" s="35"/>
       <c r="Q33" s="7"/>
@@ -3690,14 +3690,14 @@
         <v>Argentina</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="100" t="s">
+      <c r="D34" s="98" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="23">
         <f>IF(D34=Master!D30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F34" s="101"/>
+      <c r="F34" s="99"/>
       <c r="G34" s="23">
         <f>IF(F32=Master!F28,4,0)</f>
         <v>4</v>
@@ -3715,12 +3715,12 @@
         <f>IF(N32=Master!N28,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N34" s="101"/>
+      <c r="N34" s="99"/>
       <c r="O34" s="23">
         <f>IF(P34=Master!P30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P34" s="100" t="s">
+      <c r="P34" s="98" t="s">
         <v>34</v>
       </c>
       <c r="Q34" s="7"/>
@@ -3742,11 +3742,11 @@
         <v>France</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="101"/>
+      <c r="D35" s="99"/>
       <c r="E35" s="7"/>
       <c r="F35" s="35"/>
       <c r="G35" s="7"/>
-      <c r="H35" s="100" t="s">
+      <c r="H35" s="98" t="s">
         <v>25</v>
       </c>
       <c r="I35" s="7"/>
@@ -3754,13 +3754,13 @@
         <v>81</v>
       </c>
       <c r="K35" s="7"/>
-      <c r="L35" s="100" t="s">
+      <c r="L35" s="98" t="s">
         <v>14</v>
       </c>
       <c r="M35" s="7"/>
       <c r="N35" s="35"/>
       <c r="O35" s="7"/>
-      <c r="P35" s="101"/>
+      <c r="P35" s="99"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="39" t="str">
         <f>D11</f>
@@ -3781,7 +3781,7 @@
       <c r="E36" s="7"/>
       <c r="F36" s="35"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="102"/>
+      <c r="H36" s="100"/>
       <c r="I36" s="24">
         <f>IF(H35=Master!H31,6,0)</f>
         <v>6</v>
@@ -3793,7 +3793,7 @@
         <f>IF(L35=Master!L31,6,0)</f>
         <v>6</v>
       </c>
-      <c r="L36" s="102"/>
+      <c r="L36" s="100"/>
       <c r="M36" s="7"/>
       <c r="N36" s="35"/>
       <c r="O36" s="7"/>
@@ -3814,7 +3814,7 @@
         <v>Italy</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="103" t="s">
+      <c r="D37" s="101" t="s">
         <v>139</v>
       </c>
       <c r="E37" s="7"/>
@@ -3822,17 +3822,17 @@
         <v>78</v>
       </c>
       <c r="G37" s="7"/>
-      <c r="H37" s="101"/>
+      <c r="H37" s="99"/>
       <c r="I37" s="7"/>
       <c r="J37" s="35"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="101"/>
+      <c r="L37" s="99"/>
       <c r="M37" s="7"/>
       <c r="N37" s="35" t="s">
         <v>80</v>
       </c>
       <c r="O37" s="7"/>
-      <c r="P37" s="100" t="s">
+      <c r="P37" s="98" t="s">
         <v>14</v>
       </c>
       <c r="Q37" s="7"/>
@@ -3854,12 +3854,12 @@
         <v>Canada</v>
       </c>
       <c r="C38" s="7"/>
-      <c r="D38" s="104"/>
+      <c r="D38" s="102"/>
       <c r="E38" s="23">
         <f>IF(D37=Master!D33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F38" s="97" t="s">
+      <c r="F38" s="95" t="s">
         <v>12</v>
       </c>
       <c r="G38" s="23">
@@ -3878,14 +3878,14 @@
         <f>IF(N38=Master!N34,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N38" s="100" t="s">
+      <c r="N38" s="98" t="s">
         <v>14</v>
       </c>
       <c r="O38" s="23">
         <f>IF(P37=Master!P33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P38" s="101"/>
+      <c r="P38" s="99"/>
       <c r="Q38" s="7"/>
       <c r="R38" s="39" t="str">
         <f>D18</f>
@@ -3904,7 +3904,7 @@
         <v>72</v>
       </c>
       <c r="E39" s="7"/>
-      <c r="F39" s="98"/>
+      <c r="F39" s="96"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
@@ -3912,7 +3912,7 @@
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
-      <c r="N39" s="102"/>
+      <c r="N39" s="100"/>
       <c r="O39" s="7"/>
       <c r="P39" s="35" t="s">
         <v>76</v>
@@ -3931,14 +3931,14 @@
         <v>Brasil</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="100" t="s">
+      <c r="D40" s="98" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="23">
         <f>IF(D40=Master!D36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F40" s="99"/>
+      <c r="F40" s="97"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
@@ -3946,12 +3946,12 @@
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
-      <c r="N40" s="101"/>
+      <c r="N40" s="99"/>
       <c r="O40" s="23">
         <f>IF(P40=Master!P36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P40" s="100" t="s">
+      <c r="P40" s="98" t="s">
         <v>137</v>
       </c>
       <c r="Q40" s="7"/>
@@ -3973,7 +3973,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="101"/>
+      <c r="D41" s="99"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -3985,7 +3985,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="101"/>
+      <c r="P41" s="99"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="39" t="str">
         <f>D25</f>
@@ -4053,6 +4053,16 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J22:N22"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="Q19:R19"/>
     <mergeCell ref="F38:F40"/>
     <mergeCell ref="P37:P38"/>
     <mergeCell ref="P40:P41"/>
@@ -4067,16 +4077,6 @@
     <mergeCell ref="D37:D38"/>
     <mergeCell ref="H35:H37"/>
     <mergeCell ref="L35:L37"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J22:N22"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="J8:N8"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="Q19:R19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -4119,26 +4119,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="86"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="91"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="84" t="s">
+      <c r="J1" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="85"/>
-      <c r="L1" s="85"/>
-      <c r="M1" s="85"/>
-      <c r="N1" s="86"/>
-      <c r="P1" s="84" t="s">
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="91"/>
+      <c r="P1" s="89" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="85"/>
-      <c r="R1" s="86"/>
+      <c r="Q1" s="90"/>
+      <c r="R1" s="91"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -4341,23 +4341,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="93" t="s">
+      <c r="B8" s="103" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="95"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="104"/>
+      <c r="E8" s="104"/>
+      <c r="F8" s="105"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="93" t="s">
+      <c r="J8" s="103" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="94"/>
-      <c r="L8" s="94"/>
-      <c r="M8" s="94"/>
-      <c r="N8" s="95"/>
+      <c r="K8" s="104"/>
+      <c r="L8" s="104"/>
+      <c r="M8" s="104"/>
+      <c r="N8" s="105"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -4547,23 +4547,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="93" t="s">
+      <c r="B15" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="94"/>
-      <c r="D15" s="94"/>
-      <c r="E15" s="94"/>
-      <c r="F15" s="95"/>
+      <c r="C15" s="104"/>
+      <c r="D15" s="104"/>
+      <c r="E15" s="104"/>
+      <c r="F15" s="105"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="93" t="s">
+      <c r="J15" s="103" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="94"/>
-      <c r="L15" s="94"/>
-      <c r="M15" s="94"/>
-      <c r="N15" s="95"/>
+      <c r="K15" s="104"/>
+      <c r="L15" s="104"/>
+      <c r="M15" s="104"/>
+      <c r="N15" s="105"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -4684,10 +4684,10 @@
         <f t="shared" ref="N19:N20" si="5">IF(J19=L19,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Q19" s="96" t="s">
+      <c r="Q19" s="106" t="s">
         <v>82</v>
       </c>
-      <c r="R19" s="96"/>
+      <c r="R19" s="106"/>
     </row>
     <row r="20" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="27" t="s">
@@ -4742,23 +4742,23 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="93" t="s">
+      <c r="B22" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="94"/>
-      <c r="D22" s="94"/>
-      <c r="E22" s="94"/>
-      <c r="F22" s="95"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="105"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="93" t="s">
+      <c r="J22" s="103" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="94"/>
-      <c r="L22" s="94"/>
-      <c r="M22" s="94"/>
-      <c r="N22" s="95"/>
+      <c r="K22" s="104"/>
+      <c r="L22" s="104"/>
+      <c r="M22" s="104"/>
+      <c r="N22" s="105"/>
       <c r="Q22" s="49"/>
       <c r="R22" s="32" t="s">
         <v>85</v>
@@ -4989,7 +4989,7 @@
         <v>Ecuador</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="100" t="s">
+      <c r="D31" s="98" t="s">
         <v>134</v>
       </c>
       <c r="E31" s="7"/>
@@ -5007,7 +5007,7 @@
         <v>79</v>
       </c>
       <c r="O31" s="7"/>
-      <c r="P31" s="100" t="s">
+      <c r="P31" s="98" t="s">
         <v>41</v>
       </c>
       <c r="Q31" s="7"/>
@@ -5029,12 +5029,12 @@
         <v>Iran</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="101"/>
+      <c r="D32" s="99"/>
       <c r="E32" s="23">
         <f>IF(D31=Master!D27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F32" s="100" t="s">
+      <c r="F32" s="98" t="s">
         <v>25</v>
       </c>
       <c r="G32" s="7"/>
@@ -5044,14 +5044,14 @@
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
-      <c r="N32" s="100" t="s">
+      <c r="N32" s="98" t="s">
         <v>34</v>
       </c>
       <c r="O32" s="23">
         <f>IF(P31=Master!P27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P32" s="101"/>
+      <c r="P32" s="99"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="81" t="str">
         <f>D4</f>
@@ -5070,7 +5070,7 @@
         <v>70</v>
       </c>
       <c r="E33" s="7"/>
-      <c r="F33" s="102"/>
+      <c r="F33" s="100"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
@@ -5078,7 +5078,7 @@
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
-      <c r="N33" s="102"/>
+      <c r="N33" s="100"/>
       <c r="O33" s="7"/>
       <c r="P33" s="35"/>
       <c r="Q33" s="7"/>
@@ -5095,14 +5095,14 @@
         <v>Argentina</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="100" t="s">
+      <c r="D34" s="98" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="23">
         <f>IF(D34=Master!D30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F34" s="101"/>
+      <c r="F34" s="99"/>
       <c r="G34" s="23">
         <f>IF(F32=Master!F28,4,0)</f>
         <v>4</v>
@@ -5120,12 +5120,12 @@
         <f>IF(N32=Master!N28,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N34" s="101"/>
+      <c r="N34" s="99"/>
       <c r="O34" s="23">
         <f>IF(P34=Master!P30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P34" s="100" t="s">
+      <c r="P34" s="98" t="s">
         <v>34</v>
       </c>
       <c r="Q34" s="7"/>
@@ -5147,11 +5147,11 @@
         <v>France</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="101"/>
+      <c r="D35" s="99"/>
       <c r="E35" s="7"/>
       <c r="F35" s="35"/>
       <c r="G35" s="7"/>
-      <c r="H35" s="100" t="s">
+      <c r="H35" s="98" t="s">
         <v>25</v>
       </c>
       <c r="I35" s="7"/>
@@ -5159,13 +5159,13 @@
         <v>81</v>
       </c>
       <c r="K35" s="7"/>
-      <c r="L35" s="100" t="s">
+      <c r="L35" s="98" t="s">
         <v>14</v>
       </c>
       <c r="M35" s="7"/>
       <c r="N35" s="35"/>
       <c r="O35" s="7"/>
-      <c r="P35" s="101"/>
+      <c r="P35" s="99"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="81" t="str">
         <f>D11</f>
@@ -5186,7 +5186,7 @@
       <c r="E36" s="7"/>
       <c r="F36" s="35"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="102"/>
+      <c r="H36" s="100"/>
       <c r="I36" s="24">
         <f>IF(H35=Master!H31,6,0)</f>
         <v>6</v>
@@ -5198,7 +5198,7 @@
         <f>IF(L35=Master!L31,6,0)</f>
         <v>6</v>
       </c>
-      <c r="L36" s="102"/>
+      <c r="L36" s="100"/>
       <c r="M36" s="7"/>
       <c r="N36" s="35"/>
       <c r="O36" s="7"/>
@@ -5219,7 +5219,7 @@
         <v>Italy</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="103" t="s">
+      <c r="D37" s="101" t="s">
         <v>139</v>
       </c>
       <c r="E37" s="7"/>
@@ -5227,17 +5227,17 @@
         <v>78</v>
       </c>
       <c r="G37" s="7"/>
-      <c r="H37" s="101"/>
+      <c r="H37" s="99"/>
       <c r="I37" s="7"/>
       <c r="J37" s="35"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="101"/>
+      <c r="L37" s="99"/>
       <c r="M37" s="7"/>
       <c r="N37" s="35" t="s">
         <v>80</v>
       </c>
       <c r="O37" s="7"/>
-      <c r="P37" s="100" t="s">
+      <c r="P37" s="98" t="s">
         <v>14</v>
       </c>
       <c r="Q37" s="7"/>
@@ -5259,12 +5259,12 @@
         <v>Canada</v>
       </c>
       <c r="C38" s="7"/>
-      <c r="D38" s="104"/>
+      <c r="D38" s="102"/>
       <c r="E38" s="23">
         <f>IF(D37=Master!D33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F38" s="97" t="s">
+      <c r="F38" s="95" t="s">
         <v>12</v>
       </c>
       <c r="G38" s="23">
@@ -5283,14 +5283,14 @@
         <f>IF(N38=Master!N34,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N38" s="100" t="s">
+      <c r="N38" s="98" t="s">
         <v>14</v>
       </c>
       <c r="O38" s="23">
         <f>IF(P37=Master!P33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P38" s="101"/>
+      <c r="P38" s="99"/>
       <c r="Q38" s="7"/>
       <c r="R38" s="81" t="str">
         <f>D18</f>
@@ -5309,7 +5309,7 @@
         <v>72</v>
       </c>
       <c r="E39" s="7"/>
-      <c r="F39" s="98"/>
+      <c r="F39" s="96"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
@@ -5317,7 +5317,7 @@
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
-      <c r="N39" s="102"/>
+      <c r="N39" s="100"/>
       <c r="O39" s="7"/>
       <c r="P39" s="35" t="s">
         <v>76</v>
@@ -5336,14 +5336,14 @@
         <v>Brasil</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="100" t="s">
+      <c r="D40" s="98" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="23">
         <f>IF(D40=Master!D36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F40" s="99"/>
+      <c r="F40" s="97"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
@@ -5351,12 +5351,12 @@
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
-      <c r="N40" s="101"/>
+      <c r="N40" s="99"/>
       <c r="O40" s="23">
         <f>IF(P40=Master!P36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P40" s="100" t="s">
+      <c r="P40" s="98" t="s">
         <v>137</v>
       </c>
       <c r="Q40" s="7"/>
@@ -5378,7 +5378,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="101"/>
+      <c r="D41" s="99"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -5390,7 +5390,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="101"/>
+      <c r="P41" s="99"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="81" t="str">
         <f>D25</f>
@@ -5458,6 +5458,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="P34:P35"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="L35:L37"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="P37:P38"/>
+    <mergeCell ref="F38:F40"/>
+    <mergeCell ref="N38:N40"/>
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="J8:N8"/>
@@ -5474,14 +5482,6 @@
     <mergeCell ref="P31:P32"/>
     <mergeCell ref="F32:F34"/>
     <mergeCell ref="N32:N34"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="P34:P35"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="L35:L37"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="P37:P38"/>
-    <mergeCell ref="F38:F40"/>
-    <mergeCell ref="N38:N40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -5521,26 +5521,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="86"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="91"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="84" t="s">
+      <c r="J1" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="85"/>
-      <c r="L1" s="85"/>
-      <c r="M1" s="85"/>
-      <c r="N1" s="86"/>
-      <c r="P1" s="84" t="s">
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="91"/>
+      <c r="P1" s="89" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="85"/>
-      <c r="R1" s="86"/>
+      <c r="Q1" s="90"/>
+      <c r="R1" s="91"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -5743,23 +5743,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="93" t="s">
+      <c r="B8" s="103" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="95"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="104"/>
+      <c r="E8" s="104"/>
+      <c r="F8" s="105"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="93" t="s">
+      <c r="J8" s="103" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="94"/>
-      <c r="L8" s="94"/>
-      <c r="M8" s="94"/>
-      <c r="N8" s="95"/>
+      <c r="K8" s="104"/>
+      <c r="L8" s="104"/>
+      <c r="M8" s="104"/>
+      <c r="N8" s="105"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -5949,23 +5949,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="93" t="s">
+      <c r="B15" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="94"/>
-      <c r="D15" s="94"/>
-      <c r="E15" s="94"/>
-      <c r="F15" s="95"/>
+      <c r="C15" s="104"/>
+      <c r="D15" s="104"/>
+      <c r="E15" s="104"/>
+      <c r="F15" s="105"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="93" t="s">
+      <c r="J15" s="103" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="94"/>
-      <c r="L15" s="94"/>
-      <c r="M15" s="94"/>
-      <c r="N15" s="95"/>
+      <c r="K15" s="104"/>
+      <c r="L15" s="104"/>
+      <c r="M15" s="104"/>
+      <c r="N15" s="105"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -6130,23 +6130,23 @@
       <c r="N21" s="52"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="93" t="s">
+      <c r="B22" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="94"/>
-      <c r="D22" s="94"/>
-      <c r="E22" s="94"/>
-      <c r="F22" s="95"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="105"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="93" t="s">
+      <c r="J22" s="103" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="94"/>
-      <c r="L22" s="94"/>
-      <c r="M22" s="94"/>
-      <c r="N22" s="95"/>
+      <c r="K22" s="104"/>
+      <c r="L22" s="104"/>
+      <c r="M22" s="104"/>
+      <c r="N22" s="105"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B23" s="56" t="s">
@@ -6367,7 +6367,7 @@
         <v>Ecuador</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="105" t="s">
+      <c r="D31" s="107" t="s">
         <v>45</v>
       </c>
       <c r="E31" s="7"/>
@@ -6385,7 +6385,7 @@
         <v>79</v>
       </c>
       <c r="O31" s="7"/>
-      <c r="P31" s="100" t="s">
+      <c r="P31" s="98" t="s">
         <v>41</v>
       </c>
       <c r="Q31" s="7"/>
@@ -6407,12 +6407,12 @@
         <v>Iran</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="106"/>
+      <c r="D32" s="108"/>
       <c r="E32" s="23">
         <f>IF(D31=Master!D27,2,0)</f>
         <v>0</v>
       </c>
-      <c r="F32" s="105" t="s">
+      <c r="F32" s="107" t="s">
         <v>45</v>
       </c>
       <c r="G32" s="7"/>
@@ -6422,14 +6422,14 @@
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
-      <c r="N32" s="105" t="s">
+      <c r="N32" s="107" t="s">
         <v>41</v>
       </c>
       <c r="O32" s="23">
         <f>IF(P31=Master!P27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P32" s="101"/>
+      <c r="P32" s="99"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="39" t="str">
         <f>D4</f>
@@ -6448,7 +6448,7 @@
         <v>70</v>
       </c>
       <c r="E33" s="7"/>
-      <c r="F33" s="107"/>
+      <c r="F33" s="109"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
@@ -6456,7 +6456,7 @@
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
-      <c r="N33" s="107"/>
+      <c r="N33" s="109"/>
       <c r="O33" s="7"/>
       <c r="P33" s="35" t="s">
         <v>74</v>
@@ -6475,14 +6475,14 @@
         <v>Argentina</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="100" t="s">
+      <c r="D34" s="98" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="23">
         <f>IF(D34=Master!D30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F34" s="106"/>
+      <c r="F34" s="108"/>
       <c r="G34" s="23">
         <f>IF(F32=Master!F28,4,0)</f>
         <v>0</v>
@@ -6500,12 +6500,12 @@
         <f>IF(N32=Master!N28,4,0)</f>
         <v>0</v>
       </c>
-      <c r="N34" s="106"/>
+      <c r="N34" s="108"/>
       <c r="O34" s="23">
         <f>IF(P34=Master!P30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P34" s="100" t="s">
+      <c r="P34" s="98" t="s">
         <v>34</v>
       </c>
       <c r="Q34" s="7"/>
@@ -6527,11 +6527,11 @@
         <v>France</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="101"/>
+      <c r="D35" s="99"/>
       <c r="E35" s="7"/>
       <c r="F35" s="35"/>
       <c r="G35" s="7"/>
-      <c r="H35" s="105" t="s">
+      <c r="H35" s="107" t="s">
         <v>139</v>
       </c>
       <c r="I35" s="7"/>
@@ -6539,13 +6539,13 @@
         <v>81</v>
       </c>
       <c r="K35" s="7"/>
-      <c r="L35" s="105" t="s">
+      <c r="L35" s="107" t="s">
         <v>27</v>
       </c>
       <c r="M35" s="7"/>
       <c r="N35" s="35"/>
       <c r="O35" s="7"/>
-      <c r="P35" s="101"/>
+      <c r="P35" s="99"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="39" t="str">
         <f>D11</f>
@@ -6566,7 +6566,7 @@
       <c r="E36" s="7"/>
       <c r="F36" s="35"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="107"/>
+      <c r="H36" s="109"/>
       <c r="I36" s="24">
         <f>IF(H35=Master!H31,6,0)</f>
         <v>0</v>
@@ -6578,7 +6578,7 @@
         <f>IF(L35=Master!L31,6,0)</f>
         <v>0</v>
       </c>
-      <c r="L36" s="107"/>
+      <c r="L36" s="109"/>
       <c r="M36" s="7"/>
       <c r="N36" s="35"/>
       <c r="O36" s="7"/>
@@ -6599,7 +6599,7 @@
         <v>Italy</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="103" t="s">
+      <c r="D37" s="101" t="s">
         <v>139</v>
       </c>
       <c r="E37" s="7"/>
@@ -6607,17 +6607,17 @@
         <v>78</v>
       </c>
       <c r="G37" s="7"/>
-      <c r="H37" s="106"/>
+      <c r="H37" s="108"/>
       <c r="I37" s="7"/>
       <c r="J37" s="35"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="106"/>
+      <c r="L37" s="108"/>
       <c r="M37" s="7"/>
       <c r="N37" s="35" t="s">
         <v>80</v>
       </c>
       <c r="O37" s="7"/>
-      <c r="P37" s="105" t="s">
+      <c r="P37" s="107" t="s">
         <v>27</v>
       </c>
       <c r="Q37" s="7"/>
@@ -6639,12 +6639,12 @@
         <v>Canada</v>
       </c>
       <c r="C38" s="7"/>
-      <c r="D38" s="104"/>
+      <c r="D38" s="102"/>
       <c r="E38" s="23">
         <f>IF(D37=Master!D33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F38" s="105" t="s">
+      <c r="F38" s="107" t="s">
         <v>139</v>
       </c>
       <c r="G38" s="23">
@@ -6663,14 +6663,14 @@
         <f>IF(N38=Master!N34,4,0)</f>
         <v>0</v>
       </c>
-      <c r="N38" s="105" t="s">
+      <c r="N38" s="107" t="s">
         <v>27</v>
       </c>
       <c r="O38" s="23">
         <f>IF(P37=Master!P33,2,0)</f>
         <v>0</v>
       </c>
-      <c r="P38" s="106"/>
+      <c r="P38" s="108"/>
       <c r="Q38" s="7"/>
       <c r="R38" s="39" t="str">
         <f>D18</f>
@@ -6689,7 +6689,7 @@
         <v>72</v>
       </c>
       <c r="E39" s="7"/>
-      <c r="F39" s="107"/>
+      <c r="F39" s="109"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
@@ -6697,7 +6697,7 @@
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
-      <c r="N39" s="107"/>
+      <c r="N39" s="109"/>
       <c r="O39" s="7"/>
       <c r="P39" s="35" t="s">
         <v>76</v>
@@ -6716,14 +6716,14 @@
         <v>Brasil</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="100" t="s">
+      <c r="D40" s="98" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="23">
         <f>IF(D40=Master!D36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F40" s="106"/>
+      <c r="F40" s="108"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
@@ -6731,12 +6731,12 @@
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
-      <c r="N40" s="106"/>
+      <c r="N40" s="108"/>
       <c r="O40" s="23">
         <f>IF(P40=Master!P36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P40" s="100" t="s">
+      <c r="P40" s="98" t="s">
         <v>137</v>
       </c>
       <c r="Q40" s="7"/>
@@ -6758,7 +6758,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="101"/>
+      <c r="D41" s="99"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -6770,7 +6770,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="101"/>
+      <c r="P41" s="99"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="39" t="str">
         <f>D25</f>
@@ -6838,13 +6838,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="J8:N8"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="D31:D32"/>
@@ -6861,6 +6854,13 @@
     <mergeCell ref="N38:N40"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="P40:P41"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="J8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -6900,26 +6900,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="86"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="91"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="84" t="s">
+      <c r="J1" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="85"/>
-      <c r="L1" s="85"/>
-      <c r="M1" s="85"/>
-      <c r="N1" s="86"/>
-      <c r="P1" s="84" t="s">
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="91"/>
+      <c r="P1" s="89" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="85"/>
-      <c r="R1" s="86"/>
+      <c r="Q1" s="90"/>
+      <c r="R1" s="91"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -7122,23 +7122,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="93" t="s">
+      <c r="B8" s="103" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="95"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="104"/>
+      <c r="E8" s="104"/>
+      <c r="F8" s="105"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="93" t="s">
+      <c r="J8" s="103" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="94"/>
-      <c r="L8" s="94"/>
-      <c r="M8" s="94"/>
-      <c r="N8" s="95"/>
+      <c r="K8" s="104"/>
+      <c r="L8" s="104"/>
+      <c r="M8" s="104"/>
+      <c r="N8" s="105"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -7328,23 +7328,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="93" t="s">
+      <c r="B15" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="94"/>
-      <c r="D15" s="94"/>
-      <c r="E15" s="94"/>
-      <c r="F15" s="95"/>
+      <c r="C15" s="104"/>
+      <c r="D15" s="104"/>
+      <c r="E15" s="104"/>
+      <c r="F15" s="105"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="93" t="s">
+      <c r="J15" s="103" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="94"/>
-      <c r="L15" s="94"/>
-      <c r="M15" s="94"/>
-      <c r="N15" s="95"/>
+      <c r="K15" s="104"/>
+      <c r="L15" s="104"/>
+      <c r="M15" s="104"/>
+      <c r="N15" s="105"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -7511,23 +7511,23 @@
       <c r="N21" s="52"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="93" t="s">
+      <c r="B22" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="94"/>
-      <c r="D22" s="94"/>
-      <c r="E22" s="94"/>
-      <c r="F22" s="95"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="105"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="93" t="s">
+      <c r="J22" s="103" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="94"/>
-      <c r="L22" s="94"/>
-      <c r="M22" s="94"/>
-      <c r="N22" s="95"/>
+      <c r="K22" s="104"/>
+      <c r="L22" s="104"/>
+      <c r="M22" s="104"/>
+      <c r="N22" s="105"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B23" s="56" t="s">
@@ -7750,7 +7750,7 @@
         <v>Ecuador</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="108" t="s">
+      <c r="D31" s="110" t="s">
         <v>134</v>
       </c>
       <c r="E31" s="7"/>
@@ -7768,7 +7768,7 @@
         <v>79</v>
       </c>
       <c r="O31" s="7"/>
-      <c r="P31" s="108" t="s">
+      <c r="P31" s="110" t="s">
         <v>41</v>
       </c>
       <c r="Q31" s="7"/>
@@ -7790,12 +7790,12 @@
         <v>Iran</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="109"/>
+      <c r="D32" s="111"/>
       <c r="E32" s="23">
         <f>IF(D31=Master!D27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F32" s="110" t="s">
+      <c r="F32" s="112" t="s">
         <v>134</v>
       </c>
       <c r="G32" s="7"/>
@@ -7805,14 +7805,14 @@
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
-      <c r="N32" s="110" t="s">
+      <c r="N32" s="112" t="s">
         <v>13</v>
       </c>
       <c r="O32" s="23">
         <f>IF(P31=Master!P27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P32" s="109"/>
+      <c r="P32" s="111"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="39" t="str">
         <f>D4</f>
@@ -7831,7 +7831,7 @@
         <v>70</v>
       </c>
       <c r="E33" s="7"/>
-      <c r="F33" s="111"/>
+      <c r="F33" s="113"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
@@ -7839,7 +7839,7 @@
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
-      <c r="N33" s="111"/>
+      <c r="N33" s="113"/>
       <c r="O33" s="7"/>
       <c r="P33" s="35" t="s">
         <v>74</v>
@@ -7858,14 +7858,14 @@
         <v>Argentina</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="108" t="s">
+      <c r="D34" s="110" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="23">
         <f>IF(D34=Master!D30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F34" s="112"/>
+      <c r="F34" s="114"/>
       <c r="G34" s="23">
         <f>IF(F32=Master!F28,4,0)</f>
         <v>0</v>
@@ -7883,12 +7883,12 @@
         <f>IF(N32=Master!N28,4,0)</f>
         <v>0</v>
       </c>
-      <c r="N34" s="112"/>
+      <c r="N34" s="114"/>
       <c r="O34" s="23">
         <f>IF(P34=Master!P30,2,0)</f>
         <v>0</v>
       </c>
-      <c r="P34" s="110" t="s">
+      <c r="P34" s="112" t="s">
         <v>13</v>
       </c>
       <c r="Q34" s="7"/>
@@ -7910,11 +7910,11 @@
         <v>France</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="109"/>
+      <c r="D35" s="111"/>
       <c r="E35" s="7"/>
       <c r="F35" s="35"/>
       <c r="G35" s="7"/>
-      <c r="H35" s="105" t="s">
+      <c r="H35" s="107" t="s">
         <v>12</v>
       </c>
       <c r="I35" s="7"/>
@@ -7922,13 +7922,13 @@
         <v>81</v>
       </c>
       <c r="K35" s="7"/>
-      <c r="L35" s="110" t="s">
+      <c r="L35" s="112" t="s">
         <v>13</v>
       </c>
       <c r="M35" s="7"/>
       <c r="N35" s="35"/>
       <c r="O35" s="7"/>
-      <c r="P35" s="112"/>
+      <c r="P35" s="114"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="39" t="str">
         <f>D11</f>
@@ -7949,7 +7949,7 @@
       <c r="E36" s="7"/>
       <c r="F36" s="35"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="107"/>
+      <c r="H36" s="109"/>
       <c r="I36" s="24">
         <f>IF(H35=Master!H31,6,0)</f>
         <v>0</v>
@@ -7961,7 +7961,7 @@
         <f>IF(L35=Master!L31,6,0)</f>
         <v>0</v>
       </c>
-      <c r="L36" s="111"/>
+      <c r="L36" s="113"/>
       <c r="M36" s="7"/>
       <c r="N36" s="35"/>
       <c r="O36" s="7"/>
@@ -7982,7 +7982,7 @@
         <v>Italy</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="113" t="s">
+      <c r="D37" s="115" t="s">
         <v>136</v>
       </c>
       <c r="E37" s="7"/>
@@ -7990,17 +7990,17 @@
         <v>78</v>
       </c>
       <c r="G37" s="7"/>
-      <c r="H37" s="106"/>
+      <c r="H37" s="108"/>
       <c r="I37" s="7"/>
       <c r="J37" s="35"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="112"/>
+      <c r="L37" s="114"/>
       <c r="M37" s="7"/>
       <c r="N37" s="35" t="s">
         <v>80</v>
       </c>
       <c r="O37" s="7"/>
-      <c r="P37" s="108" t="s">
+      <c r="P37" s="110" t="s">
         <v>14</v>
       </c>
       <c r="Q37" s="7"/>
@@ -8022,12 +8022,12 @@
         <v>Canada</v>
       </c>
       <c r="C38" s="7"/>
-      <c r="D38" s="114"/>
+      <c r="D38" s="116"/>
       <c r="E38" s="23">
         <f>IF(D37=Master!D33,2,0)</f>
         <v>0</v>
       </c>
-      <c r="F38" s="108" t="s">
+      <c r="F38" s="110" t="s">
         <v>12</v>
       </c>
       <c r="G38" s="23">
@@ -8046,14 +8046,14 @@
         <f>IF(N38=Master!N34,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N38" s="108" t="s">
+      <c r="N38" s="110" t="s">
         <v>14</v>
       </c>
       <c r="O38" s="23">
         <f>IF(P37=Master!P33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P38" s="109"/>
+      <c r="P38" s="111"/>
       <c r="Q38" s="7"/>
       <c r="R38" s="39" t="str">
         <f>D18</f>
@@ -8072,7 +8072,7 @@
         <v>72</v>
       </c>
       <c r="E39" s="7"/>
-      <c r="F39" s="115"/>
+      <c r="F39" s="117"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
@@ -8080,7 +8080,7 @@
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
-      <c r="N39" s="115"/>
+      <c r="N39" s="117"/>
       <c r="O39" s="7"/>
       <c r="P39" s="35" t="s">
         <v>76</v>
@@ -8099,14 +8099,14 @@
         <v>Brasil</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="100" t="s">
+      <c r="D40" s="98" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="23">
         <f>IF(D40=Master!D36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F40" s="109"/>
+      <c r="F40" s="111"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
@@ -8114,12 +8114,12 @@
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
-      <c r="N40" s="109"/>
+      <c r="N40" s="111"/>
       <c r="O40" s="23">
         <f>IF(P40=Master!P36,2,0)</f>
         <v>0</v>
       </c>
-      <c r="P40" s="110" t="s">
+      <c r="P40" s="112" t="s">
         <v>140</v>
       </c>
       <c r="Q40" s="7"/>
@@ -8141,7 +8141,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="101"/>
+      <c r="D41" s="99"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -8153,7 +8153,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="112"/>
+      <c r="P41" s="114"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="39" t="str">
         <f>D25</f>
@@ -8221,13 +8221,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="J8:N8"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="D31:D32"/>
@@ -8244,6 +8237,13 @@
     <mergeCell ref="N38:N40"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="P40:P41"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="J8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -8283,26 +8283,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="86"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="91"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="84" t="s">
+      <c r="J1" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="85"/>
-      <c r="L1" s="85"/>
-      <c r="M1" s="85"/>
-      <c r="N1" s="86"/>
-      <c r="P1" s="84" t="s">
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="91"/>
+      <c r="P1" s="89" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="85"/>
-      <c r="R1" s="86"/>
+      <c r="Q1" s="90"/>
+      <c r="R1" s="91"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -8505,23 +8505,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="93" t="s">
+      <c r="B8" s="103" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="95"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="104"/>
+      <c r="E8" s="104"/>
+      <c r="F8" s="105"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="93" t="s">
+      <c r="J8" s="103" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="94"/>
-      <c r="L8" s="94"/>
-      <c r="M8" s="94"/>
-      <c r="N8" s="95"/>
+      <c r="K8" s="104"/>
+      <c r="L8" s="104"/>
+      <c r="M8" s="104"/>
+      <c r="N8" s="105"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -8711,23 +8711,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="93" t="s">
+      <c r="B15" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="94"/>
-      <c r="D15" s="94"/>
-      <c r="E15" s="94"/>
-      <c r="F15" s="95"/>
+      <c r="C15" s="104"/>
+      <c r="D15" s="104"/>
+      <c r="E15" s="104"/>
+      <c r="F15" s="105"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="93" t="s">
+      <c r="J15" s="103" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="94"/>
-      <c r="L15" s="94"/>
-      <c r="M15" s="94"/>
-      <c r="N15" s="95"/>
+      <c r="K15" s="104"/>
+      <c r="L15" s="104"/>
+      <c r="M15" s="104"/>
+      <c r="N15" s="105"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -8894,23 +8894,23 @@
       <c r="N21" s="52"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="93" t="s">
+      <c r="B22" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="94"/>
-      <c r="D22" s="94"/>
-      <c r="E22" s="94"/>
-      <c r="F22" s="95"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="105"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="93" t="s">
+      <c r="J22" s="103" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="94"/>
-      <c r="L22" s="94"/>
-      <c r="M22" s="94"/>
-      <c r="N22" s="95"/>
+      <c r="K22" s="104"/>
+      <c r="L22" s="104"/>
+      <c r="M22" s="104"/>
+      <c r="N22" s="105"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B23" s="56" t="s">
@@ -9131,7 +9131,7 @@
         <v>Ecuador</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="105" t="s">
+      <c r="D31" s="107" t="s">
         <v>45</v>
       </c>
       <c r="E31" s="7"/>
@@ -9149,7 +9149,7 @@
         <v>79</v>
       </c>
       <c r="O31" s="7"/>
-      <c r="P31" s="108" t="s">
+      <c r="P31" s="110" t="s">
         <v>41</v>
       </c>
       <c r="Q31" s="7"/>
@@ -9171,12 +9171,12 @@
         <v>Iran</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="106"/>
+      <c r="D32" s="108"/>
       <c r="E32" s="23">
         <f>IF(D31=Master!D27,2,0)</f>
         <v>0</v>
       </c>
-      <c r="F32" s="105" t="s">
+      <c r="F32" s="107" t="s">
         <v>45</v>
       </c>
       <c r="G32" s="7"/>
@@ -9186,14 +9186,14 @@
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
-      <c r="N32" s="108" t="s">
+      <c r="N32" s="110" t="s">
         <v>34</v>
       </c>
       <c r="O32" s="23">
         <f>IF(P31=Master!P27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P32" s="109"/>
+      <c r="P32" s="111"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="39" t="str">
         <f>D4</f>
@@ -9212,7 +9212,7 @@
         <v>70</v>
       </c>
       <c r="E33" s="7"/>
-      <c r="F33" s="107"/>
+      <c r="F33" s="109"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
@@ -9220,7 +9220,7 @@
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
-      <c r="N33" s="115"/>
+      <c r="N33" s="117"/>
       <c r="O33" s="7"/>
       <c r="P33" s="35" t="s">
         <v>74</v>
@@ -9239,14 +9239,14 @@
         <v>Argentina</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="108" t="s">
+      <c r="D34" s="110" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="23">
         <f>IF(D34=Master!D30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F34" s="106"/>
+      <c r="F34" s="108"/>
       <c r="G34" s="23">
         <f>IF(F32=Master!F28,4,0)</f>
         <v>0</v>
@@ -9264,12 +9264,12 @@
         <f>IF(N32=Master!N28,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N34" s="109"/>
+      <c r="N34" s="111"/>
       <c r="O34" s="23">
         <f>IF(P34=Master!P30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P34" s="108" t="s">
+      <c r="P34" s="110" t="s">
         <v>34</v>
       </c>
       <c r="Q34" s="7"/>
@@ -9291,11 +9291,11 @@
         <v>France</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="109"/>
+      <c r="D35" s="111"/>
       <c r="E35" s="7"/>
       <c r="F35" s="35"/>
       <c r="G35" s="7"/>
-      <c r="H35" s="105" t="s">
+      <c r="H35" s="107" t="s">
         <v>136</v>
       </c>
       <c r="I35" s="7"/>
@@ -9303,13 +9303,13 @@
         <v>81</v>
       </c>
       <c r="K35" s="7"/>
-      <c r="L35" s="105" t="s">
+      <c r="L35" s="107" t="s">
         <v>34</v>
       </c>
       <c r="M35" s="7"/>
       <c r="N35" s="35"/>
       <c r="O35" s="7"/>
-      <c r="P35" s="109"/>
+      <c r="P35" s="111"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="39" t="str">
         <f>D11</f>
@@ -9330,7 +9330,7 @@
       <c r="E36" s="7"/>
       <c r="F36" s="35"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="107"/>
+      <c r="H36" s="109"/>
       <c r="I36" s="24">
         <f>IF(H35=Master!H31,6,0)</f>
         <v>0</v>
@@ -9342,7 +9342,7 @@
         <f>IF(L35=Master!L31,6,0)</f>
         <v>0</v>
       </c>
-      <c r="L36" s="107"/>
+      <c r="L36" s="109"/>
       <c r="M36" s="7"/>
       <c r="N36" s="35"/>
       <c r="O36" s="7"/>
@@ -9363,7 +9363,7 @@
         <v>Italy</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="116" t="s">
+      <c r="D37" s="118" t="s">
         <v>136</v>
       </c>
       <c r="E37" s="7"/>
@@ -9371,17 +9371,17 @@
         <v>78</v>
       </c>
       <c r="G37" s="7"/>
-      <c r="H37" s="106"/>
+      <c r="H37" s="108"/>
       <c r="I37" s="7"/>
       <c r="J37" s="35"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="106"/>
+      <c r="L37" s="108"/>
       <c r="M37" s="7"/>
       <c r="N37" s="35" t="s">
         <v>80</v>
       </c>
       <c r="O37" s="7"/>
-      <c r="P37" s="108" t="s">
+      <c r="P37" s="110" t="s">
         <v>14</v>
       </c>
       <c r="Q37" s="7"/>
@@ -9403,12 +9403,12 @@
         <v>Canada</v>
       </c>
       <c r="C38" s="7"/>
-      <c r="D38" s="117"/>
+      <c r="D38" s="119"/>
       <c r="E38" s="23">
         <f>IF(D37=Master!D33,2,0)</f>
         <v>0</v>
       </c>
-      <c r="F38" s="105" t="s">
+      <c r="F38" s="107" t="s">
         <v>136</v>
       </c>
       <c r="G38" s="23">
@@ -9427,14 +9427,14 @@
         <f>IF(N38=Master!N34,4,0)</f>
         <v>0</v>
       </c>
-      <c r="N38" s="105" t="s">
+      <c r="N38" s="107" t="s">
         <v>140</v>
       </c>
       <c r="O38" s="23">
         <f>IF(P37=Master!P33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P38" s="109"/>
+      <c r="P38" s="111"/>
       <c r="Q38" s="7"/>
       <c r="R38" s="39" t="str">
         <f>D18</f>
@@ -9453,7 +9453,7 @@
         <v>72</v>
       </c>
       <c r="E39" s="7"/>
-      <c r="F39" s="107"/>
+      <c r="F39" s="109"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
@@ -9461,7 +9461,7 @@
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
-      <c r="N39" s="107"/>
+      <c r="N39" s="109"/>
       <c r="O39" s="7"/>
       <c r="P39" s="35" t="s">
         <v>76</v>
@@ -9480,14 +9480,14 @@
         <v>Brasil</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="108" t="s">
+      <c r="D40" s="110" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="23">
         <f>IF(D40=Master!D36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F40" s="106"/>
+      <c r="F40" s="108"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
@@ -9495,12 +9495,12 @@
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
-      <c r="N40" s="106"/>
+      <c r="N40" s="108"/>
       <c r="O40" s="23">
         <f>IF(P40=Master!P36,2,0)</f>
         <v>0</v>
       </c>
-      <c r="P40" s="105" t="s">
+      <c r="P40" s="107" t="s">
         <v>140</v>
       </c>
       <c r="Q40" s="7"/>
@@ -9522,7 +9522,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="109"/>
+      <c r="D41" s="111"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -9534,7 +9534,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="106"/>
+      <c r="P41" s="108"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="39" t="str">
         <f>D25</f>
@@ -9602,13 +9602,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="J8:N8"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="D31:D32"/>
@@ -9625,6 +9618,13 @@
     <mergeCell ref="N38:N40"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="P40:P41"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="J8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -9664,10 +9664,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="118" t="s">
+      <c r="B5" s="120" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="119"/>
+      <c r="C5" s="121"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" s="47"/>
@@ -9742,26 +9742,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="86"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="91"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="84" t="s">
+      <c r="J1" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="85"/>
-      <c r="L1" s="85"/>
-      <c r="M1" s="85"/>
-      <c r="N1" s="86"/>
-      <c r="P1" s="84" t="s">
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="91"/>
+      <c r="P1" s="89" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="85"/>
-      <c r="R1" s="86"/>
+      <c r="Q1" s="90"/>
+      <c r="R1" s="91"/>
       <c r="W1" s="1" t="s">
         <v>92</v>
       </c>
@@ -10069,23 +10069,23 @@
       </c>
     </row>
     <row r="8" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B8" s="93" t="s">
+      <c r="B8" s="103" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="95"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="104"/>
+      <c r="E8" s="104"/>
+      <c r="F8" s="105"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="93" t="s">
+      <c r="J8" s="103" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="94"/>
-      <c r="L8" s="94"/>
-      <c r="M8" s="94"/>
-      <c r="N8" s="95"/>
+      <c r="K8" s="104"/>
+      <c r="L8" s="104"/>
+      <c r="M8" s="104"/>
+      <c r="N8" s="105"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -10373,23 +10373,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B15" s="93" t="s">
+      <c r="B15" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="94"/>
-      <c r="D15" s="94"/>
-      <c r="E15" s="94"/>
-      <c r="F15" s="95"/>
+      <c r="C15" s="104"/>
+      <c r="D15" s="104"/>
+      <c r="E15" s="104"/>
+      <c r="F15" s="105"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="93" t="s">
+      <c r="J15" s="103" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="94"/>
-      <c r="L15" s="94"/>
-      <c r="M15" s="94"/>
-      <c r="N15" s="95"/>
+      <c r="K15" s="104"/>
+      <c r="L15" s="104"/>
+      <c r="M15" s="104"/>
+      <c r="N15" s="105"/>
     </row>
     <row r="16" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -10654,23 +10654,23 @@
       <c r="N21" s="52"/>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B22" s="93" t="s">
+      <c r="B22" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="94"/>
-      <c r="D22" s="94"/>
-      <c r="E22" s="94"/>
-      <c r="F22" s="95"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="105"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="93" t="s">
+      <c r="J22" s="103" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="94"/>
-      <c r="L22" s="94"/>
-      <c r="M22" s="94"/>
-      <c r="N22" s="95"/>
+      <c r="K22" s="104"/>
+      <c r="L22" s="104"/>
+      <c r="M22" s="104"/>
+      <c r="N22" s="105"/>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B23" s="56" t="s">
@@ -10988,7 +10988,7 @@
         <v>8</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="120" t="s">
+      <c r="D31" s="122" t="s">
         <v>8</v>
       </c>
       <c r="E31" s="7"/>
@@ -11006,7 +11006,7 @@
         <v>79</v>
       </c>
       <c r="O31" s="7"/>
-      <c r="P31" s="120" t="s">
+      <c r="P31" s="122" t="s">
         <v>31</v>
       </c>
       <c r="Q31" s="7"/>
@@ -11026,12 +11026,12 @@
         <v>24</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="121"/>
+      <c r="D32" s="123"/>
       <c r="E32" s="23">
         <f>IF(D31=Master!D27,2,0)</f>
         <v>0</v>
       </c>
-      <c r="F32" s="120" t="s">
+      <c r="F32" s="122" t="s">
         <v>8</v>
       </c>
       <c r="G32" s="7"/>
@@ -11041,14 +11041,14 @@
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
-      <c r="N32" s="120" t="s">
+      <c r="N32" s="122" t="s">
         <v>47</v>
       </c>
       <c r="O32" s="23">
         <f>IF(P31=Master!P27,2,0)</f>
         <v>0</v>
       </c>
-      <c r="P32" s="121"/>
+      <c r="P32" s="123"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="42" t="s">
         <v>31</v>
@@ -11066,7 +11066,7 @@
         <v>70</v>
       </c>
       <c r="E33" s="7"/>
-      <c r="F33" s="122"/>
+      <c r="F33" s="124"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
@@ -11074,7 +11074,7 @@
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
-      <c r="N33" s="122"/>
+      <c r="N33" s="124"/>
       <c r="O33" s="7"/>
       <c r="P33" s="35" t="s">
         <v>74</v>
@@ -11092,14 +11092,14 @@
         <v>10</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="120" t="s">
+      <c r="D34" s="122" t="s">
         <v>10</v>
       </c>
       <c r="E34" s="23">
         <f>IF(D34=Master!D30,2,0)</f>
         <v>0</v>
       </c>
-      <c r="F34" s="121"/>
+      <c r="F34" s="123"/>
       <c r="G34" s="23">
         <f>IF(F32=Master!F28,4,0)</f>
         <v>0</v>
@@ -11117,12 +11117,12 @@
         <f>IF(N32=Master!N28,4,0)</f>
         <v>0</v>
       </c>
-      <c r="N34" s="121"/>
+      <c r="N34" s="123"/>
       <c r="O34" s="23">
         <f>IF(P34=Master!P30,2,0)</f>
         <v>0</v>
       </c>
-      <c r="P34" s="120" t="s">
+      <c r="P34" s="122" t="s">
         <v>47</v>
       </c>
       <c r="Q34" s="7"/>
@@ -11142,11 +11142,11 @@
         <v>25</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="121"/>
+      <c r="D35" s="123"/>
       <c r="E35" s="7"/>
       <c r="F35" s="35"/>
       <c r="G35" s="7"/>
-      <c r="H35" s="120" t="s">
+      <c r="H35" s="122" t="s">
         <v>14</v>
       </c>
       <c r="I35" s="7"/>
@@ -11154,13 +11154,13 @@
         <v>81</v>
       </c>
       <c r="K35" s="7"/>
-      <c r="L35" s="120" t="s">
+      <c r="L35" s="122" t="s">
         <v>47</v>
       </c>
       <c r="M35" s="7"/>
       <c r="N35" s="35"/>
       <c r="O35" s="7"/>
-      <c r="P35" s="121"/>
+      <c r="P35" s="123"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="42" t="s">
         <v>34</v>
@@ -11180,7 +11180,7 @@
       <c r="E36" s="7"/>
       <c r="F36" s="35"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="122"/>
+      <c r="H36" s="124"/>
       <c r="I36" s="24">
         <f>IF(H35=Master!H31,6,0)</f>
         <v>0</v>
@@ -11192,7 +11192,7 @@
         <f>IF(L35=Master!L31,6,0)</f>
         <v>0</v>
       </c>
-      <c r="L36" s="122"/>
+      <c r="L36" s="124"/>
       <c r="M36" s="7"/>
       <c r="N36" s="35"/>
       <c r="O36" s="7"/>
@@ -11212,7 +11212,7 @@
         <v>12</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="123" t="s">
+      <c r="D37" s="125" t="s">
         <v>12</v>
       </c>
       <c r="E37" s="7"/>
@@ -11220,17 +11220,17 @@
         <v>78</v>
       </c>
       <c r="G37" s="7"/>
-      <c r="H37" s="121"/>
+      <c r="H37" s="123"/>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="121"/>
+      <c r="L37" s="123"/>
       <c r="M37" s="7"/>
       <c r="N37" s="35" t="s">
         <v>80</v>
       </c>
       <c r="O37" s="7"/>
-      <c r="P37" s="120" t="s">
+      <c r="P37" s="122" t="s">
         <v>49</v>
       </c>
       <c r="Q37" s="7"/>
@@ -11250,12 +11250,12 @@
         <v>13</v>
       </c>
       <c r="C38" s="7"/>
-      <c r="D38" s="124"/>
+      <c r="D38" s="126"/>
       <c r="E38" s="23">
         <f>IF(D37=Master!D33,2,0)</f>
         <v>0</v>
       </c>
-      <c r="F38" s="125" t="s">
+      <c r="F38" s="127" t="s">
         <v>14</v>
       </c>
       <c r="G38" s="23">
@@ -11274,14 +11274,14 @@
         <f>IF(N38=Master!N34,4,0)</f>
         <v>0</v>
       </c>
-      <c r="N38" s="120" t="s">
+      <c r="N38" s="122" t="s">
         <v>41</v>
       </c>
       <c r="O38" s="23">
         <f>IF(P37=Master!P33,2,0)</f>
         <v>0</v>
       </c>
-      <c r="P38" s="121"/>
+      <c r="P38" s="123"/>
       <c r="Q38" s="7"/>
       <c r="R38" s="42" t="s">
         <v>37</v>
@@ -11299,7 +11299,7 @@
         <v>72</v>
       </c>
       <c r="E39" s="7"/>
-      <c r="F39" s="126"/>
+      <c r="F39" s="128"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
@@ -11307,7 +11307,7 @@
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
-      <c r="N39" s="122"/>
+      <c r="N39" s="124"/>
       <c r="O39" s="7"/>
       <c r="P39" s="35" t="s">
         <v>76</v>
@@ -11325,14 +11325,14 @@
         <v>14</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="120" t="s">
+      <c r="D40" s="122" t="s">
         <v>14</v>
       </c>
       <c r="E40" s="23">
         <f>IF(D40=Master!D36,2,0)</f>
         <v>0</v>
       </c>
-      <c r="F40" s="127"/>
+      <c r="F40" s="129"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
@@ -11340,12 +11340,12 @@
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
-      <c r="N40" s="121"/>
+      <c r="N40" s="123"/>
       <c r="O40" s="23">
         <f>IF(P40=Master!P36,2,0)</f>
         <v>0</v>
       </c>
-      <c r="P40" s="120" t="s">
+      <c r="P40" s="122" t="s">
         <v>41</v>
       </c>
       <c r="Q40" s="7"/>
@@ -11365,7 +11365,7 @@
         <v>52</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="121"/>
+      <c r="D41" s="123"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -11377,7 +11377,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="121"/>
+      <c r="P41" s="123"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="42" t="s">
         <v>41</v>
@@ -11444,6 +11444,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="J8:N8"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="D31:D32"/>
@@ -11460,13 +11467,6 @@
     <mergeCell ref="N38:N40"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="P40:P41"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="J8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -11760,7 +11760,7 @@
       <c r="B11" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="C11" s="128" t="s">
+      <c r="C11" s="130" t="s">
         <v>110</v>
       </c>
       <c r="D11" s="69"/>
@@ -11782,7 +11782,7 @@
       <c r="B12" s="48" t="s">
         <v>115</v>
       </c>
-      <c r="C12" s="128"/>
+      <c r="C12" s="130"/>
       <c r="D12" s="69"/>
       <c r="E12" s="69"/>
       <c r="F12" s="69"/>
@@ -11900,7 +11900,7 @@
       <c r="B17" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="C17" s="128" t="s">
+      <c r="C17" s="130" t="s">
         <v>110</v>
       </c>
       <c r="D17" s="69"/>
@@ -11922,7 +11922,7 @@
       <c r="B18" s="49" t="s">
         <v>116</v>
       </c>
-      <c r="C18" s="128"/>
+      <c r="C18" s="130"/>
       <c r="D18" s="69"/>
       <c r="E18" s="69"/>
       <c r="F18" s="69"/>

</xml_diff>

<commit_message>
my picked unlocked css work fully complete
</commit_message>
<xml_diff>
--- a/excel docs/java testing-audit info.xlsx
+++ b/excel docs/java testing-audit info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joecollins/Desktop/documents/personal-projects/world-cup-heroku/excel docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8DC836-0192-9649-BE87-56D3E22C0F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40343C96-0BED-0A42-B823-547F0FB007CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="148">
   <si>
     <t>A1</t>
   </si>
@@ -1469,24 +1469,24 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1496,6 +1496,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1519,18 +1531,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1922,11 +1922,11 @@
       <c r="F1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="89" t="s">
+      <c r="J1" s="86" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="90"/>
-      <c r="L1" s="91"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="88"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B2" s="14" t="s">
@@ -2246,7 +2246,7 @@
         <v>Ecuador</v>
       </c>
       <c r="C27" s="7"/>
-      <c r="D27" s="86" t="s">
+      <c r="D27" s="89" t="s">
         <v>134</v>
       </c>
       <c r="E27" s="7"/>
@@ -2260,7 +2260,7 @@
       <c r="M27" s="7"/>
       <c r="N27" s="7"/>
       <c r="O27" s="7"/>
-      <c r="P27" s="86" t="s">
+      <c r="P27" s="89" t="s">
         <v>41</v>
       </c>
       <c r="Q27" s="7"/>
@@ -2282,9 +2282,9 @@
         <v>Iran</v>
       </c>
       <c r="C28" s="7"/>
-      <c r="D28" s="88"/>
+      <c r="D28" s="90"/>
       <c r="E28" s="7"/>
-      <c r="F28" s="86" t="s">
+      <c r="F28" s="89" t="s">
         <v>25</v>
       </c>
       <c r="G28" s="7"/>
@@ -2294,11 +2294,11 @@
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
       <c r="M28" s="7"/>
-      <c r="N28" s="86" t="s">
+      <c r="N28" s="89" t="s">
         <v>34</v>
       </c>
       <c r="O28" s="7"/>
-      <c r="P28" s="88"/>
+      <c r="P28" s="90"/>
       <c r="Q28" s="7"/>
       <c r="R28" s="15" t="str">
         <f>B3</f>
@@ -2315,7 +2315,7 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
-      <c r="F29" s="87"/>
+      <c r="F29" s="91"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
@@ -2323,7 +2323,7 @@
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
-      <c r="N29" s="87"/>
+      <c r="N29" s="91"/>
       <c r="O29" s="7"/>
       <c r="P29" s="7"/>
       <c r="Q29" s="7"/>
@@ -2340,11 +2340,11 @@
         <v>Argentina</v>
       </c>
       <c r="C30" s="7"/>
-      <c r="D30" s="86" t="s">
+      <c r="D30" s="89" t="s">
         <v>25</v>
       </c>
       <c r="E30" s="7"/>
-      <c r="F30" s="88"/>
+      <c r="F30" s="90"/>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
@@ -2352,9 +2352,9 @@
       <c r="K30" s="7"/>
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
-      <c r="N30" s="88"/>
+      <c r="N30" s="90"/>
       <c r="O30" s="7"/>
-      <c r="P30" s="86" t="s">
+      <c r="P30" s="89" t="s">
         <v>34</v>
       </c>
       <c r="Q30" s="7"/>
@@ -2376,7 +2376,7 @@
         <v>France</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="88"/>
+      <c r="D31" s="90"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
@@ -2392,7 +2392,7 @@
       <c r="M31" s="7"/>
       <c r="N31" s="7"/>
       <c r="O31" s="7"/>
-      <c r="P31" s="88"/>
+      <c r="P31" s="90"/>
       <c r="Q31" s="7"/>
       <c r="R31" s="15" t="str">
         <f>B9</f>
@@ -2436,7 +2436,7 @@
         <v>Italy</v>
       </c>
       <c r="C33" s="7"/>
-      <c r="D33" s="86" t="s">
+      <c r="D33" s="89" t="s">
         <v>139</v>
       </c>
       <c r="E33" s="7"/>
@@ -2450,7 +2450,7 @@
       <c r="M33" s="7"/>
       <c r="N33" s="7"/>
       <c r="O33" s="7"/>
-      <c r="P33" s="86" t="s">
+      <c r="P33" s="89" t="s">
         <v>14</v>
       </c>
       <c r="Q33" s="7"/>
@@ -2472,9 +2472,9 @@
         <v>Canada</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="88"/>
+      <c r="D34" s="90"/>
       <c r="E34" s="7"/>
-      <c r="F34" s="86" t="s">
+      <c r="F34" s="89" t="s">
         <v>12</v>
       </c>
       <c r="G34" s="7"/>
@@ -2484,11 +2484,11 @@
       <c r="K34" s="7"/>
       <c r="L34" s="7"/>
       <c r="M34" s="7"/>
-      <c r="N34" s="86" t="s">
+      <c r="N34" s="89" t="s">
         <v>14</v>
       </c>
       <c r="O34" s="7"/>
-      <c r="P34" s="88"/>
+      <c r="P34" s="90"/>
       <c r="Q34" s="7"/>
       <c r="R34" s="15" t="str">
         <f>B15</f>
@@ -2505,7 +2505,7 @@
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
-      <c r="F35" s="87"/>
+      <c r="F35" s="91"/>
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
@@ -2513,7 +2513,7 @@
       <c r="K35" s="7"/>
       <c r="L35" s="7"/>
       <c r="M35" s="7"/>
-      <c r="N35" s="87"/>
+      <c r="N35" s="91"/>
       <c r="O35" s="7"/>
       <c r="P35" s="7"/>
       <c r="Q35" s="7"/>
@@ -2530,11 +2530,11 @@
         <v>Brasil</v>
       </c>
       <c r="C36" s="7"/>
-      <c r="D36" s="86" t="s">
+      <c r="D36" s="89" t="s">
         <v>12</v>
       </c>
       <c r="E36" s="7"/>
-      <c r="F36" s="88"/>
+      <c r="F36" s="90"/>
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
       <c r="I36" s="7"/>
@@ -2542,9 +2542,9 @@
       <c r="K36" s="7"/>
       <c r="L36" s="7"/>
       <c r="M36" s="7"/>
-      <c r="N36" s="88"/>
+      <c r="N36" s="90"/>
       <c r="O36" s="7"/>
-      <c r="P36" s="86" t="s">
+      <c r="P36" s="89" t="s">
         <v>137</v>
       </c>
       <c r="Q36" s="7"/>
@@ -2566,7 +2566,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="88"/>
+      <c r="D37" s="90"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
@@ -2578,7 +2578,7 @@
       <c r="M37" s="7"/>
       <c r="N37" s="7"/>
       <c r="O37" s="7"/>
-      <c r="P37" s="88"/>
+      <c r="P37" s="90"/>
       <c r="Q37" s="7"/>
       <c r="R37" s="15" t="str">
         <f>B21</f>
@@ -2613,6 +2613,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="N28:N30"/>
+    <mergeCell ref="N34:N36"/>
+    <mergeCell ref="P27:P28"/>
+    <mergeCell ref="P30:P31"/>
+    <mergeCell ref="P33:P34"/>
+    <mergeCell ref="P36:P37"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="D27:D28"/>
     <mergeCell ref="D30:D31"/>
@@ -2622,12 +2628,6 @@
     <mergeCell ref="F34:F36"/>
     <mergeCell ref="H31:H33"/>
     <mergeCell ref="L31:L33"/>
-    <mergeCell ref="N28:N30"/>
-    <mergeCell ref="N34:N36"/>
-    <mergeCell ref="P27:P28"/>
-    <mergeCell ref="P30:P31"/>
-    <mergeCell ref="P33:P34"/>
-    <mergeCell ref="P36:P37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -2683,7 +2683,7 @@
   <dimension ref="A1:T43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2714,26 +2714,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="86" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="91"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="88"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="89" t="s">
+      <c r="J1" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="90"/>
-      <c r="L1" s="90"/>
-      <c r="M1" s="90"/>
-      <c r="N1" s="91"/>
-      <c r="P1" s="89" t="s">
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="88"/>
+      <c r="P1" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="90"/>
-      <c r="R1" s="91"/>
+      <c r="Q1" s="87"/>
+      <c r="R1" s="88"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -2936,23 +2936,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="103" t="s">
+      <c r="B8" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="104"/>
-      <c r="D8" s="104"/>
-      <c r="E8" s="104"/>
-      <c r="F8" s="105"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="96"/>
+      <c r="E8" s="96"/>
+      <c r="F8" s="97"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="103" t="s">
+      <c r="J8" s="95" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="104"/>
-      <c r="L8" s="104"/>
-      <c r="M8" s="104"/>
-      <c r="N8" s="105"/>
+      <c r="K8" s="96"/>
+      <c r="L8" s="96"/>
+      <c r="M8" s="96"/>
+      <c r="N8" s="97"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -3142,23 +3142,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="103" t="s">
+      <c r="B15" s="95" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="104"/>
-      <c r="D15" s="104"/>
-      <c r="E15" s="104"/>
-      <c r="F15" s="105"/>
+      <c r="C15" s="96"/>
+      <c r="D15" s="96"/>
+      <c r="E15" s="96"/>
+      <c r="F15" s="97"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="103" t="s">
+      <c r="J15" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="104"/>
-      <c r="L15" s="104"/>
-      <c r="M15" s="104"/>
-      <c r="N15" s="105"/>
+      <c r="K15" s="96"/>
+      <c r="L15" s="96"/>
+      <c r="M15" s="96"/>
+      <c r="N15" s="97"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -3279,10 +3279,10 @@
         <f t="shared" ref="N19:N20" si="5">IF(J19=L19,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Q19" s="106" t="s">
+      <c r="Q19" s="98" t="s">
         <v>82</v>
       </c>
-      <c r="R19" s="106"/>
+      <c r="R19" s="98"/>
     </row>
     <row r="20" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="27" t="s">
@@ -3337,23 +3337,23 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="103" t="s">
+      <c r="B22" s="95" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="104"/>
-      <c r="D22" s="104"/>
-      <c r="E22" s="104"/>
-      <c r="F22" s="105"/>
+      <c r="C22" s="96"/>
+      <c r="D22" s="96"/>
+      <c r="E22" s="96"/>
+      <c r="F22" s="97"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="103" t="s">
+      <c r="J22" s="95" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="104"/>
-      <c r="L22" s="104"/>
-      <c r="M22" s="104"/>
-      <c r="N22" s="105"/>
+      <c r="K22" s="96"/>
+      <c r="L22" s="96"/>
+      <c r="M22" s="96"/>
+      <c r="N22" s="97"/>
       <c r="Q22" s="49"/>
       <c r="R22" s="32" t="s">
         <v>85</v>
@@ -3584,7 +3584,7 @@
         <v>Ecuador</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="98" t="s">
+      <c r="D31" s="102" t="s">
         <v>134</v>
       </c>
       <c r="E31" s="7"/>
@@ -3602,7 +3602,7 @@
         <v>79</v>
       </c>
       <c r="O31" s="7"/>
-      <c r="P31" s="98" t="s">
+      <c r="P31" s="102" t="s">
         <v>41</v>
       </c>
       <c r="Q31" s="7"/>
@@ -3624,12 +3624,12 @@
         <v>Iran</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="99"/>
+      <c r="D32" s="103"/>
       <c r="E32" s="23">
         <f>IF(D31=Master!D27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F32" s="98" t="s">
+      <c r="F32" s="102" t="s">
         <v>25</v>
       </c>
       <c r="G32" s="7"/>
@@ -3639,14 +3639,14 @@
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
-      <c r="N32" s="98" t="s">
+      <c r="N32" s="102" t="s">
         <v>34</v>
       </c>
       <c r="O32" s="23">
         <f>IF(P31=Master!P27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P32" s="99"/>
+      <c r="P32" s="103"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="39" t="str">
         <f>D4</f>
@@ -3665,7 +3665,7 @@
         <v>70</v>
       </c>
       <c r="E33" s="7"/>
-      <c r="F33" s="100"/>
+      <c r="F33" s="104"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
@@ -3673,9 +3673,11 @@
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
-      <c r="N33" s="100"/>
+      <c r="N33" s="104"/>
       <c r="O33" s="7"/>
-      <c r="P33" s="35"/>
+      <c r="P33" s="35" t="s">
+        <v>74</v>
+      </c>
       <c r="Q33" s="7"/>
       <c r="R33" s="35"/>
       <c r="S33" s="7"/>
@@ -3690,14 +3692,14 @@
         <v>Argentina</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="98" t="s">
+      <c r="D34" s="102" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="23">
         <f>IF(D34=Master!D30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F34" s="99"/>
+      <c r="F34" s="103"/>
       <c r="G34" s="23">
         <f>IF(F32=Master!F28,4,0)</f>
         <v>4</v>
@@ -3715,12 +3717,12 @@
         <f>IF(N32=Master!N28,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N34" s="99"/>
+      <c r="N34" s="103"/>
       <c r="O34" s="23">
         <f>IF(P34=Master!P30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P34" s="98" t="s">
+      <c r="P34" s="102" t="s">
         <v>34</v>
       </c>
       <c r="Q34" s="7"/>
@@ -3742,11 +3744,11 @@
         <v>France</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="99"/>
+      <c r="D35" s="103"/>
       <c r="E35" s="7"/>
       <c r="F35" s="35"/>
       <c r="G35" s="7"/>
-      <c r="H35" s="98" t="s">
+      <c r="H35" s="102" t="s">
         <v>25</v>
       </c>
       <c r="I35" s="7"/>
@@ -3754,13 +3756,13 @@
         <v>81</v>
       </c>
       <c r="K35" s="7"/>
-      <c r="L35" s="98" t="s">
+      <c r="L35" s="102" t="s">
         <v>14</v>
       </c>
       <c r="M35" s="7"/>
       <c r="N35" s="35"/>
       <c r="O35" s="7"/>
-      <c r="P35" s="99"/>
+      <c r="P35" s="103"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="39" t="str">
         <f>D11</f>
@@ -3781,7 +3783,7 @@
       <c r="E36" s="7"/>
       <c r="F36" s="35"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="100"/>
+      <c r="H36" s="104"/>
       <c r="I36" s="24">
         <f>IF(H35=Master!H31,6,0)</f>
         <v>6</v>
@@ -3793,7 +3795,7 @@
         <f>IF(L35=Master!L31,6,0)</f>
         <v>6</v>
       </c>
-      <c r="L36" s="100"/>
+      <c r="L36" s="104"/>
       <c r="M36" s="7"/>
       <c r="N36" s="35"/>
       <c r="O36" s="7"/>
@@ -3814,7 +3816,7 @@
         <v>Italy</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="101" t="s">
+      <c r="D37" s="105" t="s">
         <v>139</v>
       </c>
       <c r="E37" s="7"/>
@@ -3822,17 +3824,17 @@
         <v>78</v>
       </c>
       <c r="G37" s="7"/>
-      <c r="H37" s="99"/>
+      <c r="H37" s="103"/>
       <c r="I37" s="7"/>
       <c r="J37" s="35"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="99"/>
+      <c r="L37" s="103"/>
       <c r="M37" s="7"/>
       <c r="N37" s="35" t="s">
         <v>80</v>
       </c>
       <c r="O37" s="7"/>
-      <c r="P37" s="98" t="s">
+      <c r="P37" s="102" t="s">
         <v>14</v>
       </c>
       <c r="Q37" s="7"/>
@@ -3854,12 +3856,12 @@
         <v>Canada</v>
       </c>
       <c r="C38" s="7"/>
-      <c r="D38" s="102"/>
+      <c r="D38" s="106"/>
       <c r="E38" s="23">
         <f>IF(D37=Master!D33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F38" s="95" t="s">
+      <c r="F38" s="99" t="s">
         <v>12</v>
       </c>
       <c r="G38" s="23">
@@ -3878,14 +3880,14 @@
         <f>IF(N38=Master!N34,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N38" s="98" t="s">
+      <c r="N38" s="102" t="s">
         <v>14</v>
       </c>
       <c r="O38" s="23">
         <f>IF(P37=Master!P33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P38" s="99"/>
+      <c r="P38" s="103"/>
       <c r="Q38" s="7"/>
       <c r="R38" s="39" t="str">
         <f>D18</f>
@@ -3904,7 +3906,7 @@
         <v>72</v>
       </c>
       <c r="E39" s="7"/>
-      <c r="F39" s="96"/>
+      <c r="F39" s="100"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
@@ -3912,7 +3914,7 @@
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
-      <c r="N39" s="100"/>
+      <c r="N39" s="104"/>
       <c r="O39" s="7"/>
       <c r="P39" s="35" t="s">
         <v>76</v>
@@ -3931,14 +3933,14 @@
         <v>Brasil</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="98" t="s">
+      <c r="D40" s="102" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="23">
         <f>IF(D40=Master!D36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F40" s="97"/>
+      <c r="F40" s="101"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
@@ -3946,12 +3948,12 @@
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
-      <c r="N40" s="99"/>
+      <c r="N40" s="103"/>
       <c r="O40" s="23">
         <f>IF(P40=Master!P36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P40" s="98" t="s">
+      <c r="P40" s="102" t="s">
         <v>137</v>
       </c>
       <c r="Q40" s="7"/>
@@ -3973,7 +3975,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="99"/>
+      <c r="D41" s="103"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -3985,7 +3987,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="99"/>
+      <c r="P41" s="103"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="39" t="str">
         <f>D25</f>
@@ -4053,16 +4055,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J22:N22"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="J8:N8"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="Q19:R19"/>
     <mergeCell ref="F38:F40"/>
     <mergeCell ref="P37:P38"/>
     <mergeCell ref="P40:P41"/>
@@ -4077,6 +4069,16 @@
     <mergeCell ref="D37:D38"/>
     <mergeCell ref="H35:H37"/>
     <mergeCell ref="L35:L37"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J22:N22"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="Q19:R19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -4119,26 +4121,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="86" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="91"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="88"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="89" t="s">
+      <c r="J1" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="90"/>
-      <c r="L1" s="90"/>
-      <c r="M1" s="90"/>
-      <c r="N1" s="91"/>
-      <c r="P1" s="89" t="s">
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="88"/>
+      <c r="P1" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="90"/>
-      <c r="R1" s="91"/>
+      <c r="Q1" s="87"/>
+      <c r="R1" s="88"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -4341,23 +4343,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="103" t="s">
+      <c r="B8" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="104"/>
-      <c r="D8" s="104"/>
-      <c r="E8" s="104"/>
-      <c r="F8" s="105"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="96"/>
+      <c r="E8" s="96"/>
+      <c r="F8" s="97"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="103" t="s">
+      <c r="J8" s="95" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="104"/>
-      <c r="L8" s="104"/>
-      <c r="M8" s="104"/>
-      <c r="N8" s="105"/>
+      <c r="K8" s="96"/>
+      <c r="L8" s="96"/>
+      <c r="M8" s="96"/>
+      <c r="N8" s="97"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -4547,23 +4549,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="103" t="s">
+      <c r="B15" s="95" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="104"/>
-      <c r="D15" s="104"/>
-      <c r="E15" s="104"/>
-      <c r="F15" s="105"/>
+      <c r="C15" s="96"/>
+      <c r="D15" s="96"/>
+      <c r="E15" s="96"/>
+      <c r="F15" s="97"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="103" t="s">
+      <c r="J15" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="104"/>
-      <c r="L15" s="104"/>
-      <c r="M15" s="104"/>
-      <c r="N15" s="105"/>
+      <c r="K15" s="96"/>
+      <c r="L15" s="96"/>
+      <c r="M15" s="96"/>
+      <c r="N15" s="97"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -4684,10 +4686,10 @@
         <f t="shared" ref="N19:N20" si="5">IF(J19=L19,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Q19" s="106" t="s">
+      <c r="Q19" s="98" t="s">
         <v>82</v>
       </c>
-      <c r="R19" s="106"/>
+      <c r="R19" s="98"/>
     </row>
     <row r="20" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="27" t="s">
@@ -4742,23 +4744,23 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="103" t="s">
+      <c r="B22" s="95" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="104"/>
-      <c r="D22" s="104"/>
-      <c r="E22" s="104"/>
-      <c r="F22" s="105"/>
+      <c r="C22" s="96"/>
+      <c r="D22" s="96"/>
+      <c r="E22" s="96"/>
+      <c r="F22" s="97"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="103" t="s">
+      <c r="J22" s="95" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="104"/>
-      <c r="L22" s="104"/>
-      <c r="M22" s="104"/>
-      <c r="N22" s="105"/>
+      <c r="K22" s="96"/>
+      <c r="L22" s="96"/>
+      <c r="M22" s="96"/>
+      <c r="N22" s="97"/>
       <c r="Q22" s="49"/>
       <c r="R22" s="32" t="s">
         <v>85</v>
@@ -4989,7 +4991,7 @@
         <v>Ecuador</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="98" t="s">
+      <c r="D31" s="102" t="s">
         <v>134</v>
       </c>
       <c r="E31" s="7"/>
@@ -5007,7 +5009,7 @@
         <v>79</v>
       </c>
       <c r="O31" s="7"/>
-      <c r="P31" s="98" t="s">
+      <c r="P31" s="102" t="s">
         <v>41</v>
       </c>
       <c r="Q31" s="7"/>
@@ -5029,12 +5031,12 @@
         <v>Iran</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="99"/>
+      <c r="D32" s="103"/>
       <c r="E32" s="23">
         <f>IF(D31=Master!D27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F32" s="98" t="s">
+      <c r="F32" s="102" t="s">
         <v>25</v>
       </c>
       <c r="G32" s="7"/>
@@ -5044,14 +5046,14 @@
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
-      <c r="N32" s="98" t="s">
+      <c r="N32" s="102" t="s">
         <v>34</v>
       </c>
       <c r="O32" s="23">
         <f>IF(P31=Master!P27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P32" s="99"/>
+      <c r="P32" s="103"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="81" t="str">
         <f>D4</f>
@@ -5070,7 +5072,7 @@
         <v>70</v>
       </c>
       <c r="E33" s="7"/>
-      <c r="F33" s="100"/>
+      <c r="F33" s="104"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
@@ -5078,7 +5080,7 @@
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
-      <c r="N33" s="100"/>
+      <c r="N33" s="104"/>
       <c r="O33" s="7"/>
       <c r="P33" s="35"/>
       <c r="Q33" s="7"/>
@@ -5095,14 +5097,14 @@
         <v>Argentina</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="98" t="s">
+      <c r="D34" s="102" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="23">
         <f>IF(D34=Master!D30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F34" s="99"/>
+      <c r="F34" s="103"/>
       <c r="G34" s="23">
         <f>IF(F32=Master!F28,4,0)</f>
         <v>4</v>
@@ -5120,12 +5122,12 @@
         <f>IF(N32=Master!N28,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N34" s="99"/>
+      <c r="N34" s="103"/>
       <c r="O34" s="23">
         <f>IF(P34=Master!P30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P34" s="98" t="s">
+      <c r="P34" s="102" t="s">
         <v>34</v>
       </c>
       <c r="Q34" s="7"/>
@@ -5147,11 +5149,11 @@
         <v>France</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="99"/>
+      <c r="D35" s="103"/>
       <c r="E35" s="7"/>
       <c r="F35" s="35"/>
       <c r="G35" s="7"/>
-      <c r="H35" s="98" t="s">
+      <c r="H35" s="102" t="s">
         <v>25</v>
       </c>
       <c r="I35" s="7"/>
@@ -5159,13 +5161,13 @@
         <v>81</v>
       </c>
       <c r="K35" s="7"/>
-      <c r="L35" s="98" t="s">
+      <c r="L35" s="102" t="s">
         <v>14</v>
       </c>
       <c r="M35" s="7"/>
       <c r="N35" s="35"/>
       <c r="O35" s="7"/>
-      <c r="P35" s="99"/>
+      <c r="P35" s="103"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="81" t="str">
         <f>D11</f>
@@ -5186,7 +5188,7 @@
       <c r="E36" s="7"/>
       <c r="F36" s="35"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="100"/>
+      <c r="H36" s="104"/>
       <c r="I36" s="24">
         <f>IF(H35=Master!H31,6,0)</f>
         <v>6</v>
@@ -5198,7 +5200,7 @@
         <f>IF(L35=Master!L31,6,0)</f>
         <v>6</v>
       </c>
-      <c r="L36" s="100"/>
+      <c r="L36" s="104"/>
       <c r="M36" s="7"/>
       <c r="N36" s="35"/>
       <c r="O36" s="7"/>
@@ -5219,7 +5221,7 @@
         <v>Italy</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="101" t="s">
+      <c r="D37" s="105" t="s">
         <v>139</v>
       </c>
       <c r="E37" s="7"/>
@@ -5227,17 +5229,17 @@
         <v>78</v>
       </c>
       <c r="G37" s="7"/>
-      <c r="H37" s="99"/>
+      <c r="H37" s="103"/>
       <c r="I37" s="7"/>
       <c r="J37" s="35"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="99"/>
+      <c r="L37" s="103"/>
       <c r="M37" s="7"/>
       <c r="N37" s="35" t="s">
         <v>80</v>
       </c>
       <c r="O37" s="7"/>
-      <c r="P37" s="98" t="s">
+      <c r="P37" s="102" t="s">
         <v>14</v>
       </c>
       <c r="Q37" s="7"/>
@@ -5259,12 +5261,12 @@
         <v>Canada</v>
       </c>
       <c r="C38" s="7"/>
-      <c r="D38" s="102"/>
+      <c r="D38" s="106"/>
       <c r="E38" s="23">
         <f>IF(D37=Master!D33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F38" s="95" t="s">
+      <c r="F38" s="99" t="s">
         <v>12</v>
       </c>
       <c r="G38" s="23">
@@ -5283,14 +5285,14 @@
         <f>IF(N38=Master!N34,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N38" s="98" t="s">
+      <c r="N38" s="102" t="s">
         <v>14</v>
       </c>
       <c r="O38" s="23">
         <f>IF(P37=Master!P33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P38" s="99"/>
+      <c r="P38" s="103"/>
       <c r="Q38" s="7"/>
       <c r="R38" s="81" t="str">
         <f>D18</f>
@@ -5309,7 +5311,7 @@
         <v>72</v>
       </c>
       <c r="E39" s="7"/>
-      <c r="F39" s="96"/>
+      <c r="F39" s="100"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
@@ -5317,7 +5319,7 @@
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
-      <c r="N39" s="100"/>
+      <c r="N39" s="104"/>
       <c r="O39" s="7"/>
       <c r="P39" s="35" t="s">
         <v>76</v>
@@ -5336,14 +5338,14 @@
         <v>Brasil</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="98" t="s">
+      <c r="D40" s="102" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="23">
         <f>IF(D40=Master!D36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F40" s="97"/>
+      <c r="F40" s="101"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
@@ -5351,12 +5353,12 @@
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
-      <c r="N40" s="99"/>
+      <c r="N40" s="103"/>
       <c r="O40" s="23">
         <f>IF(P40=Master!P36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P40" s="98" t="s">
+      <c r="P40" s="102" t="s">
         <v>137</v>
       </c>
       <c r="Q40" s="7"/>
@@ -5378,7 +5380,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="99"/>
+      <c r="D41" s="103"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -5390,7 +5392,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="99"/>
+      <c r="P41" s="103"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="81" t="str">
         <f>D25</f>
@@ -5458,14 +5460,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="P34:P35"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="L35:L37"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="P37:P38"/>
-    <mergeCell ref="F38:F40"/>
-    <mergeCell ref="N38:N40"/>
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="J8:N8"/>
@@ -5482,6 +5476,14 @@
     <mergeCell ref="P31:P32"/>
     <mergeCell ref="F32:F34"/>
     <mergeCell ref="N32:N34"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="P34:P35"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="L35:L37"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="P37:P38"/>
+    <mergeCell ref="F38:F40"/>
+    <mergeCell ref="N38:N40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -5521,26 +5523,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="86" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="91"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="88"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="89" t="s">
+      <c r="J1" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="90"/>
-      <c r="L1" s="90"/>
-      <c r="M1" s="90"/>
-      <c r="N1" s="91"/>
-      <c r="P1" s="89" t="s">
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="88"/>
+      <c r="P1" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="90"/>
-      <c r="R1" s="91"/>
+      <c r="Q1" s="87"/>
+      <c r="R1" s="88"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -5743,23 +5745,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="103" t="s">
+      <c r="B8" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="104"/>
-      <c r="D8" s="104"/>
-      <c r="E8" s="104"/>
-      <c r="F8" s="105"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="96"/>
+      <c r="E8" s="96"/>
+      <c r="F8" s="97"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="103" t="s">
+      <c r="J8" s="95" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="104"/>
-      <c r="L8" s="104"/>
-      <c r="M8" s="104"/>
-      <c r="N8" s="105"/>
+      <c r="K8" s="96"/>
+      <c r="L8" s="96"/>
+      <c r="M8" s="96"/>
+      <c r="N8" s="97"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -5949,23 +5951,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="103" t="s">
+      <c r="B15" s="95" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="104"/>
-      <c r="D15" s="104"/>
-      <c r="E15" s="104"/>
-      <c r="F15" s="105"/>
+      <c r="C15" s="96"/>
+      <c r="D15" s="96"/>
+      <c r="E15" s="96"/>
+      <c r="F15" s="97"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="103" t="s">
+      <c r="J15" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="104"/>
-      <c r="L15" s="104"/>
-      <c r="M15" s="104"/>
-      <c r="N15" s="105"/>
+      <c r="K15" s="96"/>
+      <c r="L15" s="96"/>
+      <c r="M15" s="96"/>
+      <c r="N15" s="97"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -6130,23 +6132,23 @@
       <c r="N21" s="52"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="103" t="s">
+      <c r="B22" s="95" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="104"/>
-      <c r="D22" s="104"/>
-      <c r="E22" s="104"/>
-      <c r="F22" s="105"/>
+      <c r="C22" s="96"/>
+      <c r="D22" s="96"/>
+      <c r="E22" s="96"/>
+      <c r="F22" s="97"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="103" t="s">
+      <c r="J22" s="95" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="104"/>
-      <c r="L22" s="104"/>
-      <c r="M22" s="104"/>
-      <c r="N22" s="105"/>
+      <c r="K22" s="96"/>
+      <c r="L22" s="96"/>
+      <c r="M22" s="96"/>
+      <c r="N22" s="97"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B23" s="56" t="s">
@@ -6385,7 +6387,7 @@
         <v>79</v>
       </c>
       <c r="O31" s="7"/>
-      <c r="P31" s="98" t="s">
+      <c r="P31" s="102" t="s">
         <v>41</v>
       </c>
       <c r="Q31" s="7"/>
@@ -6429,7 +6431,7 @@
         <f>IF(P31=Master!P27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P32" s="99"/>
+      <c r="P32" s="103"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="39" t="str">
         <f>D4</f>
@@ -6475,7 +6477,7 @@
         <v>Argentina</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="98" t="s">
+      <c r="D34" s="102" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="23">
@@ -6505,7 +6507,7 @@
         <f>IF(P34=Master!P30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P34" s="98" t="s">
+      <c r="P34" s="102" t="s">
         <v>34</v>
       </c>
       <c r="Q34" s="7"/>
@@ -6527,7 +6529,7 @@
         <v>France</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="99"/>
+      <c r="D35" s="103"/>
       <c r="E35" s="7"/>
       <c r="F35" s="35"/>
       <c r="G35" s="7"/>
@@ -6545,7 +6547,7 @@
       <c r="M35" s="7"/>
       <c r="N35" s="35"/>
       <c r="O35" s="7"/>
-      <c r="P35" s="99"/>
+      <c r="P35" s="103"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="39" t="str">
         <f>D11</f>
@@ -6599,7 +6601,7 @@
         <v>Italy</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="101" t="s">
+      <c r="D37" s="105" t="s">
         <v>139</v>
       </c>
       <c r="E37" s="7"/>
@@ -6639,7 +6641,7 @@
         <v>Canada</v>
       </c>
       <c r="C38" s="7"/>
-      <c r="D38" s="102"/>
+      <c r="D38" s="106"/>
       <c r="E38" s="23">
         <f>IF(D37=Master!D33,2,0)</f>
         <v>2</v>
@@ -6716,7 +6718,7 @@
         <v>Brasil</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="98" t="s">
+      <c r="D40" s="102" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="23">
@@ -6736,7 +6738,7 @@
         <f>IF(P40=Master!P36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P40" s="98" t="s">
+      <c r="P40" s="102" t="s">
         <v>137</v>
       </c>
       <c r="Q40" s="7"/>
@@ -6758,7 +6760,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="99"/>
+      <c r="D41" s="103"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -6770,7 +6772,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="99"/>
+      <c r="P41" s="103"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="39" t="str">
         <f>D25</f>
@@ -6838,6 +6840,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="J8:N8"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="D31:D32"/>
@@ -6854,13 +6863,6 @@
     <mergeCell ref="N38:N40"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="P40:P41"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="J8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -6900,26 +6902,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="86" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="91"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="88"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="89" t="s">
+      <c r="J1" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="90"/>
-      <c r="L1" s="90"/>
-      <c r="M1" s="90"/>
-      <c r="N1" s="91"/>
-      <c r="P1" s="89" t="s">
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="88"/>
+      <c r="P1" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="90"/>
-      <c r="R1" s="91"/>
+      <c r="Q1" s="87"/>
+      <c r="R1" s="88"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -7122,23 +7124,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="103" t="s">
+      <c r="B8" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="104"/>
-      <c r="D8" s="104"/>
-      <c r="E8" s="104"/>
-      <c r="F8" s="105"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="96"/>
+      <c r="E8" s="96"/>
+      <c r="F8" s="97"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="103" t="s">
+      <c r="J8" s="95" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="104"/>
-      <c r="L8" s="104"/>
-      <c r="M8" s="104"/>
-      <c r="N8" s="105"/>
+      <c r="K8" s="96"/>
+      <c r="L8" s="96"/>
+      <c r="M8" s="96"/>
+      <c r="N8" s="97"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -7328,23 +7330,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="103" t="s">
+      <c r="B15" s="95" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="104"/>
-      <c r="D15" s="104"/>
-      <c r="E15" s="104"/>
-      <c r="F15" s="105"/>
+      <c r="C15" s="96"/>
+      <c r="D15" s="96"/>
+      <c r="E15" s="96"/>
+      <c r="F15" s="97"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="103" t="s">
+      <c r="J15" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="104"/>
-      <c r="L15" s="104"/>
-      <c r="M15" s="104"/>
-      <c r="N15" s="105"/>
+      <c r="K15" s="96"/>
+      <c r="L15" s="96"/>
+      <c r="M15" s="96"/>
+      <c r="N15" s="97"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -7511,23 +7513,23 @@
       <c r="N21" s="52"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="103" t="s">
+      <c r="B22" s="95" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="104"/>
-      <c r="D22" s="104"/>
-      <c r="E22" s="104"/>
-      <c r="F22" s="105"/>
+      <c r="C22" s="96"/>
+      <c r="D22" s="96"/>
+      <c r="E22" s="96"/>
+      <c r="F22" s="97"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="103" t="s">
+      <c r="J22" s="95" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="104"/>
-      <c r="L22" s="104"/>
-      <c r="M22" s="104"/>
-      <c r="N22" s="105"/>
+      <c r="K22" s="96"/>
+      <c r="L22" s="96"/>
+      <c r="M22" s="96"/>
+      <c r="N22" s="97"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B23" s="56" t="s">
@@ -8099,7 +8101,7 @@
         <v>Brasil</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="98" t="s">
+      <c r="D40" s="102" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="23">
@@ -8141,7 +8143,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="99"/>
+      <c r="D41" s="103"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -8221,6 +8223,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="J8:N8"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="D31:D32"/>
@@ -8237,13 +8246,6 @@
     <mergeCell ref="N38:N40"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="P40:P41"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="J8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -8283,26 +8285,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="86" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="91"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="88"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="89" t="s">
+      <c r="J1" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="90"/>
-      <c r="L1" s="90"/>
-      <c r="M1" s="90"/>
-      <c r="N1" s="91"/>
-      <c r="P1" s="89" t="s">
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="88"/>
+      <c r="P1" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="90"/>
-      <c r="R1" s="91"/>
+      <c r="Q1" s="87"/>
+      <c r="R1" s="88"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -8505,23 +8507,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="103" t="s">
+      <c r="B8" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="104"/>
-      <c r="D8" s="104"/>
-      <c r="E8" s="104"/>
-      <c r="F8" s="105"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="96"/>
+      <c r="E8" s="96"/>
+      <c r="F8" s="97"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="103" t="s">
+      <c r="J8" s="95" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="104"/>
-      <c r="L8" s="104"/>
-      <c r="M8" s="104"/>
-      <c r="N8" s="105"/>
+      <c r="K8" s="96"/>
+      <c r="L8" s="96"/>
+      <c r="M8" s="96"/>
+      <c r="N8" s="97"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -8711,23 +8713,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="103" t="s">
+      <c r="B15" s="95" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="104"/>
-      <c r="D15" s="104"/>
-      <c r="E15" s="104"/>
-      <c r="F15" s="105"/>
+      <c r="C15" s="96"/>
+      <c r="D15" s="96"/>
+      <c r="E15" s="96"/>
+      <c r="F15" s="97"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="103" t="s">
+      <c r="J15" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="104"/>
-      <c r="L15" s="104"/>
-      <c r="M15" s="104"/>
-      <c r="N15" s="105"/>
+      <c r="K15" s="96"/>
+      <c r="L15" s="96"/>
+      <c r="M15" s="96"/>
+      <c r="N15" s="97"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -8894,23 +8896,23 @@
       <c r="N21" s="52"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="103" t="s">
+      <c r="B22" s="95" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="104"/>
-      <c r="D22" s="104"/>
-      <c r="E22" s="104"/>
-      <c r="F22" s="105"/>
+      <c r="C22" s="96"/>
+      <c r="D22" s="96"/>
+      <c r="E22" s="96"/>
+      <c r="F22" s="97"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="103" t="s">
+      <c r="J22" s="95" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="104"/>
-      <c r="L22" s="104"/>
-      <c r="M22" s="104"/>
-      <c r="N22" s="105"/>
+      <c r="K22" s="96"/>
+      <c r="L22" s="96"/>
+      <c r="M22" s="96"/>
+      <c r="N22" s="97"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B23" s="56" t="s">
@@ -9602,6 +9604,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="J8:N8"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="D31:D32"/>
@@ -9618,13 +9627,6 @@
     <mergeCell ref="N38:N40"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="P40:P41"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="J8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -9742,26 +9744,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="86" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="91"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="88"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="89" t="s">
+      <c r="J1" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="90"/>
-      <c r="L1" s="90"/>
-      <c r="M1" s="90"/>
-      <c r="N1" s="91"/>
-      <c r="P1" s="89" t="s">
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="88"/>
+      <c r="P1" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="90"/>
-      <c r="R1" s="91"/>
+      <c r="Q1" s="87"/>
+      <c r="R1" s="88"/>
       <c r="W1" s="1" t="s">
         <v>92</v>
       </c>
@@ -10069,23 +10071,23 @@
       </c>
     </row>
     <row r="8" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B8" s="103" t="s">
+      <c r="B8" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="104"/>
-      <c r="D8" s="104"/>
-      <c r="E8" s="104"/>
-      <c r="F8" s="105"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="96"/>
+      <c r="E8" s="96"/>
+      <c r="F8" s="97"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="103" t="s">
+      <c r="J8" s="95" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="104"/>
-      <c r="L8" s="104"/>
-      <c r="M8" s="104"/>
-      <c r="N8" s="105"/>
+      <c r="K8" s="96"/>
+      <c r="L8" s="96"/>
+      <c r="M8" s="96"/>
+      <c r="N8" s="97"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -10373,23 +10375,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B15" s="103" t="s">
+      <c r="B15" s="95" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="104"/>
-      <c r="D15" s="104"/>
-      <c r="E15" s="104"/>
-      <c r="F15" s="105"/>
+      <c r="C15" s="96"/>
+      <c r="D15" s="96"/>
+      <c r="E15" s="96"/>
+      <c r="F15" s="97"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="103" t="s">
+      <c r="J15" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="104"/>
-      <c r="L15" s="104"/>
-      <c r="M15" s="104"/>
-      <c r="N15" s="105"/>
+      <c r="K15" s="96"/>
+      <c r="L15" s="96"/>
+      <c r="M15" s="96"/>
+      <c r="N15" s="97"/>
     </row>
     <row r="16" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -10654,23 +10656,23 @@
       <c r="N21" s="52"/>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B22" s="103" t="s">
+      <c r="B22" s="95" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="104"/>
-      <c r="D22" s="104"/>
-      <c r="E22" s="104"/>
-      <c r="F22" s="105"/>
+      <c r="C22" s="96"/>
+      <c r="D22" s="96"/>
+      <c r="E22" s="96"/>
+      <c r="F22" s="97"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="103" t="s">
+      <c r="J22" s="95" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="104"/>
-      <c r="L22" s="104"/>
-      <c r="M22" s="104"/>
-      <c r="N22" s="105"/>
+      <c r="K22" s="96"/>
+      <c r="L22" s="96"/>
+      <c r="M22" s="96"/>
+      <c r="N22" s="97"/>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B23" s="56" t="s">
@@ -11444,13 +11446,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="J8:N8"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="D31:D32"/>
@@ -11467,6 +11462,13 @@
     <mergeCell ref="N38:N40"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="P40:P41"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="J8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
team admin page complete
</commit_message>
<xml_diff>
--- a/excel docs/java testing-audit info.xlsx
+++ b/excel docs/java testing-audit info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10520"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joecollins/Desktop/documents/personal-projects/world-cup-heroku/excel docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40343C96-0BED-0A42-B823-547F0FB007CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D270751-C433-1443-991E-22317482CB1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="149">
   <si>
     <t>A1</t>
   </si>
@@ -654,6 +654,9 @@
   </si>
   <si>
     <t>Points obtained in the group matches between teams concerned.</t>
+  </si>
+  <si>
+    <t>Wales</t>
   </si>
 </sst>
 </file>
@@ -1218,7 +1221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1469,6 +1472,15 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1479,15 +1491,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1496,6 +1499,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1508,30 +1535,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1603,6 +1606,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1887,7 +1893,7 @@
   <dimension ref="A1:T38"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1922,11 +1928,11 @@
       <c r="F1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="86" t="s">
+      <c r="J1" s="89" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="87"/>
-      <c r="L1" s="88"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="91"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B2" s="14" t="s">
@@ -1969,8 +1975,8 @@
         <v>133</v>
       </c>
       <c r="D4" s="7"/>
-      <c r="F4" s="83" t="s">
-        <v>49</v>
+      <c r="F4" s="131" t="s">
+        <v>138</v>
       </c>
       <c r="H4" s="7"/>
       <c r="J4" s="16" t="s">
@@ -1988,7 +1994,7 @@
       </c>
       <c r="D5" s="7"/>
       <c r="F5" s="15" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="H5" s="7"/>
       <c r="J5" s="16" t="s">
@@ -2246,7 +2252,7 @@
         <v>Ecuador</v>
       </c>
       <c r="C27" s="7"/>
-      <c r="D27" s="89" t="s">
+      <c r="D27" s="86" t="s">
         <v>134</v>
       </c>
       <c r="E27" s="7"/>
@@ -2260,7 +2266,7 @@
       <c r="M27" s="7"/>
       <c r="N27" s="7"/>
       <c r="O27" s="7"/>
-      <c r="P27" s="89" t="s">
+      <c r="P27" s="86" t="s">
         <v>41</v>
       </c>
       <c r="Q27" s="7"/>
@@ -2282,9 +2288,9 @@
         <v>Iran</v>
       </c>
       <c r="C28" s="7"/>
-      <c r="D28" s="90"/>
+      <c r="D28" s="88"/>
       <c r="E28" s="7"/>
-      <c r="F28" s="89" t="s">
+      <c r="F28" s="86" t="s">
         <v>25</v>
       </c>
       <c r="G28" s="7"/>
@@ -2294,11 +2300,11 @@
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
       <c r="M28" s="7"/>
-      <c r="N28" s="89" t="s">
+      <c r="N28" s="86" t="s">
         <v>34</v>
       </c>
       <c r="O28" s="7"/>
-      <c r="P28" s="90"/>
+      <c r="P28" s="88"/>
       <c r="Q28" s="7"/>
       <c r="R28" s="15" t="str">
         <f>B3</f>
@@ -2315,7 +2321,7 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
-      <c r="F29" s="91"/>
+      <c r="F29" s="87"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
@@ -2323,7 +2329,7 @@
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
-      <c r="N29" s="91"/>
+      <c r="N29" s="87"/>
       <c r="O29" s="7"/>
       <c r="P29" s="7"/>
       <c r="Q29" s="7"/>
@@ -2340,11 +2346,11 @@
         <v>Argentina</v>
       </c>
       <c r="C30" s="7"/>
-      <c r="D30" s="89" t="s">
+      <c r="D30" s="86" t="s">
         <v>25</v>
       </c>
       <c r="E30" s="7"/>
-      <c r="F30" s="90"/>
+      <c r="F30" s="88"/>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
@@ -2352,9 +2358,9 @@
       <c r="K30" s="7"/>
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
-      <c r="N30" s="90"/>
+      <c r="N30" s="88"/>
       <c r="O30" s="7"/>
-      <c r="P30" s="89" t="s">
+      <c r="P30" s="86" t="s">
         <v>34</v>
       </c>
       <c r="Q30" s="7"/>
@@ -2376,7 +2382,7 @@
         <v>France</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="90"/>
+      <c r="D31" s="88"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
@@ -2392,7 +2398,7 @@
       <c r="M31" s="7"/>
       <c r="N31" s="7"/>
       <c r="O31" s="7"/>
-      <c r="P31" s="90"/>
+      <c r="P31" s="88"/>
       <c r="Q31" s="7"/>
       <c r="R31" s="15" t="str">
         <f>B9</f>
@@ -2436,7 +2442,7 @@
         <v>Italy</v>
       </c>
       <c r="C33" s="7"/>
-      <c r="D33" s="89" t="s">
+      <c r="D33" s="86" t="s">
         <v>139</v>
       </c>
       <c r="E33" s="7"/>
@@ -2450,7 +2456,7 @@
       <c r="M33" s="7"/>
       <c r="N33" s="7"/>
       <c r="O33" s="7"/>
-      <c r="P33" s="89" t="s">
+      <c r="P33" s="86" t="s">
         <v>14</v>
       </c>
       <c r="Q33" s="7"/>
@@ -2472,9 +2478,9 @@
         <v>Canada</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="90"/>
+      <c r="D34" s="88"/>
       <c r="E34" s="7"/>
-      <c r="F34" s="89" t="s">
+      <c r="F34" s="86" t="s">
         <v>12</v>
       </c>
       <c r="G34" s="7"/>
@@ -2484,11 +2490,11 @@
       <c r="K34" s="7"/>
       <c r="L34" s="7"/>
       <c r="M34" s="7"/>
-      <c r="N34" s="89" t="s">
+      <c r="N34" s="86" t="s">
         <v>14</v>
       </c>
       <c r="O34" s="7"/>
-      <c r="P34" s="90"/>
+      <c r="P34" s="88"/>
       <c r="Q34" s="7"/>
       <c r="R34" s="15" t="str">
         <f>B15</f>
@@ -2505,7 +2511,7 @@
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
-      <c r="F35" s="91"/>
+      <c r="F35" s="87"/>
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
@@ -2513,7 +2519,7 @@
       <c r="K35" s="7"/>
       <c r="L35" s="7"/>
       <c r="M35" s="7"/>
-      <c r="N35" s="91"/>
+      <c r="N35" s="87"/>
       <c r="O35" s="7"/>
       <c r="P35" s="7"/>
       <c r="Q35" s="7"/>
@@ -2530,11 +2536,11 @@
         <v>Brasil</v>
       </c>
       <c r="C36" s="7"/>
-      <c r="D36" s="89" t="s">
+      <c r="D36" s="86" t="s">
         <v>12</v>
       </c>
       <c r="E36" s="7"/>
-      <c r="F36" s="90"/>
+      <c r="F36" s="88"/>
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
       <c r="I36" s="7"/>
@@ -2542,9 +2548,9 @@
       <c r="K36" s="7"/>
       <c r="L36" s="7"/>
       <c r="M36" s="7"/>
-      <c r="N36" s="90"/>
+      <c r="N36" s="88"/>
       <c r="O36" s="7"/>
-      <c r="P36" s="89" t="s">
+      <c r="P36" s="86" t="s">
         <v>137</v>
       </c>
       <c r="Q36" s="7"/>
@@ -2566,7 +2572,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="90"/>
+      <c r="D37" s="88"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
@@ -2578,7 +2584,7 @@
       <c r="M37" s="7"/>
       <c r="N37" s="7"/>
       <c r="O37" s="7"/>
-      <c r="P37" s="90"/>
+      <c r="P37" s="88"/>
       <c r="Q37" s="7"/>
       <c r="R37" s="15" t="str">
         <f>B21</f>
@@ -2613,12 +2619,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="N28:N30"/>
-    <mergeCell ref="N34:N36"/>
-    <mergeCell ref="P27:P28"/>
-    <mergeCell ref="P30:P31"/>
-    <mergeCell ref="P33:P34"/>
-    <mergeCell ref="P36:P37"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="D27:D28"/>
     <mergeCell ref="D30:D31"/>
@@ -2628,6 +2628,12 @@
     <mergeCell ref="F34:F36"/>
     <mergeCell ref="H31:H33"/>
     <mergeCell ref="L31:L33"/>
+    <mergeCell ref="N28:N30"/>
+    <mergeCell ref="N34:N36"/>
+    <mergeCell ref="P27:P28"/>
+    <mergeCell ref="P30:P31"/>
+    <mergeCell ref="P33:P34"/>
+    <mergeCell ref="P36:P37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -2682,8 +2688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86316F4E-9A6C-492E-9EDB-018A26A821E8}">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2714,26 +2720,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="88"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="91"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="86" t="s">
+      <c r="J1" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="88"/>
-      <c r="P1" s="86" t="s">
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="91"/>
+      <c r="P1" s="89" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="88"/>
+      <c r="Q1" s="90"/>
+      <c r="R1" s="91"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -2854,12 +2860,12 @@
       <c r="H5" s="35"/>
       <c r="I5" s="52"/>
       <c r="J5" s="26" t="s">
-        <v>49</v>
+        <v>138</v>
       </c>
       <c r="K5" s="51"/>
       <c r="L5" s="50" t="str">
         <f>Master!F4</f>
-        <v>Sweden</v>
+        <v>USA</v>
       </c>
       <c r="M5" s="51"/>
       <c r="N5" s="34">
@@ -2893,12 +2899,12 @@
       <c r="H6" s="35"/>
       <c r="I6" s="52"/>
       <c r="J6" s="27" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="K6" s="53"/>
       <c r="L6" s="60" t="str">
         <f>Master!F5</f>
-        <v>USA</v>
+        <v>Wales</v>
       </c>
       <c r="M6" s="53"/>
       <c r="N6" s="54">
@@ -2936,23 +2942,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="95" t="s">
+      <c r="B8" s="103" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="96"/>
-      <c r="D8" s="96"/>
-      <c r="E8" s="96"/>
-      <c r="F8" s="97"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="104"/>
+      <c r="E8" s="104"/>
+      <c r="F8" s="105"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="95" t="s">
+      <c r="J8" s="103" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="96"/>
-      <c r="L8" s="96"/>
-      <c r="M8" s="96"/>
-      <c r="N8" s="97"/>
+      <c r="K8" s="104"/>
+      <c r="L8" s="104"/>
+      <c r="M8" s="104"/>
+      <c r="N8" s="105"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -3142,23 +3148,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="95" t="s">
+      <c r="B15" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="96"/>
-      <c r="D15" s="96"/>
-      <c r="E15" s="96"/>
-      <c r="F15" s="97"/>
+      <c r="C15" s="104"/>
+      <c r="D15" s="104"/>
+      <c r="E15" s="104"/>
+      <c r="F15" s="105"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="95" t="s">
+      <c r="J15" s="103" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="96"/>
-      <c r="L15" s="96"/>
-      <c r="M15" s="96"/>
-      <c r="N15" s="97"/>
+      <c r="K15" s="104"/>
+      <c r="L15" s="104"/>
+      <c r="M15" s="104"/>
+      <c r="N15" s="105"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -3279,10 +3285,10 @@
         <f t="shared" ref="N19:N20" si="5">IF(J19=L19,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Q19" s="98" t="s">
+      <c r="Q19" s="106" t="s">
         <v>82</v>
       </c>
-      <c r="R19" s="98"/>
+      <c r="R19" s="106"/>
     </row>
     <row r="20" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="27" t="s">
@@ -3337,23 +3343,23 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="95" t="s">
+      <c r="B22" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="96"/>
-      <c r="D22" s="96"/>
-      <c r="E22" s="96"/>
-      <c r="F22" s="97"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="105"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="95" t="s">
+      <c r="J22" s="103" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="96"/>
-      <c r="L22" s="96"/>
-      <c r="M22" s="96"/>
-      <c r="N22" s="97"/>
+      <c r="K22" s="104"/>
+      <c r="L22" s="104"/>
+      <c r="M22" s="104"/>
+      <c r="N22" s="105"/>
       <c r="Q22" s="49"/>
       <c r="R22" s="32" t="s">
         <v>85</v>
@@ -3584,7 +3590,7 @@
         <v>Ecuador</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="102" t="s">
+      <c r="D31" s="98" t="s">
         <v>134</v>
       </c>
       <c r="E31" s="7"/>
@@ -3602,7 +3608,7 @@
         <v>79</v>
       </c>
       <c r="O31" s="7"/>
-      <c r="P31" s="102" t="s">
+      <c r="P31" s="98" t="s">
         <v>41</v>
       </c>
       <c r="Q31" s="7"/>
@@ -3624,12 +3630,12 @@
         <v>Iran</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="103"/>
+      <c r="D32" s="99"/>
       <c r="E32" s="23">
         <f>IF(D31=Master!D27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F32" s="102" t="s">
+      <c r="F32" s="98" t="s">
         <v>25</v>
       </c>
       <c r="G32" s="7"/>
@@ -3639,14 +3645,14 @@
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
-      <c r="N32" s="102" t="s">
+      <c r="N32" s="98" t="s">
         <v>34</v>
       </c>
       <c r="O32" s="23">
         <f>IF(P31=Master!P27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P32" s="103"/>
+      <c r="P32" s="99"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="39" t="str">
         <f>D4</f>
@@ -3665,7 +3671,7 @@
         <v>70</v>
       </c>
       <c r="E33" s="7"/>
-      <c r="F33" s="104"/>
+      <c r="F33" s="100"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
@@ -3673,7 +3679,7 @@
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
-      <c r="N33" s="104"/>
+      <c r="N33" s="100"/>
       <c r="O33" s="7"/>
       <c r="P33" s="35" t="s">
         <v>74</v>
@@ -3692,14 +3698,14 @@
         <v>Argentina</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="102" t="s">
+      <c r="D34" s="98" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="23">
         <f>IF(D34=Master!D30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F34" s="103"/>
+      <c r="F34" s="99"/>
       <c r="G34" s="23">
         <f>IF(F32=Master!F28,4,0)</f>
         <v>4</v>
@@ -3717,12 +3723,12 @@
         <f>IF(N32=Master!N28,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N34" s="103"/>
+      <c r="N34" s="99"/>
       <c r="O34" s="23">
         <f>IF(P34=Master!P30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P34" s="102" t="s">
+      <c r="P34" s="98" t="s">
         <v>34</v>
       </c>
       <c r="Q34" s="7"/>
@@ -3744,11 +3750,11 @@
         <v>France</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="103"/>
+      <c r="D35" s="99"/>
       <c r="E35" s="7"/>
       <c r="F35" s="35"/>
       <c r="G35" s="7"/>
-      <c r="H35" s="102" t="s">
+      <c r="H35" s="98" t="s">
         <v>25</v>
       </c>
       <c r="I35" s="7"/>
@@ -3756,13 +3762,13 @@
         <v>81</v>
       </c>
       <c r="K35" s="7"/>
-      <c r="L35" s="102" t="s">
+      <c r="L35" s="98" t="s">
         <v>14</v>
       </c>
       <c r="M35" s="7"/>
       <c r="N35" s="35"/>
       <c r="O35" s="7"/>
-      <c r="P35" s="103"/>
+      <c r="P35" s="99"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="39" t="str">
         <f>D11</f>
@@ -3783,7 +3789,7 @@
       <c r="E36" s="7"/>
       <c r="F36" s="35"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="104"/>
+      <c r="H36" s="100"/>
       <c r="I36" s="24">
         <f>IF(H35=Master!H31,6,0)</f>
         <v>6</v>
@@ -3795,7 +3801,7 @@
         <f>IF(L35=Master!L31,6,0)</f>
         <v>6</v>
       </c>
-      <c r="L36" s="104"/>
+      <c r="L36" s="100"/>
       <c r="M36" s="7"/>
       <c r="N36" s="35"/>
       <c r="O36" s="7"/>
@@ -3816,7 +3822,7 @@
         <v>Italy</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="105" t="s">
+      <c r="D37" s="101" t="s">
         <v>139</v>
       </c>
       <c r="E37" s="7"/>
@@ -3824,17 +3830,17 @@
         <v>78</v>
       </c>
       <c r="G37" s="7"/>
-      <c r="H37" s="103"/>
+      <c r="H37" s="99"/>
       <c r="I37" s="7"/>
       <c r="J37" s="35"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="103"/>
+      <c r="L37" s="99"/>
       <c r="M37" s="7"/>
       <c r="N37" s="35" t="s">
         <v>80</v>
       </c>
       <c r="O37" s="7"/>
-      <c r="P37" s="102" t="s">
+      <c r="P37" s="98" t="s">
         <v>14</v>
       </c>
       <c r="Q37" s="7"/>
@@ -3856,12 +3862,12 @@
         <v>Canada</v>
       </c>
       <c r="C38" s="7"/>
-      <c r="D38" s="106"/>
+      <c r="D38" s="102"/>
       <c r="E38" s="23">
         <f>IF(D37=Master!D33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F38" s="99" t="s">
+      <c r="F38" s="95" t="s">
         <v>12</v>
       </c>
       <c r="G38" s="23">
@@ -3880,14 +3886,14 @@
         <f>IF(N38=Master!N34,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N38" s="102" t="s">
+      <c r="N38" s="98" t="s">
         <v>14</v>
       </c>
       <c r="O38" s="23">
         <f>IF(P37=Master!P33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P38" s="103"/>
+      <c r="P38" s="99"/>
       <c r="Q38" s="7"/>
       <c r="R38" s="39" t="str">
         <f>D18</f>
@@ -3906,7 +3912,7 @@
         <v>72</v>
       </c>
       <c r="E39" s="7"/>
-      <c r="F39" s="100"/>
+      <c r="F39" s="96"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
@@ -3914,7 +3920,7 @@
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
-      <c r="N39" s="104"/>
+      <c r="N39" s="100"/>
       <c r="O39" s="7"/>
       <c r="P39" s="35" t="s">
         <v>76</v>
@@ -3933,14 +3939,14 @@
         <v>Brasil</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="102" t="s">
+      <c r="D40" s="98" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="23">
         <f>IF(D40=Master!D36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F40" s="101"/>
+      <c r="F40" s="97"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
@@ -3948,12 +3954,12 @@
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
-      <c r="N40" s="103"/>
+      <c r="N40" s="99"/>
       <c r="O40" s="23">
         <f>IF(P40=Master!P36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P40" s="102" t="s">
+      <c r="P40" s="98" t="s">
         <v>137</v>
       </c>
       <c r="Q40" s="7"/>
@@ -3975,7 +3981,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="103"/>
+      <c r="D41" s="99"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -3987,7 +3993,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="103"/>
+      <c r="P41" s="99"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="39" t="str">
         <f>D25</f>
@@ -4055,6 +4061,16 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J22:N22"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="Q19:R19"/>
     <mergeCell ref="F38:F40"/>
     <mergeCell ref="P37:P38"/>
     <mergeCell ref="P40:P41"/>
@@ -4069,16 +4085,6 @@
     <mergeCell ref="D37:D38"/>
     <mergeCell ref="H35:H37"/>
     <mergeCell ref="L35:L37"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J22:N22"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="J8:N8"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="Q19:R19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -4090,7 +4096,7 @@
   <dimension ref="A1:T43"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4121,26 +4127,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="88"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="91"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="86" t="s">
+      <c r="J1" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="88"/>
-      <c r="P1" s="86" t="s">
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="91"/>
+      <c r="P1" s="89" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="88"/>
+      <c r="Q1" s="90"/>
+      <c r="R1" s="91"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -4261,12 +4267,12 @@
       <c r="H5" s="35"/>
       <c r="I5" s="52"/>
       <c r="J5" s="26" t="s">
-        <v>49</v>
+        <v>138</v>
       </c>
       <c r="K5" s="51"/>
       <c r="L5" s="50" t="str">
         <f>Master!F4</f>
-        <v>Sweden</v>
+        <v>USA</v>
       </c>
       <c r="M5" s="51"/>
       <c r="N5" s="34">
@@ -4300,12 +4306,12 @@
       <c r="H6" s="35"/>
       <c r="I6" s="52"/>
       <c r="J6" s="27" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="K6" s="53"/>
       <c r="L6" s="60" t="str">
         <f>Master!F5</f>
-        <v>USA</v>
+        <v>Wales</v>
       </c>
       <c r="M6" s="53"/>
       <c r="N6" s="54">
@@ -4343,23 +4349,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="95" t="s">
+      <c r="B8" s="103" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="96"/>
-      <c r="D8" s="96"/>
-      <c r="E8" s="96"/>
-      <c r="F8" s="97"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="104"/>
+      <c r="E8" s="104"/>
+      <c r="F8" s="105"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="95" t="s">
+      <c r="J8" s="103" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="96"/>
-      <c r="L8" s="96"/>
-      <c r="M8" s="96"/>
-      <c r="N8" s="97"/>
+      <c r="K8" s="104"/>
+      <c r="L8" s="104"/>
+      <c r="M8" s="104"/>
+      <c r="N8" s="105"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -4549,23 +4555,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="95" t="s">
+      <c r="B15" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="96"/>
-      <c r="D15" s="96"/>
-      <c r="E15" s="96"/>
-      <c r="F15" s="97"/>
+      <c r="C15" s="104"/>
+      <c r="D15" s="104"/>
+      <c r="E15" s="104"/>
+      <c r="F15" s="105"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="95" t="s">
+      <c r="J15" s="103" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="96"/>
-      <c r="L15" s="96"/>
-      <c r="M15" s="96"/>
-      <c r="N15" s="97"/>
+      <c r="K15" s="104"/>
+      <c r="L15" s="104"/>
+      <c r="M15" s="104"/>
+      <c r="N15" s="105"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -4686,10 +4692,10 @@
         <f t="shared" ref="N19:N20" si="5">IF(J19=L19,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Q19" s="98" t="s">
+      <c r="Q19" s="106" t="s">
         <v>82</v>
       </c>
-      <c r="R19" s="98"/>
+      <c r="R19" s="106"/>
     </row>
     <row r="20" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="27" t="s">
@@ -4744,23 +4750,23 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="95" t="s">
+      <c r="B22" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="96"/>
-      <c r="D22" s="96"/>
-      <c r="E22" s="96"/>
-      <c r="F22" s="97"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="105"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="95" t="s">
+      <c r="J22" s="103" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="96"/>
-      <c r="L22" s="96"/>
-      <c r="M22" s="96"/>
-      <c r="N22" s="97"/>
+      <c r="K22" s="104"/>
+      <c r="L22" s="104"/>
+      <c r="M22" s="104"/>
+      <c r="N22" s="105"/>
       <c r="Q22" s="49"/>
       <c r="R22" s="32" t="s">
         <v>85</v>
@@ -4991,7 +4997,7 @@
         <v>Ecuador</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="102" t="s">
+      <c r="D31" s="98" t="s">
         <v>134</v>
       </c>
       <c r="E31" s="7"/>
@@ -5009,7 +5015,7 @@
         <v>79</v>
       </c>
       <c r="O31" s="7"/>
-      <c r="P31" s="102" t="s">
+      <c r="P31" s="98" t="s">
         <v>41</v>
       </c>
       <c r="Q31" s="7"/>
@@ -5031,12 +5037,12 @@
         <v>Iran</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="103"/>
+      <c r="D32" s="99"/>
       <c r="E32" s="23">
         <f>IF(D31=Master!D27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F32" s="102" t="s">
+      <c r="F32" s="98" t="s">
         <v>25</v>
       </c>
       <c r="G32" s="7"/>
@@ -5046,14 +5052,14 @@
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
-      <c r="N32" s="102" t="s">
+      <c r="N32" s="98" t="s">
         <v>34</v>
       </c>
       <c r="O32" s="23">
         <f>IF(P31=Master!P27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P32" s="103"/>
+      <c r="P32" s="99"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="81" t="str">
         <f>D4</f>
@@ -5072,7 +5078,7 @@
         <v>70</v>
       </c>
       <c r="E33" s="7"/>
-      <c r="F33" s="104"/>
+      <c r="F33" s="100"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
@@ -5080,7 +5086,7 @@
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
-      <c r="N33" s="104"/>
+      <c r="N33" s="100"/>
       <c r="O33" s="7"/>
       <c r="P33" s="35"/>
       <c r="Q33" s="7"/>
@@ -5097,14 +5103,14 @@
         <v>Argentina</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="102" t="s">
+      <c r="D34" s="98" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="23">
         <f>IF(D34=Master!D30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F34" s="103"/>
+      <c r="F34" s="99"/>
       <c r="G34" s="23">
         <f>IF(F32=Master!F28,4,0)</f>
         <v>4</v>
@@ -5122,12 +5128,12 @@
         <f>IF(N32=Master!N28,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N34" s="103"/>
+      <c r="N34" s="99"/>
       <c r="O34" s="23">
         <f>IF(P34=Master!P30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P34" s="102" t="s">
+      <c r="P34" s="98" t="s">
         <v>34</v>
       </c>
       <c r="Q34" s="7"/>
@@ -5149,11 +5155,11 @@
         <v>France</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="103"/>
+      <c r="D35" s="99"/>
       <c r="E35" s="7"/>
       <c r="F35" s="35"/>
       <c r="G35" s="7"/>
-      <c r="H35" s="102" t="s">
+      <c r="H35" s="98" t="s">
         <v>25</v>
       </c>
       <c r="I35" s="7"/>
@@ -5161,13 +5167,13 @@
         <v>81</v>
       </c>
       <c r="K35" s="7"/>
-      <c r="L35" s="102" t="s">
+      <c r="L35" s="98" t="s">
         <v>14</v>
       </c>
       <c r="M35" s="7"/>
       <c r="N35" s="35"/>
       <c r="O35" s="7"/>
-      <c r="P35" s="103"/>
+      <c r="P35" s="99"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="81" t="str">
         <f>D11</f>
@@ -5188,7 +5194,7 @@
       <c r="E36" s="7"/>
       <c r="F36" s="35"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="104"/>
+      <c r="H36" s="100"/>
       <c r="I36" s="24">
         <f>IF(H35=Master!H31,6,0)</f>
         <v>6</v>
@@ -5200,7 +5206,7 @@
         <f>IF(L35=Master!L31,6,0)</f>
         <v>6</v>
       </c>
-      <c r="L36" s="104"/>
+      <c r="L36" s="100"/>
       <c r="M36" s="7"/>
       <c r="N36" s="35"/>
       <c r="O36" s="7"/>
@@ -5221,7 +5227,7 @@
         <v>Italy</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="105" t="s">
+      <c r="D37" s="101" t="s">
         <v>139</v>
       </c>
       <c r="E37" s="7"/>
@@ -5229,17 +5235,17 @@
         <v>78</v>
       </c>
       <c r="G37" s="7"/>
-      <c r="H37" s="103"/>
+      <c r="H37" s="99"/>
       <c r="I37" s="7"/>
       <c r="J37" s="35"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="103"/>
+      <c r="L37" s="99"/>
       <c r="M37" s="7"/>
       <c r="N37" s="35" t="s">
         <v>80</v>
       </c>
       <c r="O37" s="7"/>
-      <c r="P37" s="102" t="s">
+      <c r="P37" s="98" t="s">
         <v>14</v>
       </c>
       <c r="Q37" s="7"/>
@@ -5261,12 +5267,12 @@
         <v>Canada</v>
       </c>
       <c r="C38" s="7"/>
-      <c r="D38" s="106"/>
+      <c r="D38" s="102"/>
       <c r="E38" s="23">
         <f>IF(D37=Master!D33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F38" s="99" t="s">
+      <c r="F38" s="95" t="s">
         <v>12</v>
       </c>
       <c r="G38" s="23">
@@ -5285,14 +5291,14 @@
         <f>IF(N38=Master!N34,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N38" s="102" t="s">
+      <c r="N38" s="98" t="s">
         <v>14</v>
       </c>
       <c r="O38" s="23">
         <f>IF(P37=Master!P33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P38" s="103"/>
+      <c r="P38" s="99"/>
       <c r="Q38" s="7"/>
       <c r="R38" s="81" t="str">
         <f>D18</f>
@@ -5311,7 +5317,7 @@
         <v>72</v>
       </c>
       <c r="E39" s="7"/>
-      <c r="F39" s="100"/>
+      <c r="F39" s="96"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
@@ -5319,7 +5325,7 @@
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
-      <c r="N39" s="104"/>
+      <c r="N39" s="100"/>
       <c r="O39" s="7"/>
       <c r="P39" s="35" t="s">
         <v>76</v>
@@ -5338,14 +5344,14 @@
         <v>Brasil</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="102" t="s">
+      <c r="D40" s="98" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="23">
         <f>IF(D40=Master!D36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F40" s="101"/>
+      <c r="F40" s="97"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
@@ -5353,12 +5359,12 @@
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
-      <c r="N40" s="103"/>
+      <c r="N40" s="99"/>
       <c r="O40" s="23">
         <f>IF(P40=Master!P36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P40" s="102" t="s">
+      <c r="P40" s="98" t="s">
         <v>137</v>
       </c>
       <c r="Q40" s="7"/>
@@ -5380,7 +5386,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="103"/>
+      <c r="D41" s="99"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -5392,7 +5398,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="103"/>
+      <c r="P41" s="99"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="81" t="str">
         <f>D25</f>
@@ -5460,6 +5466,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="P34:P35"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="L35:L37"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="P37:P38"/>
+    <mergeCell ref="F38:F40"/>
+    <mergeCell ref="N38:N40"/>
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="J8:N8"/>
@@ -5476,14 +5490,6 @@
     <mergeCell ref="P31:P32"/>
     <mergeCell ref="F32:F34"/>
     <mergeCell ref="N32:N34"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="P34:P35"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="L35:L37"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="P37:P38"/>
-    <mergeCell ref="F38:F40"/>
-    <mergeCell ref="N38:N40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -5494,8 +5500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C64DF09A-2D3C-4C49-8B16-319C8D3CEDC7}">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3:R5"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5523,26 +5529,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="88"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="91"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="86" t="s">
+      <c r="J1" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="88"/>
-      <c r="P1" s="86" t="s">
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="91"/>
+      <c r="P1" s="89" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="88"/>
+      <c r="Q1" s="90"/>
+      <c r="R1" s="91"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -5663,12 +5669,12 @@
       <c r="H5" s="35"/>
       <c r="I5" s="52"/>
       <c r="J5" s="26" t="s">
-        <v>41</v>
+        <v>148</v>
       </c>
       <c r="K5" s="51"/>
       <c r="L5" s="51" t="str">
         <f>Master!F4</f>
-        <v>Sweden</v>
+        <v>USA</v>
       </c>
       <c r="M5" s="51"/>
       <c r="N5" s="34">
@@ -5702,12 +5708,12 @@
       <c r="H6" s="35"/>
       <c r="I6" s="52"/>
       <c r="J6" s="27" t="s">
-        <v>45</v>
+        <v>138</v>
       </c>
       <c r="K6" s="53"/>
       <c r="L6" s="53" t="str">
         <f>Master!F5</f>
-        <v>USA</v>
+        <v>Wales</v>
       </c>
       <c r="M6" s="53"/>
       <c r="N6" s="54">
@@ -5745,23 +5751,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="95" t="s">
+      <c r="B8" s="103" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="96"/>
-      <c r="D8" s="96"/>
-      <c r="E8" s="96"/>
-      <c r="F8" s="97"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="104"/>
+      <c r="E8" s="104"/>
+      <c r="F8" s="105"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="95" t="s">
+      <c r="J8" s="103" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="96"/>
-      <c r="L8" s="96"/>
-      <c r="M8" s="96"/>
-      <c r="N8" s="97"/>
+      <c r="K8" s="104"/>
+      <c r="L8" s="104"/>
+      <c r="M8" s="104"/>
+      <c r="N8" s="105"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -5951,23 +5957,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="95" t="s">
+      <c r="B15" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="96"/>
-      <c r="D15" s="96"/>
-      <c r="E15" s="96"/>
-      <c r="F15" s="97"/>
+      <c r="C15" s="104"/>
+      <c r="D15" s="104"/>
+      <c r="E15" s="104"/>
+      <c r="F15" s="105"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="95" t="s">
+      <c r="J15" s="103" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="96"/>
-      <c r="L15" s="96"/>
-      <c r="M15" s="96"/>
-      <c r="N15" s="97"/>
+      <c r="K15" s="104"/>
+      <c r="L15" s="104"/>
+      <c r="M15" s="104"/>
+      <c r="N15" s="105"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -6132,23 +6138,23 @@
       <c r="N21" s="52"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="95" t="s">
+      <c r="B22" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="96"/>
-      <c r="D22" s="96"/>
-      <c r="E22" s="96"/>
-      <c r="F22" s="97"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="105"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="95" t="s">
+      <c r="J22" s="103" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="96"/>
-      <c r="L22" s="96"/>
-      <c r="M22" s="96"/>
-      <c r="N22" s="97"/>
+      <c r="K22" s="104"/>
+      <c r="L22" s="104"/>
+      <c r="M22" s="104"/>
+      <c r="N22" s="105"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B23" s="56" t="s">
@@ -6387,7 +6393,7 @@
         <v>79</v>
       </c>
       <c r="O31" s="7"/>
-      <c r="P31" s="102" t="s">
+      <c r="P31" s="98" t="s">
         <v>41</v>
       </c>
       <c r="Q31" s="7"/>
@@ -6431,7 +6437,7 @@
         <f>IF(P31=Master!P27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P32" s="103"/>
+      <c r="P32" s="99"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="39" t="str">
         <f>D4</f>
@@ -6477,7 +6483,7 @@
         <v>Argentina</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="102" t="s">
+      <c r="D34" s="98" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="23">
@@ -6507,7 +6513,7 @@
         <f>IF(P34=Master!P30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P34" s="102" t="s">
+      <c r="P34" s="98" t="s">
         <v>34</v>
       </c>
       <c r="Q34" s="7"/>
@@ -6529,7 +6535,7 @@
         <v>France</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="103"/>
+      <c r="D35" s="99"/>
       <c r="E35" s="7"/>
       <c r="F35" s="35"/>
       <c r="G35" s="7"/>
@@ -6547,7 +6553,7 @@
       <c r="M35" s="7"/>
       <c r="N35" s="35"/>
       <c r="O35" s="7"/>
-      <c r="P35" s="103"/>
+      <c r="P35" s="99"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="39" t="str">
         <f>D11</f>
@@ -6601,7 +6607,7 @@
         <v>Italy</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="105" t="s">
+      <c r="D37" s="101" t="s">
         <v>139</v>
       </c>
       <c r="E37" s="7"/>
@@ -6641,7 +6647,7 @@
         <v>Canada</v>
       </c>
       <c r="C38" s="7"/>
-      <c r="D38" s="106"/>
+      <c r="D38" s="102"/>
       <c r="E38" s="23">
         <f>IF(D37=Master!D33,2,0)</f>
         <v>2</v>
@@ -6718,7 +6724,7 @@
         <v>Brasil</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="102" t="s">
+      <c r="D40" s="98" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="23">
@@ -6738,7 +6744,7 @@
         <f>IF(P40=Master!P36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P40" s="102" t="s">
+      <c r="P40" s="98" t="s">
         <v>137</v>
       </c>
       <c r="Q40" s="7"/>
@@ -6760,7 +6766,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="103"/>
+      <c r="D41" s="99"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -6772,7 +6778,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="103"/>
+      <c r="P41" s="99"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="39" t="str">
         <f>D25</f>
@@ -6840,13 +6846,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="J8:N8"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="D31:D32"/>
@@ -6863,6 +6862,13 @@
     <mergeCell ref="N38:N40"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="P40:P41"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="J8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -6873,8 +6879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB731263-BF9E-B94A-B168-4AE30BA7699C}">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3:R6"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6902,26 +6908,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="88"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="91"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="86" t="s">
+      <c r="J1" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="88"/>
-      <c r="P1" s="86" t="s">
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="91"/>
+      <c r="P1" s="89" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="88"/>
+      <c r="Q1" s="90"/>
+      <c r="R1" s="91"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -7042,12 +7048,12 @@
       <c r="H5" s="35"/>
       <c r="I5" s="52"/>
       <c r="J5" s="26" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="K5" s="51"/>
       <c r="L5" s="51" t="str">
         <f>Master!F4</f>
-        <v>Sweden</v>
+        <v>USA</v>
       </c>
       <c r="M5" s="51"/>
       <c r="N5" s="34">
@@ -7081,12 +7087,12 @@
       <c r="H6" s="35"/>
       <c r="I6" s="52"/>
       <c r="J6" s="27" t="s">
-        <v>49</v>
+        <v>138</v>
       </c>
       <c r="K6" s="53"/>
       <c r="L6" s="53" t="str">
         <f>Master!F5</f>
-        <v>USA</v>
+        <v>Wales</v>
       </c>
       <c r="M6" s="53"/>
       <c r="N6" s="54">
@@ -7124,23 +7130,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="95" t="s">
+      <c r="B8" s="103" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="96"/>
-      <c r="D8" s="96"/>
-      <c r="E8" s="96"/>
-      <c r="F8" s="97"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="104"/>
+      <c r="E8" s="104"/>
+      <c r="F8" s="105"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="95" t="s">
+      <c r="J8" s="103" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="96"/>
-      <c r="L8" s="96"/>
-      <c r="M8" s="96"/>
-      <c r="N8" s="97"/>
+      <c r="K8" s="104"/>
+      <c r="L8" s="104"/>
+      <c r="M8" s="104"/>
+      <c r="N8" s="105"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -7330,23 +7336,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="95" t="s">
+      <c r="B15" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="96"/>
-      <c r="D15" s="96"/>
-      <c r="E15" s="96"/>
-      <c r="F15" s="97"/>
+      <c r="C15" s="104"/>
+      <c r="D15" s="104"/>
+      <c r="E15" s="104"/>
+      <c r="F15" s="105"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="95" t="s">
+      <c r="J15" s="103" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="96"/>
-      <c r="L15" s="96"/>
-      <c r="M15" s="96"/>
-      <c r="N15" s="97"/>
+      <c r="K15" s="104"/>
+      <c r="L15" s="104"/>
+      <c r="M15" s="104"/>
+      <c r="N15" s="105"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -7513,23 +7519,23 @@
       <c r="N21" s="52"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="95" t="s">
+      <c r="B22" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="96"/>
-      <c r="D22" s="96"/>
-      <c r="E22" s="96"/>
-      <c r="F22" s="97"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="105"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="95" t="s">
+      <c r="J22" s="103" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="96"/>
-      <c r="L22" s="96"/>
-      <c r="M22" s="96"/>
-      <c r="N22" s="97"/>
+      <c r="K22" s="104"/>
+      <c r="L22" s="104"/>
+      <c r="M22" s="104"/>
+      <c r="N22" s="105"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B23" s="56" t="s">
@@ -8101,7 +8107,7 @@
         <v>Brasil</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="102" t="s">
+      <c r="D40" s="98" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="23">
@@ -8143,7 +8149,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="103"/>
+      <c r="D41" s="99"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -8223,13 +8229,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="J8:N8"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="D31:D32"/>
@@ -8246,6 +8245,13 @@
     <mergeCell ref="N38:N40"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="P40:P41"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="J8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -8256,8 +8262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61C1E5FA-F91B-4A41-A4C1-97D69E012813}">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3:R7"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8285,26 +8291,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="88"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="91"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="86" t="s">
+      <c r="J1" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="88"/>
-      <c r="P1" s="86" t="s">
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="91"/>
+      <c r="P1" s="89" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="88"/>
+      <c r="Q1" s="90"/>
+      <c r="R1" s="91"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -8425,12 +8431,12 @@
       <c r="H5" s="35"/>
       <c r="I5" s="52"/>
       <c r="J5" s="26" t="s">
-        <v>49</v>
+        <v>138</v>
       </c>
       <c r="K5" s="51"/>
       <c r="L5" s="50" t="str">
         <f>Master!F4</f>
-        <v>Sweden</v>
+        <v>USA</v>
       </c>
       <c r="M5" s="51"/>
       <c r="N5" s="34">
@@ -8464,12 +8470,12 @@
       <c r="H6" s="35"/>
       <c r="I6" s="52"/>
       <c r="J6" s="27" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="K6" s="53"/>
       <c r="L6" s="60" t="str">
         <f>Master!F5</f>
-        <v>USA</v>
+        <v>Wales</v>
       </c>
       <c r="M6" s="53"/>
       <c r="N6" s="54">
@@ -8507,23 +8513,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="95" t="s">
+      <c r="B8" s="103" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="96"/>
-      <c r="D8" s="96"/>
-      <c r="E8" s="96"/>
-      <c r="F8" s="97"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="104"/>
+      <c r="E8" s="104"/>
+      <c r="F8" s="105"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="95" t="s">
+      <c r="J8" s="103" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="96"/>
-      <c r="L8" s="96"/>
-      <c r="M8" s="96"/>
-      <c r="N8" s="97"/>
+      <c r="K8" s="104"/>
+      <c r="L8" s="104"/>
+      <c r="M8" s="104"/>
+      <c r="N8" s="105"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -8713,23 +8719,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="95" t="s">
+      <c r="B15" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="96"/>
-      <c r="D15" s="96"/>
-      <c r="E15" s="96"/>
-      <c r="F15" s="97"/>
+      <c r="C15" s="104"/>
+      <c r="D15" s="104"/>
+      <c r="E15" s="104"/>
+      <c r="F15" s="105"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="95" t="s">
+      <c r="J15" s="103" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="96"/>
-      <c r="L15" s="96"/>
-      <c r="M15" s="96"/>
-      <c r="N15" s="97"/>
+      <c r="K15" s="104"/>
+      <c r="L15" s="104"/>
+      <c r="M15" s="104"/>
+      <c r="N15" s="105"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -8896,23 +8902,23 @@
       <c r="N21" s="52"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="95" t="s">
+      <c r="B22" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="96"/>
-      <c r="D22" s="96"/>
-      <c r="E22" s="96"/>
-      <c r="F22" s="97"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="105"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="95" t="s">
+      <c r="J22" s="103" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="96"/>
-      <c r="L22" s="96"/>
-      <c r="M22" s="96"/>
-      <c r="N22" s="97"/>
+      <c r="K22" s="104"/>
+      <c r="L22" s="104"/>
+      <c r="M22" s="104"/>
+      <c r="N22" s="105"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B23" s="56" t="s">
@@ -9604,13 +9610,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="J8:N8"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="D31:D32"/>
@@ -9627,6 +9626,13 @@
     <mergeCell ref="N38:N40"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="P40:P41"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="J8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -9744,26 +9750,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="88"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="91"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="86" t="s">
+      <c r="J1" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="88"/>
-      <c r="P1" s="86" t="s">
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="91"/>
+      <c r="P1" s="89" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="88"/>
+      <c r="Q1" s="90"/>
+      <c r="R1" s="91"/>
       <c r="W1" s="1" t="s">
         <v>92</v>
       </c>
@@ -9944,7 +9950,7 @@
       <c r="K5" s="51"/>
       <c r="L5" s="51" t="str">
         <f>Master!F4</f>
-        <v>Sweden</v>
+        <v>USA</v>
       </c>
       <c r="M5" s="51"/>
       <c r="N5" s="34">
@@ -10007,7 +10013,7 @@
       <c r="K6" s="53"/>
       <c r="L6" s="53" t="str">
         <f>Master!F5</f>
-        <v>USA</v>
+        <v>Wales</v>
       </c>
       <c r="M6" s="53"/>
       <c r="N6" s="54">
@@ -10071,23 +10077,23 @@
       </c>
     </row>
     <row r="8" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B8" s="95" t="s">
+      <c r="B8" s="103" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="96"/>
-      <c r="D8" s="96"/>
-      <c r="E8" s="96"/>
-      <c r="F8" s="97"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="104"/>
+      <c r="E8" s="104"/>
+      <c r="F8" s="105"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="95" t="s">
+      <c r="J8" s="103" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="96"/>
-      <c r="L8" s="96"/>
-      <c r="M8" s="96"/>
-      <c r="N8" s="97"/>
+      <c r="K8" s="104"/>
+      <c r="L8" s="104"/>
+      <c r="M8" s="104"/>
+      <c r="N8" s="105"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -10375,23 +10381,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B15" s="95" t="s">
+      <c r="B15" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="96"/>
-      <c r="D15" s="96"/>
-      <c r="E15" s="96"/>
-      <c r="F15" s="97"/>
+      <c r="C15" s="104"/>
+      <c r="D15" s="104"/>
+      <c r="E15" s="104"/>
+      <c r="F15" s="105"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="95" t="s">
+      <c r="J15" s="103" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="96"/>
-      <c r="L15" s="96"/>
-      <c r="M15" s="96"/>
-      <c r="N15" s="97"/>
+      <c r="K15" s="104"/>
+      <c r="L15" s="104"/>
+      <c r="M15" s="104"/>
+      <c r="N15" s="105"/>
     </row>
     <row r="16" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -10656,23 +10662,23 @@
       <c r="N21" s="52"/>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B22" s="95" t="s">
+      <c r="B22" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="96"/>
-      <c r="D22" s="96"/>
-      <c r="E22" s="96"/>
-      <c r="F22" s="97"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="105"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="95" t="s">
+      <c r="J22" s="103" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="96"/>
-      <c r="L22" s="96"/>
-      <c r="M22" s="96"/>
-      <c r="N22" s="97"/>
+      <c r="K22" s="104"/>
+      <c r="L22" s="104"/>
+      <c r="M22" s="104"/>
+      <c r="N22" s="105"/>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B23" s="56" t="s">
@@ -11446,6 +11452,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="J8:N8"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="D31:D32"/>
@@ -11462,13 +11475,6 @@
     <mergeCell ref="N38:N40"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="P40:P41"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="J8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
css work for zoom at 100%
</commit_message>
<xml_diff>
--- a/excel docs/java testing-audit info.xlsx
+++ b/excel docs/java testing-audit info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joecollins/Desktop/documents/personal-projects/world-cup-heroku/excel docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D270751-C433-1443-991E-22317482CB1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D7E637-8E9F-5842-A334-9D95479A7D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -1892,8 +1892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5501,7 +5501,7 @@
   <dimension ref="A1:T43"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5635,7 +5635,7 @@
       <c r="H4" s="35"/>
       <c r="I4" s="52"/>
       <c r="J4" s="26" t="s">
-        <v>49</v>
+        <v>148</v>
       </c>
       <c r="K4" s="51"/>
       <c r="L4" s="51" t="str">
@@ -5669,7 +5669,7 @@
       <c r="H5" s="35"/>
       <c r="I5" s="52"/>
       <c r="J5" s="26" t="s">
-        <v>148</v>
+        <v>41</v>
       </c>
       <c r="K5" s="51"/>
       <c r="L5" s="51" t="str">
@@ -5708,7 +5708,7 @@
       <c r="H6" s="35"/>
       <c r="I6" s="52"/>
       <c r="J6" s="27" t="s">
-        <v>138</v>
+        <v>45</v>
       </c>
       <c r="K6" s="53"/>
       <c r="L6" s="53" t="str">
@@ -6880,7 +6880,7 @@
   <dimension ref="A1:T43"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8262,7 +8262,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61C1E5FA-F91B-4A41-A4C1-97D69E012813}">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
edit name page complete
</commit_message>
<xml_diff>
--- a/excel docs/java testing-audit info.xlsx
+++ b/excel docs/java testing-audit info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joecollins/Desktop/documents/personal-projects/world-cup-heroku/excel docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D7E637-8E9F-5842-A334-9D95479A7D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D55E277-19D1-2348-AA45-2E7DD05302F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22780" windowHeight="18680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="150">
   <si>
     <t>A1</t>
   </si>
@@ -620,9 +620,6 @@
     <t>Netherlands</t>
   </si>
   <si>
-    <t>Italy</t>
-  </si>
-  <si>
     <t>Cameroon</t>
   </si>
   <si>
@@ -657,6 +654,12 @@
   </si>
   <si>
     <t>Wales</t>
+  </si>
+  <si>
+    <t>FADT</t>
+  </si>
+  <si>
+    <t>SCGJ</t>
   </si>
 </sst>
 </file>
@@ -1465,31 +1468,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1499,6 +1505,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1523,18 +1541,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1606,9 +1612,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1892,8 +1895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView zoomScale="115" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1928,11 +1931,11 @@
       <c r="F1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="89" t="s">
+      <c r="J1" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="90"/>
-      <c r="L1" s="91"/>
+      <c r="K1" s="88"/>
+      <c r="L1" s="89"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B2" s="14" t="s">
@@ -1975,8 +1978,8 @@
         <v>133</v>
       </c>
       <c r="D4" s="7"/>
-      <c r="F4" s="131" t="s">
-        <v>138</v>
+      <c r="F4" s="86" t="s">
+        <v>137</v>
       </c>
       <c r="H4" s="7"/>
       <c r="J4" s="16" t="s">
@@ -1994,7 +1997,7 @@
       </c>
       <c r="D5" s="7"/>
       <c r="F5" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H5" s="7"/>
       <c r="J5" s="16" t="s">
@@ -2008,7 +2011,7 @@
     </row>
     <row r="6" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J6" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="17">
@@ -2035,7 +2038,7 @@
       </c>
       <c r="D8" s="7"/>
       <c r="F8" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H8" s="7"/>
       <c r="J8" s="16"/>
@@ -2047,8 +2050,8 @@
         <v>13</v>
       </c>
       <c r="D9" s="7"/>
-      <c r="F9" s="14" t="s">
-        <v>10</v>
+      <c r="F9" s="85" t="s">
+        <v>34</v>
       </c>
       <c r="H9" s="7"/>
       <c r="J9" s="16"/>
@@ -2060,8 +2063,8 @@
         <v>28</v>
       </c>
       <c r="D10" s="7"/>
-      <c r="F10" s="83" t="s">
-        <v>31</v>
+      <c r="F10" s="85" t="s">
+        <v>10</v>
       </c>
       <c r="H10" s="7"/>
       <c r="J10" s="18"/>
@@ -2090,8 +2093,8 @@
       <c r="H13" s="28"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B14" s="83" t="s">
-        <v>136</v>
+      <c r="B14" s="85" t="s">
+        <v>27</v>
       </c>
       <c r="D14" s="7"/>
       <c r="F14" s="14" t="s">
@@ -2101,11 +2104,11 @@
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B15" s="14" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="D15" s="7"/>
       <c r="F15" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H15" s="7"/>
     </row>
@@ -2146,17 +2149,17 @@
       </c>
       <c r="D20" s="7"/>
       <c r="F20" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H20" s="7"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B21" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D21" s="7"/>
       <c r="F21" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H21" s="7"/>
     </row>
@@ -2252,7 +2255,7 @@
         <v>Ecuador</v>
       </c>
       <c r="C27" s="7"/>
-      <c r="D27" s="86" t="s">
+      <c r="D27" s="90" t="s">
         <v>134</v>
       </c>
       <c r="E27" s="7"/>
@@ -2266,7 +2269,7 @@
       <c r="M27" s="7"/>
       <c r="N27" s="7"/>
       <c r="O27" s="7"/>
-      <c r="P27" s="86" t="s">
+      <c r="P27" s="90" t="s">
         <v>41</v>
       </c>
       <c r="Q27" s="7"/>
@@ -2288,9 +2291,9 @@
         <v>Iran</v>
       </c>
       <c r="C28" s="7"/>
-      <c r="D28" s="88"/>
+      <c r="D28" s="91"/>
       <c r="E28" s="7"/>
-      <c r="F28" s="86" t="s">
+      <c r="F28" s="90" t="s">
         <v>25</v>
       </c>
       <c r="G28" s="7"/>
@@ -2300,11 +2303,12 @@
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
       <c r="M28" s="7"/>
-      <c r="N28" s="86" t="s">
-        <v>34</v>
+      <c r="N28" s="90" t="str">
+        <f>P30</f>
+        <v>Australia</v>
       </c>
       <c r="O28" s="7"/>
-      <c r="P28" s="88"/>
+      <c r="P28" s="91"/>
       <c r="Q28" s="7"/>
       <c r="R28" s="15" t="str">
         <f>B3</f>
@@ -2321,7 +2325,7 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
-      <c r="F29" s="87"/>
+      <c r="F29" s="92"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
@@ -2329,7 +2333,7 @@
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
-      <c r="N29" s="87"/>
+      <c r="N29" s="92"/>
       <c r="O29" s="7"/>
       <c r="P29" s="7"/>
       <c r="Q29" s="7"/>
@@ -2346,11 +2350,11 @@
         <v>Argentina</v>
       </c>
       <c r="C30" s="7"/>
-      <c r="D30" s="86" t="s">
+      <c r="D30" s="90" t="s">
         <v>25</v>
       </c>
       <c r="E30" s="7"/>
-      <c r="F30" s="88"/>
+      <c r="F30" s="91"/>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
@@ -2358,15 +2362,16 @@
       <c r="K30" s="7"/>
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
-      <c r="N30" s="88"/>
+      <c r="N30" s="91"/>
       <c r="O30" s="7"/>
-      <c r="P30" s="86" t="s">
-        <v>34</v>
+      <c r="P30" s="90" t="str">
+        <f>R30</f>
+        <v>Australia</v>
       </c>
       <c r="Q30" s="7"/>
       <c r="R30" s="33" t="str">
         <f>F8</f>
-        <v>Denmark</v>
+        <v>Australia</v>
       </c>
       <c r="S30" s="7" t="s">
         <v>18</v>
@@ -2379,26 +2384,27 @@
       </c>
       <c r="B31" s="15" t="str">
         <f>F9</f>
-        <v>France</v>
+        <v>Denmark</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="88"/>
+      <c r="D31" s="91"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
-      <c r="H31" s="92" t="s">
+      <c r="H31" s="93" t="s">
         <v>25</v>
       </c>
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
-      <c r="L31" s="92" t="s">
-        <v>14</v>
+      <c r="L31" s="93" t="str">
+        <f>N28</f>
+        <v>Australia</v>
       </c>
       <c r="M31" s="7"/>
       <c r="N31" s="7"/>
       <c r="O31" s="7"/>
-      <c r="P31" s="88"/>
+      <c r="P31" s="91"/>
       <c r="Q31" s="7"/>
       <c r="R31" s="15" t="str">
         <f>B9</f>
@@ -2417,13 +2423,13 @@
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
-      <c r="H32" s="93"/>
+      <c r="H32" s="94"/>
       <c r="I32" s="7"/>
       <c r="J32" s="23" t="s">
         <v>25</v>
       </c>
       <c r="K32" s="7"/>
-      <c r="L32" s="93"/>
+      <c r="L32" s="94"/>
       <c r="M32" s="7"/>
       <c r="N32" s="7"/>
       <c r="O32" s="7"/>
@@ -2439,24 +2445,24 @@
       </c>
       <c r="B33" s="33" t="str">
         <f>B14</f>
-        <v>Italy</v>
+        <v>Germany</v>
       </c>
       <c r="C33" s="7"/>
-      <c r="D33" s="86" t="s">
-        <v>139</v>
+      <c r="D33" s="90" t="s">
+        <v>138</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
-      <c r="H33" s="94"/>
+      <c r="H33" s="95"/>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
-      <c r="L33" s="94"/>
+      <c r="L33" s="95"/>
       <c r="M33" s="7"/>
       <c r="N33" s="7"/>
       <c r="O33" s="7"/>
-      <c r="P33" s="86" t="s">
+      <c r="P33" s="90" t="s">
         <v>14</v>
       </c>
       <c r="Q33" s="7"/>
@@ -2478,9 +2484,9 @@
         <v>Canada</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="88"/>
+      <c r="D34" s="91"/>
       <c r="E34" s="7"/>
-      <c r="F34" s="86" t="s">
+      <c r="F34" s="90" t="s">
         <v>12</v>
       </c>
       <c r="G34" s="7"/>
@@ -2490,15 +2496,15 @@
       <c r="K34" s="7"/>
       <c r="L34" s="7"/>
       <c r="M34" s="7"/>
-      <c r="N34" s="86" t="s">
+      <c r="N34" s="90" t="s">
         <v>14</v>
       </c>
       <c r="O34" s="7"/>
-      <c r="P34" s="88"/>
+      <c r="P34" s="91"/>
       <c r="Q34" s="7"/>
       <c r="R34" s="15" t="str">
         <f>B15</f>
-        <v>Germany</v>
+        <v>Costa Rica</v>
       </c>
       <c r="S34" s="7" t="s">
         <v>21</v>
@@ -2511,7 +2517,7 @@
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
-      <c r="F35" s="87"/>
+      <c r="F35" s="92"/>
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
@@ -2519,7 +2525,7 @@
       <c r="K35" s="7"/>
       <c r="L35" s="7"/>
       <c r="M35" s="7"/>
-      <c r="N35" s="87"/>
+      <c r="N35" s="92"/>
       <c r="O35" s="7"/>
       <c r="P35" s="7"/>
       <c r="Q35" s="7"/>
@@ -2536,11 +2542,11 @@
         <v>Brasil</v>
       </c>
       <c r="C36" s="7"/>
-      <c r="D36" s="86" t="s">
+      <c r="D36" s="90" t="s">
         <v>12</v>
       </c>
       <c r="E36" s="7"/>
-      <c r="F36" s="88"/>
+      <c r="F36" s="91"/>
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
       <c r="I36" s="7"/>
@@ -2548,10 +2554,10 @@
       <c r="K36" s="7"/>
       <c r="L36" s="7"/>
       <c r="M36" s="7"/>
-      <c r="N36" s="88"/>
+      <c r="N36" s="91"/>
       <c r="O36" s="7"/>
-      <c r="P36" s="86" t="s">
-        <v>137</v>
+      <c r="P36" s="90" t="s">
+        <v>136</v>
       </c>
       <c r="Q36" s="7"/>
       <c r="R36" s="33" t="str">
@@ -2572,7 +2578,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="88"/>
+      <c r="D37" s="91"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
@@ -2584,7 +2590,7 @@
       <c r="M37" s="7"/>
       <c r="N37" s="7"/>
       <c r="O37" s="7"/>
-      <c r="P37" s="88"/>
+      <c r="P37" s="91"/>
       <c r="Q37" s="7"/>
       <c r="R37" s="15" t="str">
         <f>B21</f>
@@ -2619,6 +2625,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="N28:N30"/>
+    <mergeCell ref="N34:N36"/>
+    <mergeCell ref="P27:P28"/>
+    <mergeCell ref="P30:P31"/>
+    <mergeCell ref="P33:P34"/>
+    <mergeCell ref="P36:P37"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="D27:D28"/>
     <mergeCell ref="D30:D31"/>
@@ -2628,12 +2640,6 @@
     <mergeCell ref="F34:F36"/>
     <mergeCell ref="H31:H33"/>
     <mergeCell ref="L31:L33"/>
-    <mergeCell ref="N28:N30"/>
-    <mergeCell ref="N34:N36"/>
-    <mergeCell ref="P27:P28"/>
-    <mergeCell ref="P30:P31"/>
-    <mergeCell ref="P33:P34"/>
-    <mergeCell ref="P36:P37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -2654,30 +2660,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="63" x14ac:dyDescent="0.2">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="84" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="42" x14ac:dyDescent="0.2">
+      <c r="A2" s="84" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="42" x14ac:dyDescent="0.2">
-      <c r="A2" s="85" t="s">
+    <row r="3" spans="1:1" ht="63" x14ac:dyDescent="0.2">
+      <c r="A3" s="84" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="63" x14ac:dyDescent="0.2">
-      <c r="A3" s="85" t="s">
+    <row r="4" spans="1:1" ht="63" x14ac:dyDescent="0.2">
+      <c r="A4" s="84" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="63" x14ac:dyDescent="0.2">
-      <c r="A4" s="85" t="s">
-        <v>147</v>
-      </c>
-    </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="84"/>
+      <c r="A5" s="83"/>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="84"/>
+      <c r="A6" s="83"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2688,8 +2694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86316F4E-9A6C-492E-9EDB-018A26A821E8}">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2720,26 +2726,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="91"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="89"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="89" t="s">
+      <c r="J1" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="90"/>
-      <c r="L1" s="90"/>
-      <c r="M1" s="90"/>
-      <c r="N1" s="91"/>
-      <c r="P1" s="89" t="s">
+      <c r="K1" s="88"/>
+      <c r="L1" s="88"/>
+      <c r="M1" s="88"/>
+      <c r="N1" s="89"/>
+      <c r="P1" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="90"/>
-      <c r="R1" s="91"/>
+      <c r="Q1" s="88"/>
+      <c r="R1" s="89"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -2844,7 +2850,7 @@
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B5" s="26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C5" s="51"/>
       <c r="D5" s="51" t="str">
@@ -2860,7 +2866,7 @@
       <c r="H5" s="35"/>
       <c r="I5" s="52"/>
       <c r="J5" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K5" s="51"/>
       <c r="L5" s="50" t="str">
@@ -2899,7 +2905,7 @@
       <c r="H6" s="35"/>
       <c r="I6" s="52"/>
       <c r="J6" s="27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K6" s="53"/>
       <c r="L6" s="60" t="str">
@@ -2942,23 +2948,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="103" t="s">
+      <c r="B8" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="104"/>
-      <c r="D8" s="104"/>
-      <c r="E8" s="104"/>
-      <c r="F8" s="105"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="98"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="103" t="s">
+      <c r="J8" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="104"/>
-      <c r="L8" s="104"/>
-      <c r="M8" s="104"/>
-      <c r="N8" s="105"/>
+      <c r="K8" s="97"/>
+      <c r="L8" s="97"/>
+      <c r="M8" s="97"/>
+      <c r="N8" s="98"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -3021,12 +3027,12 @@
       <c r="H10" s="35"/>
       <c r="I10" s="52"/>
       <c r="J10" s="26" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="K10" s="51"/>
       <c r="L10" s="49" t="str">
         <f>Master!F8</f>
-        <v>Denmark</v>
+        <v>Australia</v>
       </c>
       <c r="M10" s="51"/>
       <c r="N10" s="34">
@@ -3052,12 +3058,12 @@
       <c r="H11" s="35"/>
       <c r="I11" s="52"/>
       <c r="J11" s="26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K11" s="51"/>
       <c r="L11" s="49" t="str">
         <f>Master!F9</f>
-        <v>France</v>
+        <v>Denmark</v>
       </c>
       <c r="M11" s="51"/>
       <c r="N11" s="34">
@@ -3090,12 +3096,12 @@
       <c r="H12" s="35"/>
       <c r="I12" s="52"/>
       <c r="J12" s="26" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="K12" s="51"/>
       <c r="L12" s="50" t="str">
         <f>Master!F10</f>
-        <v>Russia</v>
+        <v>France</v>
       </c>
       <c r="M12" s="51"/>
       <c r="N12" s="34">
@@ -3148,23 +3154,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="103" t="s">
+      <c r="B15" s="96" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="104"/>
-      <c r="D15" s="104"/>
-      <c r="E15" s="104"/>
-      <c r="F15" s="105"/>
+      <c r="C15" s="97"/>
+      <c r="D15" s="97"/>
+      <c r="E15" s="97"/>
+      <c r="F15" s="98"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="103" t="s">
+      <c r="J15" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="104"/>
-      <c r="L15" s="104"/>
-      <c r="M15" s="104"/>
-      <c r="N15" s="105"/>
+      <c r="K15" s="97"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="98"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -3195,12 +3201,12 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B17" s="26" t="s">
-        <v>136</v>
+        <v>27</v>
       </c>
       <c r="C17" s="51"/>
       <c r="D17" s="47" t="str">
         <f>Master!B14</f>
-        <v>Italy</v>
+        <v>Germany</v>
       </c>
       <c r="E17" s="51"/>
       <c r="F17" s="34">
@@ -3226,12 +3232,12 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B18" s="26" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C18" s="51"/>
       <c r="D18" s="48" t="str">
         <f>Master!B15</f>
-        <v>Germany</v>
+        <v>Costa Rica</v>
       </c>
       <c r="E18" s="51"/>
       <c r="F18" s="34">
@@ -3242,7 +3248,7 @@
       <c r="H18" s="35"/>
       <c r="I18" s="52"/>
       <c r="J18" s="26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K18" s="51"/>
       <c r="L18" s="48" t="str">
@@ -3285,10 +3291,10 @@
         <f t="shared" ref="N19:N20" si="5">IF(J19=L19,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Q19" s="106" t="s">
+      <c r="Q19" s="99" t="s">
         <v>82</v>
       </c>
-      <c r="R19" s="106"/>
+      <c r="R19" s="99"/>
     </row>
     <row r="20" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="27" t="s">
@@ -3343,23 +3349,23 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="103" t="s">
+      <c r="B22" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="104"/>
-      <c r="D22" s="104"/>
-      <c r="E22" s="104"/>
-      <c r="F22" s="105"/>
+      <c r="C22" s="97"/>
+      <c r="D22" s="97"/>
+      <c r="E22" s="97"/>
+      <c r="F22" s="98"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="103" t="s">
+      <c r="J22" s="96" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="104"/>
-      <c r="L22" s="104"/>
-      <c r="M22" s="104"/>
-      <c r="N22" s="105"/>
+      <c r="K22" s="97"/>
+      <c r="L22" s="97"/>
+      <c r="M22" s="97"/>
+      <c r="N22" s="98"/>
       <c r="Q22" s="49"/>
       <c r="R22" s="32" t="s">
         <v>85</v>
@@ -3429,7 +3435,7 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B25" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C25" s="51"/>
       <c r="D25" s="48" t="str">
@@ -3445,7 +3451,7 @@
       <c r="H25" s="52"/>
       <c r="I25" s="52"/>
       <c r="J25" s="26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K25" s="51"/>
       <c r="L25" s="51" t="str">
@@ -3501,7 +3507,7 @@
         <v>1</v>
       </c>
       <c r="J27" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K27" s="19"/>
       <c r="L27" s="19" t="str">
@@ -3590,7 +3596,7 @@
         <v>Ecuador</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="98" t="s">
+      <c r="D31" s="103" t="s">
         <v>134</v>
       </c>
       <c r="E31" s="7"/>
@@ -3608,7 +3614,7 @@
         <v>79</v>
       </c>
       <c r="O31" s="7"/>
-      <c r="P31" s="98" t="s">
+      <c r="P31" s="103" t="s">
         <v>41</v>
       </c>
       <c r="Q31" s="7"/>
@@ -3630,12 +3636,12 @@
         <v>Iran</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="99"/>
+      <c r="D32" s="104"/>
       <c r="E32" s="23">
         <f>IF(D31=Master!D27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F32" s="98" t="s">
+      <c r="F32" s="103" t="s">
         <v>25</v>
       </c>
       <c r="G32" s="7"/>
@@ -3645,14 +3651,15 @@
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
-      <c r="N32" s="98" t="s">
-        <v>34</v>
+      <c r="N32" s="103" t="str">
+        <f>P34</f>
+        <v>Australia</v>
       </c>
       <c r="O32" s="23">
         <f>IF(P31=Master!P27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P32" s="99"/>
+      <c r="P32" s="104"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="39" t="str">
         <f>D4</f>
@@ -3671,7 +3678,7 @@
         <v>70</v>
       </c>
       <c r="E33" s="7"/>
-      <c r="F33" s="100"/>
+      <c r="F33" s="105"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
@@ -3679,7 +3686,7 @@
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
-      <c r="N33" s="100"/>
+      <c r="N33" s="105"/>
       <c r="O33" s="7"/>
       <c r="P33" s="35" t="s">
         <v>74</v>
@@ -3698,14 +3705,14 @@
         <v>Argentina</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="98" t="s">
+      <c r="D34" s="103" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="23">
         <f>IF(D34=Master!D30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F34" s="99"/>
+      <c r="F34" s="104"/>
       <c r="G34" s="23">
         <f>IF(F32=Master!F28,4,0)</f>
         <v>4</v>
@@ -3723,18 +3730,18 @@
         <f>IF(N32=Master!N28,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N34" s="99"/>
+      <c r="N34" s="104"/>
       <c r="O34" s="23">
         <f>IF(P34=Master!P30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P34" s="98" t="s">
-        <v>34</v>
+      <c r="P34" s="103" t="s">
+        <v>35</v>
       </c>
       <c r="Q34" s="7"/>
       <c r="R34" s="38" t="str">
         <f>L10</f>
-        <v>Denmark</v>
+        <v>Australia</v>
       </c>
       <c r="S34" s="7" t="s">
         <v>18</v>
@@ -3747,14 +3754,14 @@
       </c>
       <c r="B35" s="63" t="str">
         <f>L11</f>
-        <v>France</v>
+        <v>Denmark</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="99"/>
+      <c r="D35" s="104"/>
       <c r="E35" s="7"/>
       <c r="F35" s="35"/>
       <c r="G35" s="7"/>
-      <c r="H35" s="98" t="s">
+      <c r="H35" s="103" t="s">
         <v>25</v>
       </c>
       <c r="I35" s="7"/>
@@ -3762,13 +3769,14 @@
         <v>81</v>
       </c>
       <c r="K35" s="7"/>
-      <c r="L35" s="98" t="s">
-        <v>14</v>
+      <c r="L35" s="103" t="str">
+        <f>N32</f>
+        <v>Australia</v>
       </c>
       <c r="M35" s="7"/>
       <c r="N35" s="35"/>
       <c r="O35" s="7"/>
-      <c r="P35" s="99"/>
+      <c r="P35" s="104"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="39" t="str">
         <f>D11</f>
@@ -3789,7 +3797,7 @@
       <c r="E36" s="7"/>
       <c r="F36" s="35"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="100"/>
+      <c r="H36" s="105"/>
       <c r="I36" s="24">
         <f>IF(H35=Master!H31,6,0)</f>
         <v>6</v>
@@ -3801,7 +3809,7 @@
         <f>IF(L35=Master!L31,6,0)</f>
         <v>6</v>
       </c>
-      <c r="L36" s="100"/>
+      <c r="L36" s="105"/>
       <c r="M36" s="7"/>
       <c r="N36" s="35"/>
       <c r="O36" s="7"/>
@@ -3819,28 +3827,28 @@
       </c>
       <c r="B37" s="64" t="str">
         <f>D17</f>
-        <v>Italy</v>
+        <v>Germany</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="101" t="s">
-        <v>139</v>
+      <c r="D37" s="106" t="s">
+        <v>138</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="35" t="s">
         <v>78</v>
       </c>
       <c r="G37" s="7"/>
-      <c r="H37" s="99"/>
+      <c r="H37" s="104"/>
       <c r="I37" s="7"/>
       <c r="J37" s="35"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="99"/>
+      <c r="L37" s="104"/>
       <c r="M37" s="7"/>
       <c r="N37" s="35" t="s">
         <v>80</v>
       </c>
       <c r="O37" s="7"/>
-      <c r="P37" s="98" t="s">
+      <c r="P37" s="103" t="s">
         <v>14</v>
       </c>
       <c r="Q37" s="7"/>
@@ -3862,12 +3870,12 @@
         <v>Canada</v>
       </c>
       <c r="C38" s="7"/>
-      <c r="D38" s="102"/>
+      <c r="D38" s="107"/>
       <c r="E38" s="23">
         <f>IF(D37=Master!D33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F38" s="95" t="s">
+      <c r="F38" s="100" t="s">
         <v>12</v>
       </c>
       <c r="G38" s="23">
@@ -3886,18 +3894,18 @@
         <f>IF(N38=Master!N34,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N38" s="98" t="s">
+      <c r="N38" s="103" t="s">
         <v>14</v>
       </c>
       <c r="O38" s="23">
         <f>IF(P37=Master!P33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P38" s="99"/>
+      <c r="P38" s="104"/>
       <c r="Q38" s="7"/>
       <c r="R38" s="39" t="str">
         <f>D18</f>
-        <v>Germany</v>
+        <v>Costa Rica</v>
       </c>
       <c r="S38" s="7" t="s">
         <v>21</v>
@@ -3912,7 +3920,7 @@
         <v>72</v>
       </c>
       <c r="E39" s="7"/>
-      <c r="F39" s="96"/>
+      <c r="F39" s="101"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
@@ -3920,7 +3928,7 @@
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
-      <c r="N39" s="100"/>
+      <c r="N39" s="105"/>
       <c r="O39" s="7"/>
       <c r="P39" s="35" t="s">
         <v>76</v>
@@ -3939,14 +3947,14 @@
         <v>Brasil</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="98" t="s">
+      <c r="D40" s="103" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="23">
         <f>IF(D40=Master!D36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F40" s="97"/>
+      <c r="F40" s="102"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
@@ -3954,13 +3962,13 @@
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
-      <c r="N40" s="99"/>
+      <c r="N40" s="104"/>
       <c r="O40" s="23">
         <f>IF(P40=Master!P36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P40" s="98" t="s">
-        <v>137</v>
+      <c r="P40" s="103" t="s">
+        <v>136</v>
       </c>
       <c r="Q40" s="7"/>
       <c r="R40" s="38" t="str">
@@ -3981,7 +3989,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="99"/>
+      <c r="D41" s="104"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -3993,7 +4001,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="99"/>
+      <c r="P41" s="104"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="39" t="str">
         <f>D25</f>
@@ -4061,16 +4069,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J22:N22"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="J8:N8"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="Q19:R19"/>
     <mergeCell ref="F38:F40"/>
     <mergeCell ref="P37:P38"/>
     <mergeCell ref="P40:P41"/>
@@ -4085,6 +4083,16 @@
     <mergeCell ref="D37:D38"/>
     <mergeCell ref="H35:H37"/>
     <mergeCell ref="L35:L37"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J22:N22"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="Q19:R19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -4095,8 +4103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69337711-055D-1241-BEB8-C726DCD4CFE4}">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4127,26 +4135,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="91"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="89"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="89" t="s">
+      <c r="J1" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="90"/>
-      <c r="L1" s="90"/>
-      <c r="M1" s="90"/>
-      <c r="N1" s="91"/>
-      <c r="P1" s="89" t="s">
+      <c r="K1" s="88"/>
+      <c r="L1" s="88"/>
+      <c r="M1" s="88"/>
+      <c r="N1" s="89"/>
+      <c r="P1" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="90"/>
-      <c r="R1" s="91"/>
+      <c r="Q1" s="88"/>
+      <c r="R1" s="89"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -4251,7 +4259,7 @@
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B5" s="26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C5" s="51"/>
       <c r="D5" s="51" t="str">
@@ -4267,7 +4275,7 @@
       <c r="H5" s="35"/>
       <c r="I5" s="52"/>
       <c r="J5" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K5" s="51"/>
       <c r="L5" s="50" t="str">
@@ -4306,7 +4314,7 @@
       <c r="H6" s="35"/>
       <c r="I6" s="52"/>
       <c r="J6" s="27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K6" s="53"/>
       <c r="L6" s="60" t="str">
@@ -4349,23 +4357,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="103" t="s">
+      <c r="B8" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="104"/>
-      <c r="D8" s="104"/>
-      <c r="E8" s="104"/>
-      <c r="F8" s="105"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="98"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="103" t="s">
+      <c r="J8" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="104"/>
-      <c r="L8" s="104"/>
-      <c r="M8" s="104"/>
-      <c r="N8" s="105"/>
+      <c r="K8" s="97"/>
+      <c r="L8" s="97"/>
+      <c r="M8" s="97"/>
+      <c r="N8" s="98"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -4428,12 +4436,12 @@
       <c r="H10" s="35"/>
       <c r="I10" s="52"/>
       <c r="J10" s="26" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="K10" s="51"/>
       <c r="L10" s="49" t="str">
         <f>Master!F8</f>
-        <v>Denmark</v>
+        <v>Australia</v>
       </c>
       <c r="M10" s="51"/>
       <c r="N10" s="34">
@@ -4459,12 +4467,12 @@
       <c r="H11" s="35"/>
       <c r="I11" s="52"/>
       <c r="J11" s="26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K11" s="51"/>
       <c r="L11" s="49" t="str">
         <f>Master!F9</f>
-        <v>France</v>
+        <v>Denmark</v>
       </c>
       <c r="M11" s="51"/>
       <c r="N11" s="34">
@@ -4497,12 +4505,12 @@
       <c r="H12" s="35"/>
       <c r="I12" s="52"/>
       <c r="J12" s="26" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="K12" s="51"/>
       <c r="L12" s="50" t="str">
         <f>Master!F10</f>
-        <v>Russia</v>
+        <v>France</v>
       </c>
       <c r="M12" s="51"/>
       <c r="N12" s="34">
@@ -4555,23 +4563,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="103" t="s">
+      <c r="B15" s="96" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="104"/>
-      <c r="D15" s="104"/>
-      <c r="E15" s="104"/>
-      <c r="F15" s="105"/>
+      <c r="C15" s="97"/>
+      <c r="D15" s="97"/>
+      <c r="E15" s="97"/>
+      <c r="F15" s="98"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="103" t="s">
+      <c r="J15" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="104"/>
-      <c r="L15" s="104"/>
-      <c r="M15" s="104"/>
-      <c r="N15" s="105"/>
+      <c r="K15" s="97"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="98"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -4602,12 +4610,12 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B17" s="26" t="s">
-        <v>136</v>
+        <v>27</v>
       </c>
       <c r="C17" s="51"/>
       <c r="D17" s="47" t="str">
         <f>Master!B14</f>
-        <v>Italy</v>
+        <v>Germany</v>
       </c>
       <c r="E17" s="51"/>
       <c r="F17" s="34">
@@ -4633,12 +4641,12 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B18" s="26" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C18" s="51"/>
       <c r="D18" s="48" t="str">
         <f>Master!B15</f>
-        <v>Germany</v>
+        <v>Costa Rica</v>
       </c>
       <c r="E18" s="51"/>
       <c r="F18" s="34">
@@ -4649,7 +4657,7 @@
       <c r="H18" s="35"/>
       <c r="I18" s="52"/>
       <c r="J18" s="26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K18" s="51"/>
       <c r="L18" s="48" t="str">
@@ -4692,10 +4700,10 @@
         <f t="shared" ref="N19:N20" si="5">IF(J19=L19,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Q19" s="106" t="s">
+      <c r="Q19" s="99" t="s">
         <v>82</v>
       </c>
-      <c r="R19" s="106"/>
+      <c r="R19" s="99"/>
     </row>
     <row r="20" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="27" t="s">
@@ -4750,23 +4758,23 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="103" t="s">
+      <c r="B22" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="104"/>
-      <c r="D22" s="104"/>
-      <c r="E22" s="104"/>
-      <c r="F22" s="105"/>
+      <c r="C22" s="97"/>
+      <c r="D22" s="97"/>
+      <c r="E22" s="97"/>
+      <c r="F22" s="98"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="103" t="s">
+      <c r="J22" s="96" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="104"/>
-      <c r="L22" s="104"/>
-      <c r="M22" s="104"/>
-      <c r="N22" s="105"/>
+      <c r="K22" s="97"/>
+      <c r="L22" s="97"/>
+      <c r="M22" s="97"/>
+      <c r="N22" s="98"/>
       <c r="Q22" s="49"/>
       <c r="R22" s="32" t="s">
         <v>85</v>
@@ -4836,7 +4844,7 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B25" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C25" s="51"/>
       <c r="D25" s="48" t="str">
@@ -4852,7 +4860,7 @@
       <c r="H25" s="52"/>
       <c r="I25" s="52"/>
       <c r="J25" s="26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K25" s="51"/>
       <c r="L25" s="51" t="str">
@@ -4908,7 +4916,7 @@
         <v>1</v>
       </c>
       <c r="J27" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K27" s="19"/>
       <c r="L27" s="19" t="str">
@@ -4997,7 +5005,7 @@
         <v>Ecuador</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="98" t="s">
+      <c r="D31" s="103" t="s">
         <v>134</v>
       </c>
       <c r="E31" s="7"/>
@@ -5015,7 +5023,7 @@
         <v>79</v>
       </c>
       <c r="O31" s="7"/>
-      <c r="P31" s="98" t="s">
+      <c r="P31" s="103" t="s">
         <v>41</v>
       </c>
       <c r="Q31" s="7"/>
@@ -5037,12 +5045,12 @@
         <v>Iran</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="99"/>
+      <c r="D32" s="104"/>
       <c r="E32" s="23">
         <f>IF(D31=Master!D27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F32" s="98" t="s">
+      <c r="F32" s="103" t="s">
         <v>25</v>
       </c>
       <c r="G32" s="7"/>
@@ -5052,14 +5060,15 @@
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
-      <c r="N32" s="98" t="s">
-        <v>34</v>
+      <c r="N32" s="103" t="str">
+        <f>P34</f>
+        <v>Australia</v>
       </c>
       <c r="O32" s="23">
         <f>IF(P31=Master!P27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P32" s="99"/>
+      <c r="P32" s="104"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="81" t="str">
         <f>D4</f>
@@ -5078,7 +5087,7 @@
         <v>70</v>
       </c>
       <c r="E33" s="7"/>
-      <c r="F33" s="100"/>
+      <c r="F33" s="105"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
@@ -5086,7 +5095,7 @@
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
-      <c r="N33" s="100"/>
+      <c r="N33" s="105"/>
       <c r="O33" s="7"/>
       <c r="P33" s="35"/>
       <c r="Q33" s="7"/>
@@ -5103,14 +5112,14 @@
         <v>Argentina</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="98" t="s">
+      <c r="D34" s="103" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="23">
         <f>IF(D34=Master!D30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F34" s="99"/>
+      <c r="F34" s="104"/>
       <c r="G34" s="23">
         <f>IF(F32=Master!F28,4,0)</f>
         <v>4</v>
@@ -5128,18 +5137,18 @@
         <f>IF(N32=Master!N28,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N34" s="99"/>
+      <c r="N34" s="104"/>
       <c r="O34" s="23">
         <f>IF(P34=Master!P30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P34" s="98" t="s">
-        <v>34</v>
+      <c r="P34" s="103" t="s">
+        <v>35</v>
       </c>
       <c r="Q34" s="7"/>
       <c r="R34" s="80" t="str">
         <f>L10</f>
-        <v>Denmark</v>
+        <v>Australia</v>
       </c>
       <c r="S34" s="7" t="s">
         <v>18</v>
@@ -5152,14 +5161,14 @@
       </c>
       <c r="B35" s="63" t="str">
         <f>L11</f>
-        <v>France</v>
+        <v>Denmark</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="99"/>
+      <c r="D35" s="104"/>
       <c r="E35" s="7"/>
       <c r="F35" s="35"/>
       <c r="G35" s="7"/>
-      <c r="H35" s="98" t="s">
+      <c r="H35" s="103" t="s">
         <v>25</v>
       </c>
       <c r="I35" s="7"/>
@@ -5167,13 +5176,14 @@
         <v>81</v>
       </c>
       <c r="K35" s="7"/>
-      <c r="L35" s="98" t="s">
-        <v>14</v>
+      <c r="L35" s="103" t="str">
+        <f>N32</f>
+        <v>Australia</v>
       </c>
       <c r="M35" s="7"/>
       <c r="N35" s="35"/>
       <c r="O35" s="7"/>
-      <c r="P35" s="99"/>
+      <c r="P35" s="104"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="81" t="str">
         <f>D11</f>
@@ -5194,7 +5204,7 @@
       <c r="E36" s="7"/>
       <c r="F36" s="35"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="100"/>
+      <c r="H36" s="105"/>
       <c r="I36" s="24">
         <f>IF(H35=Master!H31,6,0)</f>
         <v>6</v>
@@ -5206,7 +5216,7 @@
         <f>IF(L35=Master!L31,6,0)</f>
         <v>6</v>
       </c>
-      <c r="L36" s="100"/>
+      <c r="L36" s="105"/>
       <c r="M36" s="7"/>
       <c r="N36" s="35"/>
       <c r="O36" s="7"/>
@@ -5224,28 +5234,28 @@
       </c>
       <c r="B37" s="64" t="str">
         <f>D17</f>
-        <v>Italy</v>
+        <v>Germany</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="101" t="s">
-        <v>139</v>
+      <c r="D37" s="106" t="s">
+        <v>138</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="35" t="s">
         <v>78</v>
       </c>
       <c r="G37" s="7"/>
-      <c r="H37" s="99"/>
+      <c r="H37" s="104"/>
       <c r="I37" s="7"/>
       <c r="J37" s="35"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="99"/>
+      <c r="L37" s="104"/>
       <c r="M37" s="7"/>
       <c r="N37" s="35" t="s">
         <v>80</v>
       </c>
       <c r="O37" s="7"/>
-      <c r="P37" s="98" t="s">
+      <c r="P37" s="103" t="s">
         <v>14</v>
       </c>
       <c r="Q37" s="7"/>
@@ -5267,12 +5277,12 @@
         <v>Canada</v>
       </c>
       <c r="C38" s="7"/>
-      <c r="D38" s="102"/>
+      <c r="D38" s="107"/>
       <c r="E38" s="23">
         <f>IF(D37=Master!D33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F38" s="95" t="s">
+      <c r="F38" s="100" t="s">
         <v>12</v>
       </c>
       <c r="G38" s="23">
@@ -5291,18 +5301,18 @@
         <f>IF(N38=Master!N34,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N38" s="98" t="s">
+      <c r="N38" s="103" t="s">
         <v>14</v>
       </c>
       <c r="O38" s="23">
         <f>IF(P37=Master!P33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P38" s="99"/>
+      <c r="P38" s="104"/>
       <c r="Q38" s="7"/>
       <c r="R38" s="81" t="str">
         <f>D18</f>
-        <v>Germany</v>
+        <v>Costa Rica</v>
       </c>
       <c r="S38" s="7" t="s">
         <v>21</v>
@@ -5317,7 +5327,7 @@
         <v>72</v>
       </c>
       <c r="E39" s="7"/>
-      <c r="F39" s="96"/>
+      <c r="F39" s="101"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
@@ -5325,7 +5335,7 @@
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
-      <c r="N39" s="100"/>
+      <c r="N39" s="105"/>
       <c r="O39" s="7"/>
       <c r="P39" s="35" t="s">
         <v>76</v>
@@ -5344,14 +5354,14 @@
         <v>Brasil</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="98" t="s">
+      <c r="D40" s="103" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="23">
         <f>IF(D40=Master!D36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F40" s="97"/>
+      <c r="F40" s="102"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
@@ -5359,13 +5369,13 @@
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
-      <c r="N40" s="99"/>
+      <c r="N40" s="104"/>
       <c r="O40" s="23">
         <f>IF(P40=Master!P36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P40" s="98" t="s">
-        <v>137</v>
+      <c r="P40" s="103" t="s">
+        <v>136</v>
       </c>
       <c r="Q40" s="7"/>
       <c r="R40" s="80" t="str">
@@ -5386,7 +5396,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="99"/>
+      <c r="D41" s="104"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -5398,7 +5408,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="99"/>
+      <c r="P41" s="104"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="81" t="str">
         <f>D25</f>
@@ -5466,14 +5476,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="P34:P35"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="L35:L37"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="P37:P38"/>
-    <mergeCell ref="F38:F40"/>
-    <mergeCell ref="N38:N40"/>
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="J8:N8"/>
@@ -5490,6 +5492,14 @@
     <mergeCell ref="P31:P32"/>
     <mergeCell ref="F32:F34"/>
     <mergeCell ref="N32:N34"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="P34:P35"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="L35:L37"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="P37:P38"/>
+    <mergeCell ref="F38:F40"/>
+    <mergeCell ref="N38:N40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -5500,8 +5510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C64DF09A-2D3C-4C49-8B16-319C8D3CEDC7}">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView topLeftCell="A14" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5529,26 +5539,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="91"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="89"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="89" t="s">
+      <c r="J1" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="90"/>
-      <c r="L1" s="90"/>
-      <c r="M1" s="90"/>
-      <c r="N1" s="91"/>
-      <c r="P1" s="89" t="s">
+      <c r="K1" s="88"/>
+      <c r="L1" s="88"/>
+      <c r="M1" s="88"/>
+      <c r="N1" s="89"/>
+      <c r="P1" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="90"/>
-      <c r="R1" s="91"/>
+      <c r="Q1" s="88"/>
+      <c r="R1" s="89"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -5596,7 +5606,7 @@
       <c r="H3" s="35"/>
       <c r="I3" s="52"/>
       <c r="J3" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K3" s="51"/>
       <c r="L3" s="51" t="str">
@@ -5635,7 +5645,7 @@
       <c r="H4" s="35"/>
       <c r="I4" s="52"/>
       <c r="J4" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K4" s="51"/>
       <c r="L4" s="51" t="str">
@@ -5751,23 +5761,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="103" t="s">
+      <c r="B8" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="104"/>
-      <c r="D8" s="104"/>
-      <c r="E8" s="104"/>
-      <c r="F8" s="105"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="98"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="103" t="s">
+      <c r="J8" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="104"/>
-      <c r="L8" s="104"/>
-      <c r="M8" s="104"/>
-      <c r="N8" s="105"/>
+      <c r="K8" s="97"/>
+      <c r="L8" s="97"/>
+      <c r="M8" s="97"/>
+      <c r="N8" s="98"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -5830,12 +5840,12 @@
       <c r="H10" s="35"/>
       <c r="I10" s="52"/>
       <c r="J10" s="26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K10" s="51"/>
       <c r="L10" s="47" t="str">
         <f>Master!F8</f>
-        <v>Denmark</v>
+        <v>Australia</v>
       </c>
       <c r="M10" s="51"/>
       <c r="N10" s="34">
@@ -5861,12 +5871,12 @@
       <c r="H11" s="35"/>
       <c r="I11" s="52"/>
       <c r="J11" s="26" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="K11" s="51"/>
       <c r="L11" s="48" t="str">
         <f>Master!F9</f>
-        <v>France</v>
+        <v>Denmark</v>
       </c>
       <c r="M11" s="51"/>
       <c r="N11" s="34">
@@ -5904,7 +5914,7 @@
       <c r="K12" s="51"/>
       <c r="L12" s="51" t="str">
         <f>Master!F10</f>
-        <v>Russia</v>
+        <v>France</v>
       </c>
       <c r="M12" s="51"/>
       <c r="N12" s="34">
@@ -5930,7 +5940,7 @@
       <c r="H13" s="35"/>
       <c r="I13" s="52"/>
       <c r="J13" s="27" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="K13" s="53"/>
       <c r="L13" s="53" t="str">
@@ -5957,23 +5967,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="103" t="s">
+      <c r="B15" s="96" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="104"/>
-      <c r="D15" s="104"/>
-      <c r="E15" s="104"/>
-      <c r="F15" s="105"/>
+      <c r="C15" s="97"/>
+      <c r="D15" s="97"/>
+      <c r="E15" s="97"/>
+      <c r="F15" s="98"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="103" t="s">
+      <c r="J15" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="104"/>
-      <c r="L15" s="104"/>
-      <c r="M15" s="104"/>
-      <c r="N15" s="105"/>
+      <c r="K15" s="97"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="98"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -6004,12 +6014,12 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B17" s="26" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C17" s="51"/>
       <c r="D17" s="51" t="str">
         <f>Master!B14</f>
-        <v>Italy</v>
+        <v>Germany</v>
       </c>
       <c r="E17" s="51"/>
       <c r="F17" s="34">
@@ -6039,7 +6049,7 @@
       <c r="C18" s="51"/>
       <c r="D18" s="49" t="str">
         <f>Master!B15</f>
-        <v>Germany</v>
+        <v>Costa Rica</v>
       </c>
       <c r="E18" s="51"/>
       <c r="F18" s="34">
@@ -6049,7 +6059,7 @@
       <c r="H18" s="35"/>
       <c r="I18" s="52"/>
       <c r="J18" s="26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K18" s="51"/>
       <c r="L18" s="48" t="str">
@@ -6064,7 +6074,7 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B19" s="26" t="s">
-        <v>136</v>
+        <v>27</v>
       </c>
       <c r="C19" s="51"/>
       <c r="D19" s="51" t="str">
@@ -6138,23 +6148,23 @@
       <c r="N21" s="52"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="103" t="s">
+      <c r="B22" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="104"/>
-      <c r="D22" s="104"/>
-      <c r="E22" s="104"/>
-      <c r="F22" s="105"/>
+      <c r="C22" s="97"/>
+      <c r="D22" s="97"/>
+      <c r="E22" s="97"/>
+      <c r="F22" s="98"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="103" t="s">
+      <c r="J22" s="96" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="104"/>
-      <c r="L22" s="104"/>
-      <c r="M22" s="104"/>
-      <c r="N22" s="105"/>
+      <c r="K22" s="97"/>
+      <c r="L22" s="97"/>
+      <c r="M22" s="97"/>
+      <c r="N22" s="98"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B23" s="56" t="s">
@@ -6215,7 +6225,7 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B25" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C25" s="51"/>
       <c r="D25" s="48" t="str">
@@ -6231,7 +6241,7 @@
       <c r="H25" s="52"/>
       <c r="I25" s="52"/>
       <c r="J25" s="26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K25" s="51"/>
       <c r="L25" s="51" t="str">
@@ -6286,7 +6296,7 @@
         <v>1</v>
       </c>
       <c r="J27" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K27" s="19"/>
       <c r="L27" s="19" t="str">
@@ -6375,7 +6385,7 @@
         <v>Ecuador</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="107" t="s">
+      <c r="D31" s="108" t="s">
         <v>45</v>
       </c>
       <c r="E31" s="7"/>
@@ -6393,7 +6403,7 @@
         <v>79</v>
       </c>
       <c r="O31" s="7"/>
-      <c r="P31" s="98" t="s">
+      <c r="P31" s="103" t="s">
         <v>41</v>
       </c>
       <c r="Q31" s="7"/>
@@ -6415,12 +6425,12 @@
         <v>Iran</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="108"/>
+      <c r="D32" s="109"/>
       <c r="E32" s="23">
         <f>IF(D31=Master!D27,2,0)</f>
         <v>0</v>
       </c>
-      <c r="F32" s="107" t="s">
+      <c r="F32" s="108" t="s">
         <v>45</v>
       </c>
       <c r="G32" s="7"/>
@@ -6430,14 +6440,14 @@
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
-      <c r="N32" s="107" t="s">
+      <c r="N32" s="108" t="s">
         <v>41</v>
       </c>
       <c r="O32" s="23">
         <f>IF(P31=Master!P27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P32" s="99"/>
+      <c r="P32" s="104"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="39" t="str">
         <f>D4</f>
@@ -6456,7 +6466,7 @@
         <v>70</v>
       </c>
       <c r="E33" s="7"/>
-      <c r="F33" s="109"/>
+      <c r="F33" s="110"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
@@ -6464,7 +6474,7 @@
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
-      <c r="N33" s="109"/>
+      <c r="N33" s="110"/>
       <c r="O33" s="7"/>
       <c r="P33" s="35" t="s">
         <v>74</v>
@@ -6483,14 +6493,14 @@
         <v>Argentina</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="98" t="s">
+      <c r="D34" s="103" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="23">
         <f>IF(D34=Master!D30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F34" s="108"/>
+      <c r="F34" s="109"/>
       <c r="G34" s="23">
         <f>IF(F32=Master!F28,4,0)</f>
         <v>0</v>
@@ -6508,18 +6518,18 @@
         <f>IF(N32=Master!N28,4,0)</f>
         <v>0</v>
       </c>
-      <c r="N34" s="108"/>
+      <c r="N34" s="109"/>
       <c r="O34" s="23">
         <f>IF(P34=Master!P30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P34" s="98" t="s">
-        <v>34</v>
+      <c r="P34" s="103" t="s">
+        <v>35</v>
       </c>
       <c r="Q34" s="7"/>
       <c r="R34" s="38" t="str">
         <f>L10</f>
-        <v>Denmark</v>
+        <v>Australia</v>
       </c>
       <c r="S34" s="7" t="s">
         <v>18</v>
@@ -6532,28 +6542,29 @@
       </c>
       <c r="B35" s="63" t="str">
         <f>L11</f>
-        <v>France</v>
+        <v>Denmark</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="99"/>
+      <c r="D35" s="104"/>
       <c r="E35" s="7"/>
       <c r="F35" s="35"/>
       <c r="G35" s="7"/>
-      <c r="H35" s="107" t="s">
-        <v>139</v>
+      <c r="H35" s="108" t="s">
+        <v>138</v>
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="35" t="s">
         <v>81</v>
       </c>
       <c r="K35" s="7"/>
-      <c r="L35" s="107" t="s">
-        <v>27</v>
+      <c r="L35" s="108" t="str">
+        <f>N38</f>
+        <v>Costa Rica</v>
       </c>
       <c r="M35" s="7"/>
       <c r="N35" s="35"/>
       <c r="O35" s="7"/>
-      <c r="P35" s="99"/>
+      <c r="P35" s="104"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="39" t="str">
         <f>D11</f>
@@ -6574,19 +6585,19 @@
       <c r="E36" s="7"/>
       <c r="F36" s="35"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="109"/>
+      <c r="H36" s="110"/>
       <c r="I36" s="24">
         <f>IF(H35=Master!H31,6,0)</f>
         <v>0</v>
       </c>
       <c r="J36" s="68" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K36" s="25">
         <f>IF(L35=Master!L31,6,0)</f>
         <v>0</v>
       </c>
-      <c r="L36" s="109"/>
+      <c r="L36" s="110"/>
       <c r="M36" s="7"/>
       <c r="N36" s="35"/>
       <c r="O36" s="7"/>
@@ -6604,29 +6615,29 @@
       </c>
       <c r="B37" s="64" t="str">
         <f>D17</f>
-        <v>Italy</v>
+        <v>Germany</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="101" t="s">
-        <v>139</v>
+      <c r="D37" s="106" t="s">
+        <v>138</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="35" t="s">
         <v>78</v>
       </c>
       <c r="G37" s="7"/>
-      <c r="H37" s="108"/>
+      <c r="H37" s="109"/>
       <c r="I37" s="7"/>
       <c r="J37" s="35"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="108"/>
+      <c r="L37" s="109"/>
       <c r="M37" s="7"/>
       <c r="N37" s="35" t="s">
         <v>80</v>
       </c>
       <c r="O37" s="7"/>
-      <c r="P37" s="107" t="s">
-        <v>27</v>
+      <c r="P37" s="108" t="s">
+        <v>38</v>
       </c>
       <c r="Q37" s="7"/>
       <c r="R37" s="38" t="str">
@@ -6647,13 +6658,13 @@
         <v>Canada</v>
       </c>
       <c r="C38" s="7"/>
-      <c r="D38" s="102"/>
+      <c r="D38" s="107"/>
       <c r="E38" s="23">
         <f>IF(D37=Master!D33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F38" s="107" t="s">
-        <v>139</v>
+      <c r="F38" s="108" t="s">
+        <v>138</v>
       </c>
       <c r="G38" s="23">
         <f>IF(F38=Master!F34,4,0)</f>
@@ -6671,18 +6682,19 @@
         <f>IF(N38=Master!N34,4,0)</f>
         <v>0</v>
       </c>
-      <c r="N38" s="107" t="s">
-        <v>27</v>
+      <c r="N38" s="108" t="str">
+        <f>P37</f>
+        <v>Costa Rica</v>
       </c>
       <c r="O38" s="23">
         <f>IF(P37=Master!P33,2,0)</f>
         <v>0</v>
       </c>
-      <c r="P38" s="108"/>
+      <c r="P38" s="109"/>
       <c r="Q38" s="7"/>
       <c r="R38" s="39" t="str">
         <f>D18</f>
-        <v>Germany</v>
+        <v>Costa Rica</v>
       </c>
       <c r="S38" s="7" t="s">
         <v>21</v>
@@ -6697,7 +6709,7 @@
         <v>72</v>
       </c>
       <c r="E39" s="7"/>
-      <c r="F39" s="109"/>
+      <c r="F39" s="110"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
@@ -6705,7 +6717,7 @@
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
-      <c r="N39" s="109"/>
+      <c r="N39" s="110"/>
       <c r="O39" s="7"/>
       <c r="P39" s="35" t="s">
         <v>76</v>
@@ -6724,14 +6736,14 @@
         <v>Brasil</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="98" t="s">
+      <c r="D40" s="103" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="23">
         <f>IF(D40=Master!D36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F40" s="108"/>
+      <c r="F40" s="109"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
@@ -6739,13 +6751,13 @@
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
-      <c r="N40" s="108"/>
+      <c r="N40" s="109"/>
       <c r="O40" s="23">
         <f>IF(P40=Master!P36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P40" s="98" t="s">
-        <v>137</v>
+      <c r="P40" s="103" t="s">
+        <v>136</v>
       </c>
       <c r="Q40" s="7"/>
       <c r="R40" s="38" t="str">
@@ -6766,7 +6778,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="99"/>
+      <c r="D41" s="104"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -6778,7 +6790,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="99"/>
+      <c r="P41" s="104"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="39" t="str">
         <f>D25</f>
@@ -6846,6 +6858,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="J8:N8"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="D31:D32"/>
@@ -6862,13 +6881,6 @@
     <mergeCell ref="N38:N40"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="P40:P41"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="J8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -6879,8 +6891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB731263-BF9E-B94A-B168-4AE30BA7699C}">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6908,26 +6920,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="91"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="89"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="89" t="s">
+      <c r="J1" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="90"/>
-      <c r="L1" s="90"/>
-      <c r="M1" s="90"/>
-      <c r="N1" s="91"/>
-      <c r="P1" s="89" t="s">
+      <c r="K1" s="88"/>
+      <c r="L1" s="88"/>
+      <c r="M1" s="88"/>
+      <c r="N1" s="89"/>
+      <c r="P1" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="90"/>
-      <c r="R1" s="91"/>
+      <c r="Q1" s="88"/>
+      <c r="R1" s="89"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -7048,7 +7060,7 @@
       <c r="H5" s="35"/>
       <c r="I5" s="52"/>
       <c r="J5" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K5" s="51"/>
       <c r="L5" s="51" t="str">
@@ -7087,7 +7099,7 @@
       <c r="H6" s="35"/>
       <c r="I6" s="52"/>
       <c r="J6" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K6" s="53"/>
       <c r="L6" s="53" t="str">
@@ -7130,23 +7142,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="103" t="s">
+      <c r="B8" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="104"/>
-      <c r="D8" s="104"/>
-      <c r="E8" s="104"/>
-      <c r="F8" s="105"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="98"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="103" t="s">
+      <c r="J8" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="104"/>
-      <c r="L8" s="104"/>
-      <c r="M8" s="104"/>
-      <c r="N8" s="105"/>
+      <c r="K8" s="97"/>
+      <c r="L8" s="97"/>
+      <c r="M8" s="97"/>
+      <c r="N8" s="98"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -7209,12 +7221,12 @@
       <c r="H10" s="35"/>
       <c r="I10" s="52"/>
       <c r="J10" s="26" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="K10" s="51"/>
       <c r="L10" s="49" t="str">
         <f>Master!F8</f>
-        <v>Denmark</v>
+        <v>Australia</v>
       </c>
       <c r="M10" s="51"/>
       <c r="N10" s="34">
@@ -7240,12 +7252,12 @@
       <c r="H11" s="35"/>
       <c r="I11" s="52"/>
       <c r="J11" s="26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K11" s="51"/>
       <c r="L11" s="49" t="str">
         <f>Master!F9</f>
-        <v>France</v>
+        <v>Denmark</v>
       </c>
       <c r="M11" s="51"/>
       <c r="N11" s="34">
@@ -7278,12 +7290,12 @@
       <c r="H12" s="35"/>
       <c r="I12" s="52"/>
       <c r="J12" s="26" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="K12" s="51"/>
       <c r="L12" s="50" t="str">
         <f>Master!F10</f>
-        <v>Russia</v>
+        <v>France</v>
       </c>
       <c r="M12" s="51"/>
       <c r="N12" s="34">
@@ -7336,23 +7348,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="103" t="s">
+      <c r="B15" s="96" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="104"/>
-      <c r="D15" s="104"/>
-      <c r="E15" s="104"/>
-      <c r="F15" s="105"/>
+      <c r="C15" s="97"/>
+      <c r="D15" s="97"/>
+      <c r="E15" s="97"/>
+      <c r="F15" s="98"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="103" t="s">
+      <c r="J15" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="104"/>
-      <c r="L15" s="104"/>
-      <c r="M15" s="104"/>
-      <c r="N15" s="105"/>
+      <c r="K15" s="97"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="98"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -7383,12 +7395,12 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B17" s="26" t="s">
-        <v>136</v>
+        <v>27</v>
       </c>
       <c r="C17" s="51"/>
       <c r="D17" s="47" t="str">
         <f>Master!B14</f>
-        <v>Italy</v>
+        <v>Germany</v>
       </c>
       <c r="E17" s="51"/>
       <c r="F17" s="34">
@@ -7414,12 +7426,12 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B18" s="26" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C18" s="51"/>
       <c r="D18" s="48" t="str">
         <f>Master!B15</f>
-        <v>Germany</v>
+        <v>Costa Rica</v>
       </c>
       <c r="E18" s="51"/>
       <c r="F18" s="34">
@@ -7492,7 +7504,7 @@
       <c r="H20" s="55"/>
       <c r="I20" s="52"/>
       <c r="J20" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K20" s="53"/>
       <c r="L20" s="53" t="str">
@@ -7519,23 +7531,23 @@
       <c r="N21" s="52"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="103" t="s">
+      <c r="B22" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="104"/>
-      <c r="D22" s="104"/>
-      <c r="E22" s="104"/>
-      <c r="F22" s="105"/>
+      <c r="C22" s="97"/>
+      <c r="D22" s="97"/>
+      <c r="E22" s="97"/>
+      <c r="F22" s="98"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="103" t="s">
+      <c r="J22" s="96" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="104"/>
-      <c r="L22" s="104"/>
-      <c r="M22" s="104"/>
-      <c r="N22" s="105"/>
+      <c r="K22" s="97"/>
+      <c r="L22" s="97"/>
+      <c r="M22" s="97"/>
+      <c r="N22" s="98"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B23" s="56" t="s">
@@ -7597,7 +7609,7 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B25" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C25" s="51"/>
       <c r="D25" s="48" t="str">
@@ -7641,7 +7653,7 @@
         <v>1</v>
       </c>
       <c r="J26" s="26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K26" s="32"/>
       <c r="L26" s="32" t="str">
@@ -7669,7 +7681,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K27" s="19"/>
       <c r="L27" s="19" t="str">
@@ -7758,7 +7770,7 @@
         <v>Ecuador</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="110" t="s">
+      <c r="D31" s="111" t="s">
         <v>134</v>
       </c>
       <c r="E31" s="7"/>
@@ -7776,7 +7788,7 @@
         <v>79</v>
       </c>
       <c r="O31" s="7"/>
-      <c r="P31" s="110" t="s">
+      <c r="P31" s="111" t="s">
         <v>41</v>
       </c>
       <c r="Q31" s="7"/>
@@ -7798,12 +7810,12 @@
         <v>Iran</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="111"/>
+      <c r="D32" s="112"/>
       <c r="E32" s="23">
         <f>IF(D31=Master!D27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F32" s="112" t="s">
+      <c r="F32" s="113" t="s">
         <v>134</v>
       </c>
       <c r="G32" s="7"/>
@@ -7813,14 +7825,14 @@
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
-      <c r="N32" s="112" t="s">
+      <c r="N32" s="113" t="s">
         <v>13</v>
       </c>
       <c r="O32" s="23">
         <f>IF(P31=Master!P27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P32" s="111"/>
+      <c r="P32" s="112"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="39" t="str">
         <f>D4</f>
@@ -7839,7 +7851,7 @@
         <v>70</v>
       </c>
       <c r="E33" s="7"/>
-      <c r="F33" s="113"/>
+      <c r="F33" s="114"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
@@ -7847,7 +7859,7 @@
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
-      <c r="N33" s="113"/>
+      <c r="N33" s="114"/>
       <c r="O33" s="7"/>
       <c r="P33" s="35" t="s">
         <v>74</v>
@@ -7866,14 +7878,14 @@
         <v>Argentina</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="110" t="s">
+      <c r="D34" s="111" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="23">
         <f>IF(D34=Master!D30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F34" s="114"/>
+      <c r="F34" s="115"/>
       <c r="G34" s="23">
         <f>IF(F32=Master!F28,4,0)</f>
         <v>0</v>
@@ -7891,18 +7903,18 @@
         <f>IF(N32=Master!N28,4,0)</f>
         <v>0</v>
       </c>
-      <c r="N34" s="114"/>
+      <c r="N34" s="115"/>
       <c r="O34" s="23">
         <f>IF(P34=Master!P30,2,0)</f>
         <v>0</v>
       </c>
-      <c r="P34" s="112" t="s">
+      <c r="P34" s="113" t="s">
         <v>13</v>
       </c>
       <c r="Q34" s="7"/>
       <c r="R34" s="38" t="str">
         <f>L10</f>
-        <v>Denmark</v>
+        <v>Australia</v>
       </c>
       <c r="S34" s="7" t="s">
         <v>18</v>
@@ -7915,14 +7927,14 @@
       </c>
       <c r="B35" s="63" t="str">
         <f>L11</f>
-        <v>France</v>
+        <v>Denmark</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="111"/>
+      <c r="D35" s="112"/>
       <c r="E35" s="7"/>
       <c r="F35" s="35"/>
       <c r="G35" s="7"/>
-      <c r="H35" s="107" t="s">
+      <c r="H35" s="108" t="s">
         <v>12</v>
       </c>
       <c r="I35" s="7"/>
@@ -7930,13 +7942,13 @@
         <v>81</v>
       </c>
       <c r="K35" s="7"/>
-      <c r="L35" s="112" t="s">
+      <c r="L35" s="113" t="s">
         <v>13</v>
       </c>
       <c r="M35" s="7"/>
       <c r="N35" s="35"/>
       <c r="O35" s="7"/>
-      <c r="P35" s="114"/>
+      <c r="P35" s="115"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="39" t="str">
         <f>D11</f>
@@ -7957,7 +7969,7 @@
       <c r="E36" s="7"/>
       <c r="F36" s="35"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="109"/>
+      <c r="H36" s="110"/>
       <c r="I36" s="24">
         <f>IF(H35=Master!H31,6,0)</f>
         <v>0</v>
@@ -7969,7 +7981,7 @@
         <f>IF(L35=Master!L31,6,0)</f>
         <v>0</v>
       </c>
-      <c r="L36" s="113"/>
+      <c r="L36" s="114"/>
       <c r="M36" s="7"/>
       <c r="N36" s="35"/>
       <c r="O36" s="7"/>
@@ -7987,28 +7999,28 @@
       </c>
       <c r="B37" s="64" t="str">
         <f>D17</f>
-        <v>Italy</v>
+        <v>Germany</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="115" t="s">
-        <v>136</v>
+      <c r="D37" s="116" t="s">
+        <v>27</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="35" t="s">
         <v>78</v>
       </c>
       <c r="G37" s="7"/>
-      <c r="H37" s="108"/>
+      <c r="H37" s="109"/>
       <c r="I37" s="7"/>
       <c r="J37" s="35"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="114"/>
+      <c r="L37" s="115"/>
       <c r="M37" s="7"/>
       <c r="N37" s="35" t="s">
         <v>80</v>
       </c>
       <c r="O37" s="7"/>
-      <c r="P37" s="110" t="s">
+      <c r="P37" s="111" t="s">
         <v>14</v>
       </c>
       <c r="Q37" s="7"/>
@@ -8030,12 +8042,12 @@
         <v>Canada</v>
       </c>
       <c r="C38" s="7"/>
-      <c r="D38" s="116"/>
+      <c r="D38" s="117"/>
       <c r="E38" s="23">
         <f>IF(D37=Master!D33,2,0)</f>
         <v>0</v>
       </c>
-      <c r="F38" s="110" t="s">
+      <c r="F38" s="111" t="s">
         <v>12</v>
       </c>
       <c r="G38" s="23">
@@ -8054,18 +8066,18 @@
         <f>IF(N38=Master!N34,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N38" s="110" t="s">
+      <c r="N38" s="111" t="s">
         <v>14</v>
       </c>
       <c r="O38" s="23">
         <f>IF(P37=Master!P33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P38" s="111"/>
+      <c r="P38" s="112"/>
       <c r="Q38" s="7"/>
       <c r="R38" s="39" t="str">
         <f>D18</f>
-        <v>Germany</v>
+        <v>Costa Rica</v>
       </c>
       <c r="S38" s="7" t="s">
         <v>21</v>
@@ -8080,7 +8092,7 @@
         <v>72</v>
       </c>
       <c r="E39" s="7"/>
-      <c r="F39" s="117"/>
+      <c r="F39" s="118"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
@@ -8088,7 +8100,7 @@
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
-      <c r="N39" s="117"/>
+      <c r="N39" s="118"/>
       <c r="O39" s="7"/>
       <c r="P39" s="35" t="s">
         <v>76</v>
@@ -8107,14 +8119,14 @@
         <v>Brasil</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="98" t="s">
+      <c r="D40" s="103" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="23">
         <f>IF(D40=Master!D36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F40" s="111"/>
+      <c r="F40" s="112"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
@@ -8122,13 +8134,13 @@
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
-      <c r="N40" s="111"/>
+      <c r="N40" s="112"/>
       <c r="O40" s="23">
         <f>IF(P40=Master!P36,2,0)</f>
         <v>0</v>
       </c>
-      <c r="P40" s="112" t="s">
-        <v>140</v>
+      <c r="P40" s="113" t="s">
+        <v>139</v>
       </c>
       <c r="Q40" s="7"/>
       <c r="R40" s="38" t="str">
@@ -8149,7 +8161,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="99"/>
+      <c r="D41" s="104"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -8161,7 +8173,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="114"/>
+      <c r="P41" s="115"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="39" t="str">
         <f>D25</f>
@@ -8229,6 +8241,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="J8:N8"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="D31:D32"/>
@@ -8245,13 +8264,6 @@
     <mergeCell ref="N38:N40"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="P40:P41"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="J8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -8262,8 +8274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61C1E5FA-F91B-4A41-A4C1-97D69E012813}">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8291,26 +8303,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="91"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="89"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="89" t="s">
+      <c r="J1" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="90"/>
-      <c r="L1" s="90"/>
-      <c r="M1" s="90"/>
-      <c r="N1" s="91"/>
-      <c r="P1" s="89" t="s">
+      <c r="K1" s="88"/>
+      <c r="L1" s="88"/>
+      <c r="M1" s="88"/>
+      <c r="N1" s="89"/>
+      <c r="P1" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="90"/>
-      <c r="R1" s="91"/>
+      <c r="Q1" s="88"/>
+      <c r="R1" s="89"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -8431,7 +8443,7 @@
       <c r="H5" s="35"/>
       <c r="I5" s="52"/>
       <c r="J5" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K5" s="51"/>
       <c r="L5" s="50" t="str">
@@ -8470,7 +8482,7 @@
       <c r="H6" s="35"/>
       <c r="I6" s="52"/>
       <c r="J6" s="27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K6" s="53"/>
       <c r="L6" s="60" t="str">
@@ -8513,23 +8525,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="103" t="s">
+      <c r="B8" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="104"/>
-      <c r="D8" s="104"/>
-      <c r="E8" s="104"/>
-      <c r="F8" s="105"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="98"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="103" t="s">
+      <c r="J8" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="104"/>
-      <c r="L8" s="104"/>
-      <c r="M8" s="104"/>
-      <c r="N8" s="105"/>
+      <c r="K8" s="97"/>
+      <c r="L8" s="97"/>
+      <c r="M8" s="97"/>
+      <c r="N8" s="98"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -8592,12 +8604,12 @@
       <c r="H10" s="35"/>
       <c r="I10" s="52"/>
       <c r="J10" s="26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K10" s="51"/>
       <c r="L10" s="47" t="str">
         <f>Master!F8</f>
-        <v>Denmark</v>
+        <v>Australia</v>
       </c>
       <c r="M10" s="51"/>
       <c r="N10" s="34">
@@ -8628,7 +8640,7 @@
       <c r="K11" s="51"/>
       <c r="L11" s="51" t="str">
         <f>Master!F9</f>
-        <v>France</v>
+        <v>Denmark</v>
       </c>
       <c r="M11" s="51"/>
       <c r="N11" s="34">
@@ -8661,12 +8673,12 @@
       <c r="H12" s="35"/>
       <c r="I12" s="52"/>
       <c r="J12" s="26" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="K12" s="51"/>
       <c r="L12" s="50" t="str">
         <f>Master!F10</f>
-        <v>Russia</v>
+        <v>France</v>
       </c>
       <c r="M12" s="51"/>
       <c r="N12" s="34">
@@ -8692,7 +8704,7 @@
       <c r="H13" s="35"/>
       <c r="I13" s="52"/>
       <c r="J13" s="27" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="K13" s="53"/>
       <c r="L13" s="53" t="str">
@@ -8719,23 +8731,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="103" t="s">
+      <c r="B15" s="96" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="104"/>
-      <c r="D15" s="104"/>
-      <c r="E15" s="104"/>
-      <c r="F15" s="105"/>
+      <c r="C15" s="97"/>
+      <c r="D15" s="97"/>
+      <c r="E15" s="97"/>
+      <c r="F15" s="98"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="103" t="s">
+      <c r="J15" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="104"/>
-      <c r="L15" s="104"/>
-      <c r="M15" s="104"/>
-      <c r="N15" s="105"/>
+      <c r="K15" s="97"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="98"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -8766,12 +8778,12 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B17" s="26" t="s">
-        <v>136</v>
+        <v>27</v>
       </c>
       <c r="C17" s="51"/>
       <c r="D17" s="47" t="str">
         <f>Master!B14</f>
-        <v>Italy</v>
+        <v>Germany</v>
       </c>
       <c r="E17" s="51"/>
       <c r="F17" s="34">
@@ -8779,7 +8791,9 @@
         <v>3</v>
       </c>
       <c r="G17" s="52"/>
-      <c r="H17" s="35"/>
+      <c r="H17" s="35" t="s">
+        <v>148</v>
+      </c>
       <c r="I17" s="52"/>
       <c r="J17" s="26" t="s">
         <v>14</v>
@@ -8797,12 +8811,12 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B18" s="26" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C18" s="51"/>
       <c r="D18" s="48" t="str">
         <f>Master!B15</f>
-        <v>Germany</v>
+        <v>Costa Rica</v>
       </c>
       <c r="E18" s="51"/>
       <c r="F18" s="34">
@@ -8810,7 +8824,9 @@
         <v>2</v>
       </c>
       <c r="G18" s="52"/>
-      <c r="H18" s="35"/>
+      <c r="H18" s="35" t="s">
+        <v>149</v>
+      </c>
       <c r="I18" s="52"/>
       <c r="J18" s="26" t="s">
         <v>46</v>
@@ -8844,7 +8860,7 @@
       <c r="H19" s="35"/>
       <c r="I19" s="59"/>
       <c r="J19" s="26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K19" s="51"/>
       <c r="L19" s="51" t="str">
@@ -8902,23 +8918,23 @@
       <c r="N21" s="52"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="103" t="s">
+      <c r="B22" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="104"/>
-      <c r="D22" s="104"/>
-      <c r="E22" s="104"/>
-      <c r="F22" s="105"/>
+      <c r="C22" s="97"/>
+      <c r="D22" s="97"/>
+      <c r="E22" s="97"/>
+      <c r="F22" s="98"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="103" t="s">
+      <c r="J22" s="96" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="104"/>
-      <c r="L22" s="104"/>
-      <c r="M22" s="104"/>
-      <c r="N22" s="105"/>
+      <c r="K22" s="97"/>
+      <c r="L22" s="97"/>
+      <c r="M22" s="97"/>
+      <c r="N22" s="98"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B23" s="56" t="s">
@@ -8979,7 +8995,7 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B25" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C25" s="51"/>
       <c r="D25" s="48" t="str">
@@ -8995,7 +9011,7 @@
       <c r="H25" s="52"/>
       <c r="I25" s="52"/>
       <c r="J25" s="26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K25" s="51"/>
       <c r="L25" s="51" t="str">
@@ -9050,7 +9066,7 @@
         <v>1</v>
       </c>
       <c r="J27" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K27" s="19"/>
       <c r="L27" s="19" t="str">
@@ -9139,7 +9155,7 @@
         <v>Ecuador</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="107" t="s">
+      <c r="D31" s="108" t="s">
         <v>45</v>
       </c>
       <c r="E31" s="7"/>
@@ -9157,7 +9173,7 @@
         <v>79</v>
       </c>
       <c r="O31" s="7"/>
-      <c r="P31" s="110" t="s">
+      <c r="P31" s="111" t="s">
         <v>41</v>
       </c>
       <c r="Q31" s="7"/>
@@ -9179,12 +9195,12 @@
         <v>Iran</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="108"/>
+      <c r="D32" s="109"/>
       <c r="E32" s="23">
         <f>IF(D31=Master!D27,2,0)</f>
         <v>0</v>
       </c>
-      <c r="F32" s="107" t="s">
+      <c r="F32" s="108" t="s">
         <v>45</v>
       </c>
       <c r="G32" s="7"/>
@@ -9194,14 +9210,15 @@
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
-      <c r="N32" s="110" t="s">
-        <v>34</v>
+      <c r="N32" s="111" t="str">
+        <f>P34</f>
+        <v>Australia</v>
       </c>
       <c r="O32" s="23">
         <f>IF(P31=Master!P27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P32" s="111"/>
+      <c r="P32" s="112"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="39" t="str">
         <f>D4</f>
@@ -9220,7 +9237,7 @@
         <v>70</v>
       </c>
       <c r="E33" s="7"/>
-      <c r="F33" s="109"/>
+      <c r="F33" s="110"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
@@ -9228,7 +9245,7 @@
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
-      <c r="N33" s="117"/>
+      <c r="N33" s="118"/>
       <c r="O33" s="7"/>
       <c r="P33" s="35" t="s">
         <v>74</v>
@@ -9247,14 +9264,14 @@
         <v>Argentina</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="110" t="s">
+      <c r="D34" s="111" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="23">
         <f>IF(D34=Master!D30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F34" s="108"/>
+      <c r="F34" s="109"/>
       <c r="G34" s="23">
         <f>IF(F32=Master!F28,4,0)</f>
         <v>0</v>
@@ -9272,18 +9289,18 @@
         <f>IF(N32=Master!N28,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N34" s="111"/>
+      <c r="N34" s="112"/>
       <c r="O34" s="23">
         <f>IF(P34=Master!P30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P34" s="110" t="s">
-        <v>34</v>
+      <c r="P34" s="111" t="s">
+        <v>35</v>
       </c>
       <c r="Q34" s="7"/>
       <c r="R34" s="38" t="str">
         <f>L10</f>
-        <v>Denmark</v>
+        <v>Australia</v>
       </c>
       <c r="S34" s="7" t="s">
         <v>18</v>
@@ -9296,28 +9313,30 @@
       </c>
       <c r="B35" s="63" t="str">
         <f>L11</f>
-        <v>France</v>
+        <v>Denmark</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="111"/>
+      <c r="D35" s="112"/>
       <c r="E35" s="7"/>
       <c r="F35" s="35"/>
       <c r="G35" s="7"/>
-      <c r="H35" s="107" t="s">
-        <v>136</v>
+      <c r="H35" s="108" t="str">
+        <f>F38</f>
+        <v>Germany</v>
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="35" t="s">
         <v>81</v>
       </c>
       <c r="K35" s="7"/>
-      <c r="L35" s="107" t="s">
-        <v>34</v>
+      <c r="L35" s="108" t="str">
+        <f>N38</f>
+        <v>Ghana</v>
       </c>
       <c r="M35" s="7"/>
       <c r="N35" s="35"/>
       <c r="O35" s="7"/>
-      <c r="P35" s="111"/>
+      <c r="P35" s="112"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="39" t="str">
         <f>D11</f>
@@ -9338,19 +9357,20 @@
       <c r="E36" s="7"/>
       <c r="F36" s="35"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="109"/>
+      <c r="H36" s="110"/>
       <c r="I36" s="24">
         <f>IF(H35=Master!H31,6,0)</f>
         <v>0</v>
       </c>
-      <c r="J36" s="68" t="s">
-        <v>136</v>
+      <c r="J36" s="68" t="str">
+        <f>H35</f>
+        <v>Germany</v>
       </c>
       <c r="K36" s="25">
         <f>IF(L35=Master!L31,6,0)</f>
         <v>0</v>
       </c>
-      <c r="L36" s="109"/>
+      <c r="L36" s="110"/>
       <c r="M36" s="7"/>
       <c r="N36" s="35"/>
       <c r="O36" s="7"/>
@@ -9368,28 +9388,28 @@
       </c>
       <c r="B37" s="64" t="str">
         <f>D17</f>
-        <v>Italy</v>
+        <v>Germany</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="118" t="s">
-        <v>136</v>
+      <c r="D37" s="119" t="s">
+        <v>27</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="35" t="s">
         <v>78</v>
       </c>
       <c r="G37" s="7"/>
-      <c r="H37" s="108"/>
+      <c r="H37" s="109"/>
       <c r="I37" s="7"/>
       <c r="J37" s="35"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="108"/>
+      <c r="L37" s="109"/>
       <c r="M37" s="7"/>
       <c r="N37" s="35" t="s">
         <v>80</v>
       </c>
       <c r="O37" s="7"/>
-      <c r="P37" s="110" t="s">
+      <c r="P37" s="111" t="s">
         <v>14</v>
       </c>
       <c r="Q37" s="7"/>
@@ -9411,13 +9431,14 @@
         <v>Canada</v>
       </c>
       <c r="C38" s="7"/>
-      <c r="D38" s="119"/>
+      <c r="D38" s="120"/>
       <c r="E38" s="23">
         <f>IF(D37=Master!D33,2,0)</f>
         <v>0</v>
       </c>
-      <c r="F38" s="107" t="s">
-        <v>136</v>
+      <c r="F38" s="108" t="str">
+        <f>D37</f>
+        <v>Germany</v>
       </c>
       <c r="G38" s="23">
         <f>IF(F38=Master!F34,4,0)</f>
@@ -9435,18 +9456,18 @@
         <f>IF(N38=Master!N34,4,0)</f>
         <v>0</v>
       </c>
-      <c r="N38" s="107" t="s">
-        <v>140</v>
+      <c r="N38" s="108" t="s">
+        <v>139</v>
       </c>
       <c r="O38" s="23">
         <f>IF(P37=Master!P33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P38" s="111"/>
+      <c r="P38" s="112"/>
       <c r="Q38" s="7"/>
       <c r="R38" s="39" t="str">
         <f>D18</f>
-        <v>Germany</v>
+        <v>Costa Rica</v>
       </c>
       <c r="S38" s="7" t="s">
         <v>21</v>
@@ -9461,7 +9482,7 @@
         <v>72</v>
       </c>
       <c r="E39" s="7"/>
-      <c r="F39" s="109"/>
+      <c r="F39" s="110"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
@@ -9469,7 +9490,7 @@
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
-      <c r="N39" s="109"/>
+      <c r="N39" s="110"/>
       <c r="O39" s="7"/>
       <c r="P39" s="35" t="s">
         <v>76</v>
@@ -9488,14 +9509,14 @@
         <v>Brasil</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="110" t="s">
+      <c r="D40" s="111" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="23">
         <f>IF(D40=Master!D36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F40" s="108"/>
+      <c r="F40" s="109"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
@@ -9503,13 +9524,13 @@
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
-      <c r="N40" s="108"/>
+      <c r="N40" s="109"/>
       <c r="O40" s="23">
         <f>IF(P40=Master!P36,2,0)</f>
         <v>0</v>
       </c>
-      <c r="P40" s="107" t="s">
-        <v>140</v>
+      <c r="P40" s="108" t="s">
+        <v>139</v>
       </c>
       <c r="Q40" s="7"/>
       <c r="R40" s="38" t="str">
@@ -9530,7 +9551,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="111"/>
+      <c r="D41" s="112"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -9542,7 +9563,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="108"/>
+      <c r="P41" s="109"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="39" t="str">
         <f>D25</f>
@@ -9610,6 +9631,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="J8:N8"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="D31:D32"/>
@@ -9626,13 +9654,6 @@
     <mergeCell ref="N38:N40"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="P40:P41"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="J8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -9672,10 +9693,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="120" t="s">
+      <c r="B5" s="121" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="121"/>
+      <c r="C5" s="122"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" s="47"/>
@@ -9750,26 +9771,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="91"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="89"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="89" t="s">
+      <c r="J1" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="90"/>
-      <c r="L1" s="90"/>
-      <c r="M1" s="90"/>
-      <c r="N1" s="91"/>
-      <c r="P1" s="89" t="s">
+      <c r="K1" s="88"/>
+      <c r="L1" s="88"/>
+      <c r="M1" s="88"/>
+      <c r="N1" s="89"/>
+      <c r="P1" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="90"/>
-      <c r="R1" s="91"/>
+      <c r="Q1" s="88"/>
+      <c r="R1" s="89"/>
       <c r="W1" s="1" t="s">
         <v>92</v>
       </c>
@@ -10077,23 +10098,23 @@
       </c>
     </row>
     <row r="8" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B8" s="103" t="s">
+      <c r="B8" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="104"/>
-      <c r="D8" s="104"/>
-      <c r="E8" s="104"/>
-      <c r="F8" s="105"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="98"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="103" t="s">
+      <c r="J8" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="104"/>
-      <c r="L8" s="104"/>
-      <c r="M8" s="104"/>
-      <c r="N8" s="105"/>
+      <c r="K8" s="97"/>
+      <c r="L8" s="97"/>
+      <c r="M8" s="97"/>
+      <c r="N8" s="98"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -10161,7 +10182,7 @@
       <c r="K10" s="51"/>
       <c r="L10" s="51" t="str">
         <f>Master!F8</f>
-        <v>Denmark</v>
+        <v>Australia</v>
       </c>
       <c r="M10" s="51"/>
       <c r="N10" s="34">
@@ -10216,7 +10237,7 @@
       <c r="K11" s="51"/>
       <c r="L11" s="51" t="str">
         <f>Master!F9</f>
-        <v>France</v>
+        <v>Denmark</v>
       </c>
       <c r="M11" s="51"/>
       <c r="N11" s="34">
@@ -10278,7 +10299,7 @@
       <c r="K12" s="51"/>
       <c r="L12" s="51" t="str">
         <f>Master!F10</f>
-        <v>Russia</v>
+        <v>France</v>
       </c>
       <c r="M12" s="51"/>
       <c r="N12" s="34">
@@ -10381,23 +10402,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B15" s="103" t="s">
+      <c r="B15" s="96" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="104"/>
-      <c r="D15" s="104"/>
-      <c r="E15" s="104"/>
-      <c r="F15" s="105"/>
+      <c r="C15" s="97"/>
+      <c r="D15" s="97"/>
+      <c r="E15" s="97"/>
+      <c r="F15" s="98"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="103" t="s">
+      <c r="J15" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="104"/>
-      <c r="L15" s="104"/>
-      <c r="M15" s="104"/>
-      <c r="N15" s="105"/>
+      <c r="K15" s="97"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="98"/>
     </row>
     <row r="16" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -10433,7 +10454,7 @@
       <c r="C17" s="51"/>
       <c r="D17" s="51" t="str">
         <f>Master!B14</f>
-        <v>Italy</v>
+        <v>Germany</v>
       </c>
       <c r="E17" s="51"/>
       <c r="F17" s="34">
@@ -10488,7 +10509,7 @@
       <c r="C18" s="51"/>
       <c r="D18" s="51" t="str">
         <f>Master!B15</f>
-        <v>Germany</v>
+        <v>Costa Rica</v>
       </c>
       <c r="E18" s="51"/>
       <c r="F18" s="34">
@@ -10662,23 +10683,23 @@
       <c r="N21" s="52"/>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B22" s="103" t="s">
+      <c r="B22" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="104"/>
-      <c r="D22" s="104"/>
-      <c r="E22" s="104"/>
-      <c r="F22" s="105"/>
+      <c r="C22" s="97"/>
+      <c r="D22" s="97"/>
+      <c r="E22" s="97"/>
+      <c r="F22" s="98"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="103" t="s">
+      <c r="J22" s="96" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="104"/>
-      <c r="L22" s="104"/>
-      <c r="M22" s="104"/>
-      <c r="N22" s="105"/>
+      <c r="K22" s="97"/>
+      <c r="L22" s="97"/>
+      <c r="M22" s="97"/>
+      <c r="N22" s="98"/>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B23" s="56" t="s">
@@ -10996,7 +11017,7 @@
         <v>8</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="122" t="s">
+      <c r="D31" s="123" t="s">
         <v>8</v>
       </c>
       <c r="E31" s="7"/>
@@ -11014,7 +11035,7 @@
         <v>79</v>
       </c>
       <c r="O31" s="7"/>
-      <c r="P31" s="122" t="s">
+      <c r="P31" s="123" t="s">
         <v>31</v>
       </c>
       <c r="Q31" s="7"/>
@@ -11034,12 +11055,12 @@
         <v>24</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="123"/>
+      <c r="D32" s="124"/>
       <c r="E32" s="23">
         <f>IF(D31=Master!D27,2,0)</f>
         <v>0</v>
       </c>
-      <c r="F32" s="122" t="s">
+      <c r="F32" s="123" t="s">
         <v>8</v>
       </c>
       <c r="G32" s="7"/>
@@ -11049,14 +11070,14 @@
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
-      <c r="N32" s="122" t="s">
+      <c r="N32" s="123" t="s">
         <v>47</v>
       </c>
       <c r="O32" s="23">
         <f>IF(P31=Master!P27,2,0)</f>
         <v>0</v>
       </c>
-      <c r="P32" s="123"/>
+      <c r="P32" s="124"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="42" t="s">
         <v>31</v>
@@ -11074,7 +11095,7 @@
         <v>70</v>
       </c>
       <c r="E33" s="7"/>
-      <c r="F33" s="124"/>
+      <c r="F33" s="125"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
@@ -11082,7 +11103,7 @@
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
-      <c r="N33" s="124"/>
+      <c r="N33" s="125"/>
       <c r="O33" s="7"/>
       <c r="P33" s="35" t="s">
         <v>74</v>
@@ -11100,14 +11121,14 @@
         <v>10</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="122" t="s">
+      <c r="D34" s="123" t="s">
         <v>10</v>
       </c>
       <c r="E34" s="23">
         <f>IF(D34=Master!D30,2,0)</f>
         <v>0</v>
       </c>
-      <c r="F34" s="123"/>
+      <c r="F34" s="124"/>
       <c r="G34" s="23">
         <f>IF(F32=Master!F28,4,0)</f>
         <v>0</v>
@@ -11125,12 +11146,12 @@
         <f>IF(N32=Master!N28,4,0)</f>
         <v>0</v>
       </c>
-      <c r="N34" s="123"/>
+      <c r="N34" s="124"/>
       <c r="O34" s="23">
         <f>IF(P34=Master!P30,2,0)</f>
         <v>0</v>
       </c>
-      <c r="P34" s="122" t="s">
+      <c r="P34" s="123" t="s">
         <v>47</v>
       </c>
       <c r="Q34" s="7"/>
@@ -11150,11 +11171,11 @@
         <v>25</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="123"/>
+      <c r="D35" s="124"/>
       <c r="E35" s="7"/>
       <c r="F35" s="35"/>
       <c r="G35" s="7"/>
-      <c r="H35" s="122" t="s">
+      <c r="H35" s="123" t="s">
         <v>14</v>
       </c>
       <c r="I35" s="7"/>
@@ -11162,13 +11183,13 @@
         <v>81</v>
       </c>
       <c r="K35" s="7"/>
-      <c r="L35" s="122" t="s">
+      <c r="L35" s="123" t="s">
         <v>47</v>
       </c>
       <c r="M35" s="7"/>
       <c r="N35" s="35"/>
       <c r="O35" s="7"/>
-      <c r="P35" s="123"/>
+      <c r="P35" s="124"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="42" t="s">
         <v>34</v>
@@ -11188,7 +11209,7 @@
       <c r="E36" s="7"/>
       <c r="F36" s="35"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="124"/>
+      <c r="H36" s="125"/>
       <c r="I36" s="24">
         <f>IF(H35=Master!H31,6,0)</f>
         <v>0</v>
@@ -11200,7 +11221,7 @@
         <f>IF(L35=Master!L31,6,0)</f>
         <v>0</v>
       </c>
-      <c r="L36" s="124"/>
+      <c r="L36" s="125"/>
       <c r="M36" s="7"/>
       <c r="N36" s="35"/>
       <c r="O36" s="7"/>
@@ -11220,7 +11241,7 @@
         <v>12</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="125" t="s">
+      <c r="D37" s="126" t="s">
         <v>12</v>
       </c>
       <c r="E37" s="7"/>
@@ -11228,17 +11249,17 @@
         <v>78</v>
       </c>
       <c r="G37" s="7"/>
-      <c r="H37" s="123"/>
+      <c r="H37" s="124"/>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="123"/>
+      <c r="L37" s="124"/>
       <c r="M37" s="7"/>
       <c r="N37" s="35" t="s">
         <v>80</v>
       </c>
       <c r="O37" s="7"/>
-      <c r="P37" s="122" t="s">
+      <c r="P37" s="123" t="s">
         <v>49</v>
       </c>
       <c r="Q37" s="7"/>
@@ -11258,12 +11279,12 @@
         <v>13</v>
       </c>
       <c r="C38" s="7"/>
-      <c r="D38" s="126"/>
+      <c r="D38" s="127"/>
       <c r="E38" s="23">
         <f>IF(D37=Master!D33,2,0)</f>
         <v>0</v>
       </c>
-      <c r="F38" s="127" t="s">
+      <c r="F38" s="128" t="s">
         <v>14</v>
       </c>
       <c r="G38" s="23">
@@ -11282,14 +11303,14 @@
         <f>IF(N38=Master!N34,4,0)</f>
         <v>0</v>
       </c>
-      <c r="N38" s="122" t="s">
+      <c r="N38" s="123" t="s">
         <v>41</v>
       </c>
       <c r="O38" s="23">
         <f>IF(P37=Master!P33,2,0)</f>
         <v>0</v>
       </c>
-      <c r="P38" s="123"/>
+      <c r="P38" s="124"/>
       <c r="Q38" s="7"/>
       <c r="R38" s="42" t="s">
         <v>37</v>
@@ -11307,7 +11328,7 @@
         <v>72</v>
       </c>
       <c r="E39" s="7"/>
-      <c r="F39" s="128"/>
+      <c r="F39" s="129"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
@@ -11315,7 +11336,7 @@
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
-      <c r="N39" s="124"/>
+      <c r="N39" s="125"/>
       <c r="O39" s="7"/>
       <c r="P39" s="35" t="s">
         <v>76</v>
@@ -11333,14 +11354,14 @@
         <v>14</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="122" t="s">
+      <c r="D40" s="123" t="s">
         <v>14</v>
       </c>
       <c r="E40" s="23">
         <f>IF(D40=Master!D36,2,0)</f>
         <v>0</v>
       </c>
-      <c r="F40" s="129"/>
+      <c r="F40" s="130"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
@@ -11348,12 +11369,12 @@
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
-      <c r="N40" s="123"/>
+      <c r="N40" s="124"/>
       <c r="O40" s="23">
         <f>IF(P40=Master!P36,2,0)</f>
         <v>0</v>
       </c>
-      <c r="P40" s="122" t="s">
+      <c r="P40" s="123" t="s">
         <v>41</v>
       </c>
       <c r="Q40" s="7"/>
@@ -11373,7 +11394,7 @@
         <v>52</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="123"/>
+      <c r="D41" s="124"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -11385,7 +11406,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="123"/>
+      <c r="P41" s="124"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="42" t="s">
         <v>41</v>
@@ -11452,13 +11473,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="J8:N8"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="D31:D32"/>
@@ -11475,6 +11489,13 @@
     <mergeCell ref="N38:N40"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="P40:P41"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="J8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -11768,7 +11789,7 @@
       <c r="B11" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="C11" s="130" t="s">
+      <c r="C11" s="131" t="s">
         <v>110</v>
       </c>
       <c r="D11" s="69"/>
@@ -11790,7 +11811,7 @@
       <c r="B12" s="48" t="s">
         <v>115</v>
       </c>
-      <c r="C12" s="130"/>
+      <c r="C12" s="131"/>
       <c r="D12" s="69"/>
       <c r="E12" s="69"/>
       <c r="F12" s="69"/>
@@ -11908,7 +11929,7 @@
       <c r="B17" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="C17" s="130" t="s">
+      <c r="C17" s="131" t="s">
         <v>110</v>
       </c>
       <c r="D17" s="69"/>
@@ -11930,7 +11951,7 @@
       <c r="B18" s="49" t="s">
         <v>116</v>
       </c>
-      <c r="C18" s="130"/>
+      <c r="C18" s="131"/>
       <c r="D18" s="69"/>
       <c r="E18" s="69"/>
       <c r="F18" s="69"/>

</xml_diff>

<commit_message>
leaderboard func updated to incorporate scenario 11.  also re-ddi all of leaderboard calc func code
</commit_message>
<xml_diff>
--- a/excel docs/java testing-audit info.xlsx
+++ b/excel docs/java testing-audit info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joecollins/Desktop/documents/personal-projects/world-cup-heroku/excel docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D55E277-19D1-2348-AA45-2E7DD05302F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D9D15B-310D-CC4F-9F36-0C18377C6F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="22780" windowHeight="18680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26200" windowHeight="15800" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -1478,6 +1478,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1488,15 +1497,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1505,6 +1505,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1516,30 +1540,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1931,11 +1931,11 @@
       <c r="F1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="87" t="s">
+      <c r="J1" s="90" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="88"/>
-      <c r="L1" s="89"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="92"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B2" s="14" t="s">
@@ -2255,7 +2255,7 @@
         <v>Ecuador</v>
       </c>
       <c r="C27" s="7"/>
-      <c r="D27" s="90" t="s">
+      <c r="D27" s="87" t="s">
         <v>134</v>
       </c>
       <c r="E27" s="7"/>
@@ -2269,7 +2269,7 @@
       <c r="M27" s="7"/>
       <c r="N27" s="7"/>
       <c r="O27" s="7"/>
-      <c r="P27" s="90" t="s">
+      <c r="P27" s="87" t="s">
         <v>41</v>
       </c>
       <c r="Q27" s="7"/>
@@ -2291,9 +2291,9 @@
         <v>Iran</v>
       </c>
       <c r="C28" s="7"/>
-      <c r="D28" s="91"/>
+      <c r="D28" s="89"/>
       <c r="E28" s="7"/>
-      <c r="F28" s="90" t="s">
+      <c r="F28" s="87" t="s">
         <v>25</v>
       </c>
       <c r="G28" s="7"/>
@@ -2303,12 +2303,12 @@
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
       <c r="M28" s="7"/>
-      <c r="N28" s="90" t="str">
+      <c r="N28" s="87" t="str">
         <f>P30</f>
         <v>Australia</v>
       </c>
       <c r="O28" s="7"/>
-      <c r="P28" s="91"/>
+      <c r="P28" s="89"/>
       <c r="Q28" s="7"/>
       <c r="R28" s="15" t="str">
         <f>B3</f>
@@ -2325,7 +2325,7 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
-      <c r="F29" s="92"/>
+      <c r="F29" s="88"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
@@ -2333,7 +2333,7 @@
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
-      <c r="N29" s="92"/>
+      <c r="N29" s="88"/>
       <c r="O29" s="7"/>
       <c r="P29" s="7"/>
       <c r="Q29" s="7"/>
@@ -2350,11 +2350,11 @@
         <v>Argentina</v>
       </c>
       <c r="C30" s="7"/>
-      <c r="D30" s="90" t="s">
+      <c r="D30" s="87" t="s">
         <v>25</v>
       </c>
       <c r="E30" s="7"/>
-      <c r="F30" s="91"/>
+      <c r="F30" s="89"/>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
@@ -2362,9 +2362,9 @@
       <c r="K30" s="7"/>
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
-      <c r="N30" s="91"/>
+      <c r="N30" s="89"/>
       <c r="O30" s="7"/>
-      <c r="P30" s="90" t="str">
+      <c r="P30" s="87" t="str">
         <f>R30</f>
         <v>Australia</v>
       </c>
@@ -2387,7 +2387,7 @@
         <v>Denmark</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="91"/>
+      <c r="D31" s="89"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
@@ -2404,7 +2404,7 @@
       <c r="M31" s="7"/>
       <c r="N31" s="7"/>
       <c r="O31" s="7"/>
-      <c r="P31" s="91"/>
+      <c r="P31" s="89"/>
       <c r="Q31" s="7"/>
       <c r="R31" s="15" t="str">
         <f>B9</f>
@@ -2448,7 +2448,7 @@
         <v>Germany</v>
       </c>
       <c r="C33" s="7"/>
-      <c r="D33" s="90" t="s">
+      <c r="D33" s="87" t="s">
         <v>138</v>
       </c>
       <c r="E33" s="7"/>
@@ -2462,7 +2462,7 @@
       <c r="M33" s="7"/>
       <c r="N33" s="7"/>
       <c r="O33" s="7"/>
-      <c r="P33" s="90" t="s">
+      <c r="P33" s="87" t="s">
         <v>14</v>
       </c>
       <c r="Q33" s="7"/>
@@ -2484,9 +2484,9 @@
         <v>Canada</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="91"/>
+      <c r="D34" s="89"/>
       <c r="E34" s="7"/>
-      <c r="F34" s="90" t="s">
+      <c r="F34" s="87" t="s">
         <v>12</v>
       </c>
       <c r="G34" s="7"/>
@@ -2496,11 +2496,11 @@
       <c r="K34" s="7"/>
       <c r="L34" s="7"/>
       <c r="M34" s="7"/>
-      <c r="N34" s="90" t="s">
+      <c r="N34" s="87" t="s">
         <v>14</v>
       </c>
       <c r="O34" s="7"/>
-      <c r="P34" s="91"/>
+      <c r="P34" s="89"/>
       <c r="Q34" s="7"/>
       <c r="R34" s="15" t="str">
         <f>B15</f>
@@ -2517,7 +2517,7 @@
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
-      <c r="F35" s="92"/>
+      <c r="F35" s="88"/>
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
@@ -2525,7 +2525,7 @@
       <c r="K35" s="7"/>
       <c r="L35" s="7"/>
       <c r="M35" s="7"/>
-      <c r="N35" s="92"/>
+      <c r="N35" s="88"/>
       <c r="O35" s="7"/>
       <c r="P35" s="7"/>
       <c r="Q35" s="7"/>
@@ -2542,11 +2542,11 @@
         <v>Brasil</v>
       </c>
       <c r="C36" s="7"/>
-      <c r="D36" s="90" t="s">
+      <c r="D36" s="87" t="s">
         <v>12</v>
       </c>
       <c r="E36" s="7"/>
-      <c r="F36" s="91"/>
+      <c r="F36" s="89"/>
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
       <c r="I36" s="7"/>
@@ -2554,9 +2554,9 @@
       <c r="K36" s="7"/>
       <c r="L36" s="7"/>
       <c r="M36" s="7"/>
-      <c r="N36" s="91"/>
+      <c r="N36" s="89"/>
       <c r="O36" s="7"/>
-      <c r="P36" s="90" t="s">
+      <c r="P36" s="87" t="s">
         <v>136</v>
       </c>
       <c r="Q36" s="7"/>
@@ -2578,7 +2578,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="91"/>
+      <c r="D37" s="89"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
@@ -2590,7 +2590,7 @@
       <c r="M37" s="7"/>
       <c r="N37" s="7"/>
       <c r="O37" s="7"/>
-      <c r="P37" s="91"/>
+      <c r="P37" s="89"/>
       <c r="Q37" s="7"/>
       <c r="R37" s="15" t="str">
         <f>B21</f>
@@ -2625,12 +2625,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="N28:N30"/>
-    <mergeCell ref="N34:N36"/>
-    <mergeCell ref="P27:P28"/>
-    <mergeCell ref="P30:P31"/>
-    <mergeCell ref="P33:P34"/>
-    <mergeCell ref="P36:P37"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="D27:D28"/>
     <mergeCell ref="D30:D31"/>
@@ -2640,6 +2634,12 @@
     <mergeCell ref="F34:F36"/>
     <mergeCell ref="H31:H33"/>
     <mergeCell ref="L31:L33"/>
+    <mergeCell ref="N28:N30"/>
+    <mergeCell ref="N34:N36"/>
+    <mergeCell ref="P27:P28"/>
+    <mergeCell ref="P30:P31"/>
+    <mergeCell ref="P33:P34"/>
+    <mergeCell ref="P36:P37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -2694,7 +2694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86316F4E-9A6C-492E-9EDB-018A26A821E8}">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -2726,26 +2726,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="89"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="92"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="87" t="s">
+      <c r="J1" s="90" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="88"/>
-      <c r="N1" s="89"/>
-      <c r="P1" s="87" t="s">
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="92"/>
+      <c r="P1" s="90" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="88"/>
-      <c r="R1" s="89"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="92"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -2948,23 +2948,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="96" t="s">
+      <c r="B8" s="104" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="97"/>
-      <c r="D8" s="97"/>
-      <c r="E8" s="97"/>
-      <c r="F8" s="98"/>
+      <c r="C8" s="105"/>
+      <c r="D8" s="105"/>
+      <c r="E8" s="105"/>
+      <c r="F8" s="106"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="96" t="s">
+      <c r="J8" s="104" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="97"/>
-      <c r="L8" s="97"/>
-      <c r="M8" s="97"/>
-      <c r="N8" s="98"/>
+      <c r="K8" s="105"/>
+      <c r="L8" s="105"/>
+      <c r="M8" s="105"/>
+      <c r="N8" s="106"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -3154,23 +3154,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="96" t="s">
+      <c r="B15" s="104" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="97"/>
-      <c r="D15" s="97"/>
-      <c r="E15" s="97"/>
-      <c r="F15" s="98"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="105"/>
+      <c r="E15" s="105"/>
+      <c r="F15" s="106"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="96" t="s">
+      <c r="J15" s="104" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="97"/>
-      <c r="L15" s="97"/>
-      <c r="M15" s="97"/>
-      <c r="N15" s="98"/>
+      <c r="K15" s="105"/>
+      <c r="L15" s="105"/>
+      <c r="M15" s="105"/>
+      <c r="N15" s="106"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -3291,10 +3291,10 @@
         <f t="shared" ref="N19:N20" si="5">IF(J19=L19,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Q19" s="99" t="s">
+      <c r="Q19" s="107" t="s">
         <v>82</v>
       </c>
-      <c r="R19" s="99"/>
+      <c r="R19" s="107"/>
     </row>
     <row r="20" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="27" t="s">
@@ -3349,23 +3349,23 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="96" t="s">
+      <c r="B22" s="104" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="97"/>
-      <c r="D22" s="97"/>
-      <c r="E22" s="97"/>
-      <c r="F22" s="98"/>
+      <c r="C22" s="105"/>
+      <c r="D22" s="105"/>
+      <c r="E22" s="105"/>
+      <c r="F22" s="106"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="96" t="s">
+      <c r="J22" s="104" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="97"/>
-      <c r="L22" s="97"/>
-      <c r="M22" s="97"/>
-      <c r="N22" s="98"/>
+      <c r="K22" s="105"/>
+      <c r="L22" s="105"/>
+      <c r="M22" s="105"/>
+      <c r="N22" s="106"/>
       <c r="Q22" s="49"/>
       <c r="R22" s="32" t="s">
         <v>85</v>
@@ -3596,7 +3596,7 @@
         <v>Ecuador</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="103" t="s">
+      <c r="D31" s="99" t="s">
         <v>134</v>
       </c>
       <c r="E31" s="7"/>
@@ -3614,7 +3614,7 @@
         <v>79</v>
       </c>
       <c r="O31" s="7"/>
-      <c r="P31" s="103" t="s">
+      <c r="P31" s="99" t="s">
         <v>41</v>
       </c>
       <c r="Q31" s="7"/>
@@ -3636,12 +3636,12 @@
         <v>Iran</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="104"/>
+      <c r="D32" s="100"/>
       <c r="E32" s="23">
         <f>IF(D31=Master!D27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F32" s="103" t="s">
+      <c r="F32" s="99" t="s">
         <v>25</v>
       </c>
       <c r="G32" s="7"/>
@@ -3651,7 +3651,7 @@
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
-      <c r="N32" s="103" t="str">
+      <c r="N32" s="99" t="str">
         <f>P34</f>
         <v>Australia</v>
       </c>
@@ -3659,7 +3659,7 @@
         <f>IF(P31=Master!P27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P32" s="104"/>
+      <c r="P32" s="100"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="39" t="str">
         <f>D4</f>
@@ -3678,7 +3678,7 @@
         <v>70</v>
       </c>
       <c r="E33" s="7"/>
-      <c r="F33" s="105"/>
+      <c r="F33" s="101"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
@@ -3686,7 +3686,7 @@
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
-      <c r="N33" s="105"/>
+      <c r="N33" s="101"/>
       <c r="O33" s="7"/>
       <c r="P33" s="35" t="s">
         <v>74</v>
@@ -3705,14 +3705,14 @@
         <v>Argentina</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="103" t="s">
+      <c r="D34" s="99" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="23">
         <f>IF(D34=Master!D30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F34" s="104"/>
+      <c r="F34" s="100"/>
       <c r="G34" s="23">
         <f>IF(F32=Master!F28,4,0)</f>
         <v>4</v>
@@ -3730,12 +3730,12 @@
         <f>IF(N32=Master!N28,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N34" s="104"/>
+      <c r="N34" s="100"/>
       <c r="O34" s="23">
         <f>IF(P34=Master!P30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P34" s="103" t="s">
+      <c r="P34" s="99" t="s">
         <v>35</v>
       </c>
       <c r="Q34" s="7"/>
@@ -3757,11 +3757,11 @@
         <v>Denmark</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="104"/>
+      <c r="D35" s="100"/>
       <c r="E35" s="7"/>
       <c r="F35" s="35"/>
       <c r="G35" s="7"/>
-      <c r="H35" s="103" t="s">
+      <c r="H35" s="99" t="s">
         <v>25</v>
       </c>
       <c r="I35" s="7"/>
@@ -3769,14 +3769,14 @@
         <v>81</v>
       </c>
       <c r="K35" s="7"/>
-      <c r="L35" s="103" t="str">
+      <c r="L35" s="99" t="str">
         <f>N32</f>
         <v>Australia</v>
       </c>
       <c r="M35" s="7"/>
       <c r="N35" s="35"/>
       <c r="O35" s="7"/>
-      <c r="P35" s="104"/>
+      <c r="P35" s="100"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="39" t="str">
         <f>D11</f>
@@ -3797,7 +3797,7 @@
       <c r="E36" s="7"/>
       <c r="F36" s="35"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="105"/>
+      <c r="H36" s="101"/>
       <c r="I36" s="24">
         <f>IF(H35=Master!H31,6,0)</f>
         <v>6</v>
@@ -3809,7 +3809,7 @@
         <f>IF(L35=Master!L31,6,0)</f>
         <v>6</v>
       </c>
-      <c r="L36" s="105"/>
+      <c r="L36" s="101"/>
       <c r="M36" s="7"/>
       <c r="N36" s="35"/>
       <c r="O36" s="7"/>
@@ -3830,7 +3830,7 @@
         <v>Germany</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="106" t="s">
+      <c r="D37" s="102" t="s">
         <v>138</v>
       </c>
       <c r="E37" s="7"/>
@@ -3838,17 +3838,17 @@
         <v>78</v>
       </c>
       <c r="G37" s="7"/>
-      <c r="H37" s="104"/>
+      <c r="H37" s="100"/>
       <c r="I37" s="7"/>
       <c r="J37" s="35"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="104"/>
+      <c r="L37" s="100"/>
       <c r="M37" s="7"/>
       <c r="N37" s="35" t="s">
         <v>80</v>
       </c>
       <c r="O37" s="7"/>
-      <c r="P37" s="103" t="s">
+      <c r="P37" s="99" t="s">
         <v>14</v>
       </c>
       <c r="Q37" s="7"/>
@@ -3870,12 +3870,12 @@
         <v>Canada</v>
       </c>
       <c r="C38" s="7"/>
-      <c r="D38" s="107"/>
+      <c r="D38" s="103"/>
       <c r="E38" s="23">
         <f>IF(D37=Master!D33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F38" s="100" t="s">
+      <c r="F38" s="96" t="s">
         <v>12</v>
       </c>
       <c r="G38" s="23">
@@ -3894,14 +3894,14 @@
         <f>IF(N38=Master!N34,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N38" s="103" t="s">
+      <c r="N38" s="99" t="s">
         <v>14</v>
       </c>
       <c r="O38" s="23">
         <f>IF(P37=Master!P33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P38" s="104"/>
+      <c r="P38" s="100"/>
       <c r="Q38" s="7"/>
       <c r="R38" s="39" t="str">
         <f>D18</f>
@@ -3920,7 +3920,7 @@
         <v>72</v>
       </c>
       <c r="E39" s="7"/>
-      <c r="F39" s="101"/>
+      <c r="F39" s="97"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
@@ -3928,7 +3928,7 @@
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
-      <c r="N39" s="105"/>
+      <c r="N39" s="101"/>
       <c r="O39" s="7"/>
       <c r="P39" s="35" t="s">
         <v>76</v>
@@ -3947,14 +3947,14 @@
         <v>Brasil</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="103" t="s">
+      <c r="D40" s="99" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="23">
         <f>IF(D40=Master!D36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F40" s="102"/>
+      <c r="F40" s="98"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
@@ -3962,12 +3962,12 @@
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
-      <c r="N40" s="104"/>
+      <c r="N40" s="100"/>
       <c r="O40" s="23">
         <f>IF(P40=Master!P36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P40" s="103" t="s">
+      <c r="P40" s="99" t="s">
         <v>136</v>
       </c>
       <c r="Q40" s="7"/>
@@ -3989,7 +3989,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="104"/>
+      <c r="D41" s="100"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -4001,7 +4001,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="104"/>
+      <c r="P41" s="100"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="39" t="str">
         <f>D25</f>
@@ -4069,6 +4069,16 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J22:N22"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="Q19:R19"/>
     <mergeCell ref="F38:F40"/>
     <mergeCell ref="P37:P38"/>
     <mergeCell ref="P40:P41"/>
@@ -4083,16 +4093,6 @@
     <mergeCell ref="D37:D38"/>
     <mergeCell ref="H35:H37"/>
     <mergeCell ref="L35:L37"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J22:N22"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="J8:N8"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="Q19:R19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -4103,7 +4103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69337711-055D-1241-BEB8-C726DCD4CFE4}">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
@@ -4135,26 +4135,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="89"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="92"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="87" t="s">
+      <c r="J1" s="90" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="88"/>
-      <c r="N1" s="89"/>
-      <c r="P1" s="87" t="s">
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="92"/>
+      <c r="P1" s="90" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="88"/>
-      <c r="R1" s="89"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="92"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -4357,23 +4357,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="96" t="s">
+      <c r="B8" s="104" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="97"/>
-      <c r="D8" s="97"/>
-      <c r="E8" s="97"/>
-      <c r="F8" s="98"/>
+      <c r="C8" s="105"/>
+      <c r="D8" s="105"/>
+      <c r="E8" s="105"/>
+      <c r="F8" s="106"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="96" t="s">
+      <c r="J8" s="104" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="97"/>
-      <c r="L8" s="97"/>
-      <c r="M8" s="97"/>
-      <c r="N8" s="98"/>
+      <c r="K8" s="105"/>
+      <c r="L8" s="105"/>
+      <c r="M8" s="105"/>
+      <c r="N8" s="106"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -4563,23 +4563,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="96" t="s">
+      <c r="B15" s="104" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="97"/>
-      <c r="D15" s="97"/>
-      <c r="E15" s="97"/>
-      <c r="F15" s="98"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="105"/>
+      <c r="E15" s="105"/>
+      <c r="F15" s="106"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="96" t="s">
+      <c r="J15" s="104" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="97"/>
-      <c r="L15" s="97"/>
-      <c r="M15" s="97"/>
-      <c r="N15" s="98"/>
+      <c r="K15" s="105"/>
+      <c r="L15" s="105"/>
+      <c r="M15" s="105"/>
+      <c r="N15" s="106"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -4700,10 +4700,10 @@
         <f t="shared" ref="N19:N20" si="5">IF(J19=L19,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Q19" s="99" t="s">
+      <c r="Q19" s="107" t="s">
         <v>82</v>
       </c>
-      <c r="R19" s="99"/>
+      <c r="R19" s="107"/>
     </row>
     <row r="20" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="27" t="s">
@@ -4758,23 +4758,23 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="96" t="s">
+      <c r="B22" s="104" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="97"/>
-      <c r="D22" s="97"/>
-      <c r="E22" s="97"/>
-      <c r="F22" s="98"/>
+      <c r="C22" s="105"/>
+      <c r="D22" s="105"/>
+      <c r="E22" s="105"/>
+      <c r="F22" s="106"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="96" t="s">
+      <c r="J22" s="104" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="97"/>
-      <c r="L22" s="97"/>
-      <c r="M22" s="97"/>
-      <c r="N22" s="98"/>
+      <c r="K22" s="105"/>
+      <c r="L22" s="105"/>
+      <c r="M22" s="105"/>
+      <c r="N22" s="106"/>
       <c r="Q22" s="49"/>
       <c r="R22" s="32" t="s">
         <v>85</v>
@@ -5005,7 +5005,7 @@
         <v>Ecuador</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="103" t="s">
+      <c r="D31" s="99" t="s">
         <v>134</v>
       </c>
       <c r="E31" s="7"/>
@@ -5023,7 +5023,7 @@
         <v>79</v>
       </c>
       <c r="O31" s="7"/>
-      <c r="P31" s="103" t="s">
+      <c r="P31" s="99" t="s">
         <v>41</v>
       </c>
       <c r="Q31" s="7"/>
@@ -5045,12 +5045,12 @@
         <v>Iran</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="104"/>
+      <c r="D32" s="100"/>
       <c r="E32" s="23">
         <f>IF(D31=Master!D27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F32" s="103" t="s">
+      <c r="F32" s="99" t="s">
         <v>25</v>
       </c>
       <c r="G32" s="7"/>
@@ -5060,7 +5060,7 @@
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
-      <c r="N32" s="103" t="str">
+      <c r="N32" s="99" t="str">
         <f>P34</f>
         <v>Australia</v>
       </c>
@@ -5068,7 +5068,7 @@
         <f>IF(P31=Master!P27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P32" s="104"/>
+      <c r="P32" s="100"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="81" t="str">
         <f>D4</f>
@@ -5087,7 +5087,7 @@
         <v>70</v>
       </c>
       <c r="E33" s="7"/>
-      <c r="F33" s="105"/>
+      <c r="F33" s="101"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
@@ -5095,7 +5095,7 @@
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
-      <c r="N33" s="105"/>
+      <c r="N33" s="101"/>
       <c r="O33" s="7"/>
       <c r="P33" s="35"/>
       <c r="Q33" s="7"/>
@@ -5112,14 +5112,14 @@
         <v>Argentina</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="103" t="s">
+      <c r="D34" s="99" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="23">
         <f>IF(D34=Master!D30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F34" s="104"/>
+      <c r="F34" s="100"/>
       <c r="G34" s="23">
         <f>IF(F32=Master!F28,4,0)</f>
         <v>4</v>
@@ -5137,12 +5137,12 @@
         <f>IF(N32=Master!N28,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N34" s="104"/>
+      <c r="N34" s="100"/>
       <c r="O34" s="23">
         <f>IF(P34=Master!P30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P34" s="103" t="s">
+      <c r="P34" s="99" t="s">
         <v>35</v>
       </c>
       <c r="Q34" s="7"/>
@@ -5164,11 +5164,11 @@
         <v>Denmark</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="104"/>
+      <c r="D35" s="100"/>
       <c r="E35" s="7"/>
       <c r="F35" s="35"/>
       <c r="G35" s="7"/>
-      <c r="H35" s="103" t="s">
+      <c r="H35" s="99" t="s">
         <v>25</v>
       </c>
       <c r="I35" s="7"/>
@@ -5176,14 +5176,14 @@
         <v>81</v>
       </c>
       <c r="K35" s="7"/>
-      <c r="L35" s="103" t="str">
+      <c r="L35" s="99" t="str">
         <f>N32</f>
         <v>Australia</v>
       </c>
       <c r="M35" s="7"/>
       <c r="N35" s="35"/>
       <c r="O35" s="7"/>
-      <c r="P35" s="104"/>
+      <c r="P35" s="100"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="81" t="str">
         <f>D11</f>
@@ -5204,7 +5204,7 @@
       <c r="E36" s="7"/>
       <c r="F36" s="35"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="105"/>
+      <c r="H36" s="101"/>
       <c r="I36" s="24">
         <f>IF(H35=Master!H31,6,0)</f>
         <v>6</v>
@@ -5216,7 +5216,7 @@
         <f>IF(L35=Master!L31,6,0)</f>
         <v>6</v>
       </c>
-      <c r="L36" s="105"/>
+      <c r="L36" s="101"/>
       <c r="M36" s="7"/>
       <c r="N36" s="35"/>
       <c r="O36" s="7"/>
@@ -5237,7 +5237,7 @@
         <v>Germany</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="106" t="s">
+      <c r="D37" s="102" t="s">
         <v>138</v>
       </c>
       <c r="E37" s="7"/>
@@ -5245,17 +5245,17 @@
         <v>78</v>
       </c>
       <c r="G37" s="7"/>
-      <c r="H37" s="104"/>
+      <c r="H37" s="100"/>
       <c r="I37" s="7"/>
       <c r="J37" s="35"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="104"/>
+      <c r="L37" s="100"/>
       <c r="M37" s="7"/>
       <c r="N37" s="35" t="s">
         <v>80</v>
       </c>
       <c r="O37" s="7"/>
-      <c r="P37" s="103" t="s">
+      <c r="P37" s="99" t="s">
         <v>14</v>
       </c>
       <c r="Q37" s="7"/>
@@ -5277,12 +5277,12 @@
         <v>Canada</v>
       </c>
       <c r="C38" s="7"/>
-      <c r="D38" s="107"/>
+      <c r="D38" s="103"/>
       <c r="E38" s="23">
         <f>IF(D37=Master!D33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F38" s="100" t="s">
+      <c r="F38" s="96" t="s">
         <v>12</v>
       </c>
       <c r="G38" s="23">
@@ -5301,14 +5301,14 @@
         <f>IF(N38=Master!N34,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N38" s="103" t="s">
+      <c r="N38" s="99" t="s">
         <v>14</v>
       </c>
       <c r="O38" s="23">
         <f>IF(P37=Master!P33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P38" s="104"/>
+      <c r="P38" s="100"/>
       <c r="Q38" s="7"/>
       <c r="R38" s="81" t="str">
         <f>D18</f>
@@ -5327,7 +5327,7 @@
         <v>72</v>
       </c>
       <c r="E39" s="7"/>
-      <c r="F39" s="101"/>
+      <c r="F39" s="97"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
@@ -5335,7 +5335,7 @@
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
-      <c r="N39" s="105"/>
+      <c r="N39" s="101"/>
       <c r="O39" s="7"/>
       <c r="P39" s="35" t="s">
         <v>76</v>
@@ -5354,14 +5354,14 @@
         <v>Brasil</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="103" t="s">
+      <c r="D40" s="99" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="23">
         <f>IF(D40=Master!D36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F40" s="102"/>
+      <c r="F40" s="98"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
@@ -5369,12 +5369,12 @@
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
-      <c r="N40" s="104"/>
+      <c r="N40" s="100"/>
       <c r="O40" s="23">
         <f>IF(P40=Master!P36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P40" s="103" t="s">
+      <c r="P40" s="99" t="s">
         <v>136</v>
       </c>
       <c r="Q40" s="7"/>
@@ -5396,7 +5396,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="104"/>
+      <c r="D41" s="100"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -5408,7 +5408,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="104"/>
+      <c r="P41" s="100"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="81" t="str">
         <f>D25</f>
@@ -5476,6 +5476,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="P34:P35"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="L35:L37"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="P37:P38"/>
+    <mergeCell ref="F38:F40"/>
+    <mergeCell ref="N38:N40"/>
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="J8:N8"/>
@@ -5492,14 +5500,6 @@
     <mergeCell ref="P31:P32"/>
     <mergeCell ref="F32:F34"/>
     <mergeCell ref="N32:N34"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="P34:P35"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="L35:L37"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="P37:P38"/>
-    <mergeCell ref="F38:F40"/>
-    <mergeCell ref="N38:N40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -5539,26 +5539,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="89"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="92"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="87" t="s">
+      <c r="J1" s="90" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="88"/>
-      <c r="N1" s="89"/>
-      <c r="P1" s="87" t="s">
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="92"/>
+      <c r="P1" s="90" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="88"/>
-      <c r="R1" s="89"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="92"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -5761,23 +5761,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="96" t="s">
+      <c r="B8" s="104" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="97"/>
-      <c r="D8" s="97"/>
-      <c r="E8" s="97"/>
-      <c r="F8" s="98"/>
+      <c r="C8" s="105"/>
+      <c r="D8" s="105"/>
+      <c r="E8" s="105"/>
+      <c r="F8" s="106"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="96" t="s">
+      <c r="J8" s="104" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="97"/>
-      <c r="L8" s="97"/>
-      <c r="M8" s="97"/>
-      <c r="N8" s="98"/>
+      <c r="K8" s="105"/>
+      <c r="L8" s="105"/>
+      <c r="M8" s="105"/>
+      <c r="N8" s="106"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -5967,23 +5967,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="96" t="s">
+      <c r="B15" s="104" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="97"/>
-      <c r="D15" s="97"/>
-      <c r="E15" s="97"/>
-      <c r="F15" s="98"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="105"/>
+      <c r="E15" s="105"/>
+      <c r="F15" s="106"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="96" t="s">
+      <c r="J15" s="104" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="97"/>
-      <c r="L15" s="97"/>
-      <c r="M15" s="97"/>
-      <c r="N15" s="98"/>
+      <c r="K15" s="105"/>
+      <c r="L15" s="105"/>
+      <c r="M15" s="105"/>
+      <c r="N15" s="106"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -6148,23 +6148,23 @@
       <c r="N21" s="52"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="96" t="s">
+      <c r="B22" s="104" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="97"/>
-      <c r="D22" s="97"/>
-      <c r="E22" s="97"/>
-      <c r="F22" s="98"/>
+      <c r="C22" s="105"/>
+      <c r="D22" s="105"/>
+      <c r="E22" s="105"/>
+      <c r="F22" s="106"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="96" t="s">
+      <c r="J22" s="104" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="97"/>
-      <c r="L22" s="97"/>
-      <c r="M22" s="97"/>
-      <c r="N22" s="98"/>
+      <c r="K22" s="105"/>
+      <c r="L22" s="105"/>
+      <c r="M22" s="105"/>
+      <c r="N22" s="106"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B23" s="56" t="s">
@@ -6403,7 +6403,7 @@
         <v>79</v>
       </c>
       <c r="O31" s="7"/>
-      <c r="P31" s="103" t="s">
+      <c r="P31" s="99" t="s">
         <v>41</v>
       </c>
       <c r="Q31" s="7"/>
@@ -6447,7 +6447,7 @@
         <f>IF(P31=Master!P27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P32" s="104"/>
+      <c r="P32" s="100"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="39" t="str">
         <f>D4</f>
@@ -6493,7 +6493,7 @@
         <v>Argentina</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="103" t="s">
+      <c r="D34" s="99" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="23">
@@ -6523,7 +6523,7 @@
         <f>IF(P34=Master!P30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P34" s="103" t="s">
+      <c r="P34" s="99" t="s">
         <v>35</v>
       </c>
       <c r="Q34" s="7"/>
@@ -6545,7 +6545,7 @@
         <v>Denmark</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="104"/>
+      <c r="D35" s="100"/>
       <c r="E35" s="7"/>
       <c r="F35" s="35"/>
       <c r="G35" s="7"/>
@@ -6564,7 +6564,7 @@
       <c r="M35" s="7"/>
       <c r="N35" s="35"/>
       <c r="O35" s="7"/>
-      <c r="P35" s="104"/>
+      <c r="P35" s="100"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="39" t="str">
         <f>D11</f>
@@ -6618,7 +6618,7 @@
         <v>Germany</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="106" t="s">
+      <c r="D37" s="102" t="s">
         <v>138</v>
       </c>
       <c r="E37" s="7"/>
@@ -6658,7 +6658,7 @@
         <v>Canada</v>
       </c>
       <c r="C38" s="7"/>
-      <c r="D38" s="107"/>
+      <c r="D38" s="103"/>
       <c r="E38" s="23">
         <f>IF(D37=Master!D33,2,0)</f>
         <v>2</v>
@@ -6736,7 +6736,7 @@
         <v>Brasil</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="103" t="s">
+      <c r="D40" s="99" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="23">
@@ -6756,7 +6756,7 @@
         <f>IF(P40=Master!P36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P40" s="103" t="s">
+      <c r="P40" s="99" t="s">
         <v>136</v>
       </c>
       <c r="Q40" s="7"/>
@@ -6778,7 +6778,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="104"/>
+      <c r="D41" s="100"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -6790,7 +6790,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="104"/>
+      <c r="P41" s="100"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="39" t="str">
         <f>D25</f>
@@ -6858,13 +6858,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="J8:N8"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="D31:D32"/>
@@ -6881,6 +6874,13 @@
     <mergeCell ref="N38:N40"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="P40:P41"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="J8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -6920,26 +6920,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="89"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="92"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="87" t="s">
+      <c r="J1" s="90" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="88"/>
-      <c r="N1" s="89"/>
-      <c r="P1" s="87" t="s">
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="92"/>
+      <c r="P1" s="90" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="88"/>
-      <c r="R1" s="89"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="92"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -7142,23 +7142,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="96" t="s">
+      <c r="B8" s="104" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="97"/>
-      <c r="D8" s="97"/>
-      <c r="E8" s="97"/>
-      <c r="F8" s="98"/>
+      <c r="C8" s="105"/>
+      <c r="D8" s="105"/>
+      <c r="E8" s="105"/>
+      <c r="F8" s="106"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="96" t="s">
+      <c r="J8" s="104" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="97"/>
-      <c r="L8" s="97"/>
-      <c r="M8" s="97"/>
-      <c r="N8" s="98"/>
+      <c r="K8" s="105"/>
+      <c r="L8" s="105"/>
+      <c r="M8" s="105"/>
+      <c r="N8" s="106"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -7348,23 +7348,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="96" t="s">
+      <c r="B15" s="104" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="97"/>
-      <c r="D15" s="97"/>
-      <c r="E15" s="97"/>
-      <c r="F15" s="98"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="105"/>
+      <c r="E15" s="105"/>
+      <c r="F15" s="106"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="96" t="s">
+      <c r="J15" s="104" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="97"/>
-      <c r="L15" s="97"/>
-      <c r="M15" s="97"/>
-      <c r="N15" s="98"/>
+      <c r="K15" s="105"/>
+      <c r="L15" s="105"/>
+      <c r="M15" s="105"/>
+      <c r="N15" s="106"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -7531,23 +7531,23 @@
       <c r="N21" s="52"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="96" t="s">
+      <c r="B22" s="104" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="97"/>
-      <c r="D22" s="97"/>
-      <c r="E22" s="97"/>
-      <c r="F22" s="98"/>
+      <c r="C22" s="105"/>
+      <c r="D22" s="105"/>
+      <c r="E22" s="105"/>
+      <c r="F22" s="106"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="96" t="s">
+      <c r="J22" s="104" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="97"/>
-      <c r="L22" s="97"/>
-      <c r="M22" s="97"/>
-      <c r="N22" s="98"/>
+      <c r="K22" s="105"/>
+      <c r="L22" s="105"/>
+      <c r="M22" s="105"/>
+      <c r="N22" s="106"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B23" s="56" t="s">
@@ -8119,7 +8119,7 @@
         <v>Brasil</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="103" t="s">
+      <c r="D40" s="99" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="23">
@@ -8161,7 +8161,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="104"/>
+      <c r="D41" s="100"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -8241,13 +8241,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="J8:N8"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="D31:D32"/>
@@ -8264,6 +8257,13 @@
     <mergeCell ref="N38:N40"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="P40:P41"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="J8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -8274,7 +8274,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61C1E5FA-F91B-4A41-A4C1-97D69E012813}">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
@@ -8303,26 +8303,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="89"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="92"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="87" t="s">
+      <c r="J1" s="90" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="88"/>
-      <c r="N1" s="89"/>
-      <c r="P1" s="87" t="s">
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="92"/>
+      <c r="P1" s="90" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="88"/>
-      <c r="R1" s="89"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="92"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -8525,23 +8525,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="96" t="s">
+      <c r="B8" s="104" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="97"/>
-      <c r="D8" s="97"/>
-      <c r="E8" s="97"/>
-      <c r="F8" s="98"/>
+      <c r="C8" s="105"/>
+      <c r="D8" s="105"/>
+      <c r="E8" s="105"/>
+      <c r="F8" s="106"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="96" t="s">
+      <c r="J8" s="104" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="97"/>
-      <c r="L8" s="97"/>
-      <c r="M8" s="97"/>
-      <c r="N8" s="98"/>
+      <c r="K8" s="105"/>
+      <c r="L8" s="105"/>
+      <c r="M8" s="105"/>
+      <c r="N8" s="106"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -8731,23 +8731,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="96" t="s">
+      <c r="B15" s="104" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="97"/>
-      <c r="D15" s="97"/>
-      <c r="E15" s="97"/>
-      <c r="F15" s="98"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="105"/>
+      <c r="E15" s="105"/>
+      <c r="F15" s="106"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="96" t="s">
+      <c r="J15" s="104" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="97"/>
-      <c r="L15" s="97"/>
-      <c r="M15" s="97"/>
-      <c r="N15" s="98"/>
+      <c r="K15" s="105"/>
+      <c r="L15" s="105"/>
+      <c r="M15" s="105"/>
+      <c r="N15" s="106"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -8918,23 +8918,23 @@
       <c r="N21" s="52"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="96" t="s">
+      <c r="B22" s="104" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="97"/>
-      <c r="D22" s="97"/>
-      <c r="E22" s="97"/>
-      <c r="F22" s="98"/>
+      <c r="C22" s="105"/>
+      <c r="D22" s="105"/>
+      <c r="E22" s="105"/>
+      <c r="F22" s="106"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="96" t="s">
+      <c r="J22" s="104" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="97"/>
-      <c r="L22" s="97"/>
-      <c r="M22" s="97"/>
-      <c r="N22" s="98"/>
+      <c r="K22" s="105"/>
+      <c r="L22" s="105"/>
+      <c r="M22" s="105"/>
+      <c r="N22" s="106"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B23" s="56" t="s">
@@ -9631,13 +9631,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="J8:N8"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="D31:D32"/>
@@ -9654,6 +9647,13 @@
     <mergeCell ref="N38:N40"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="P40:P41"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="J8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -9771,26 +9771,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="89"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="92"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="87" t="s">
+      <c r="J1" s="90" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="88"/>
-      <c r="N1" s="89"/>
-      <c r="P1" s="87" t="s">
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="92"/>
+      <c r="P1" s="90" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="88"/>
-      <c r="R1" s="89"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="92"/>
       <c r="W1" s="1" t="s">
         <v>92</v>
       </c>
@@ -10098,23 +10098,23 @@
       </c>
     </row>
     <row r="8" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B8" s="96" t="s">
+      <c r="B8" s="104" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="97"/>
-      <c r="D8" s="97"/>
-      <c r="E8" s="97"/>
-      <c r="F8" s="98"/>
+      <c r="C8" s="105"/>
+      <c r="D8" s="105"/>
+      <c r="E8" s="105"/>
+      <c r="F8" s="106"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="96" t="s">
+      <c r="J8" s="104" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="97"/>
-      <c r="L8" s="97"/>
-      <c r="M8" s="97"/>
-      <c r="N8" s="98"/>
+      <c r="K8" s="105"/>
+      <c r="L8" s="105"/>
+      <c r="M8" s="105"/>
+      <c r="N8" s="106"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -10402,23 +10402,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B15" s="96" t="s">
+      <c r="B15" s="104" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="97"/>
-      <c r="D15" s="97"/>
-      <c r="E15" s="97"/>
-      <c r="F15" s="98"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="105"/>
+      <c r="E15" s="105"/>
+      <c r="F15" s="106"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="96" t="s">
+      <c r="J15" s="104" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="97"/>
-      <c r="L15" s="97"/>
-      <c r="M15" s="97"/>
-      <c r="N15" s="98"/>
+      <c r="K15" s="105"/>
+      <c r="L15" s="105"/>
+      <c r="M15" s="105"/>
+      <c r="N15" s="106"/>
     </row>
     <row r="16" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -10683,23 +10683,23 @@
       <c r="N21" s="52"/>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B22" s="96" t="s">
+      <c r="B22" s="104" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="97"/>
-      <c r="D22" s="97"/>
-      <c r="E22" s="97"/>
-      <c r="F22" s="98"/>
+      <c r="C22" s="105"/>
+      <c r="D22" s="105"/>
+      <c r="E22" s="105"/>
+      <c r="F22" s="106"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="96" t="s">
+      <c r="J22" s="104" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="97"/>
-      <c r="L22" s="97"/>
-      <c r="M22" s="97"/>
-      <c r="N22" s="98"/>
+      <c r="K22" s="105"/>
+      <c r="L22" s="105"/>
+      <c r="M22" s="105"/>
+      <c r="N22" s="106"/>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B23" s="56" t="s">
@@ -11473,6 +11473,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="J8:N8"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="D31:D32"/>
@@ -11489,13 +11496,6 @@
     <mergeCell ref="N38:N40"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="P40:P41"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="J8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -11506,8 +11506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12EDD3BB-E2B5-AA49-89B4-1F42796E5997}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView zoomScale="132" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
forgot pw updates before folder re-arrangments
</commit_message>
<xml_diff>
--- a/excel docs/java testing-audit info.xlsx
+++ b/excel docs/java testing-audit info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joecollins/Desktop/documents/personal-projects/world-cup-heroku/excel docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D9D15B-310D-CC4F-9F36-0C18377C6F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E636BEB-1212-A14B-B84E-5873982E49D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26200" windowHeight="15800" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41400" yWindow="-1980" windowWidth="26200" windowHeight="15800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -1478,24 +1478,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1505,6 +1505,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1528,18 +1540,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1931,11 +1931,11 @@
       <c r="F1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="90" t="s">
+      <c r="J1" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="91"/>
-      <c r="L1" s="92"/>
+      <c r="K1" s="88"/>
+      <c r="L1" s="89"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B2" s="14" t="s">
@@ -2255,7 +2255,7 @@
         <v>Ecuador</v>
       </c>
       <c r="C27" s="7"/>
-      <c r="D27" s="87" t="s">
+      <c r="D27" s="90" t="s">
         <v>134</v>
       </c>
       <c r="E27" s="7"/>
@@ -2269,7 +2269,7 @@
       <c r="M27" s="7"/>
       <c r="N27" s="7"/>
       <c r="O27" s="7"/>
-      <c r="P27" s="87" t="s">
+      <c r="P27" s="90" t="s">
         <v>41</v>
       </c>
       <c r="Q27" s="7"/>
@@ -2291,9 +2291,9 @@
         <v>Iran</v>
       </c>
       <c r="C28" s="7"/>
-      <c r="D28" s="89"/>
+      <c r="D28" s="91"/>
       <c r="E28" s="7"/>
-      <c r="F28" s="87" t="s">
+      <c r="F28" s="90" t="s">
         <v>25</v>
       </c>
       <c r="G28" s="7"/>
@@ -2303,12 +2303,12 @@
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
       <c r="M28" s="7"/>
-      <c r="N28" s="87" t="str">
+      <c r="N28" s="90" t="str">
         <f>P30</f>
         <v>Australia</v>
       </c>
       <c r="O28" s="7"/>
-      <c r="P28" s="89"/>
+      <c r="P28" s="91"/>
       <c r="Q28" s="7"/>
       <c r="R28" s="15" t="str">
         <f>B3</f>
@@ -2325,7 +2325,7 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
-      <c r="F29" s="88"/>
+      <c r="F29" s="92"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
@@ -2333,7 +2333,7 @@
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
-      <c r="N29" s="88"/>
+      <c r="N29" s="92"/>
       <c r="O29" s="7"/>
       <c r="P29" s="7"/>
       <c r="Q29" s="7"/>
@@ -2350,11 +2350,11 @@
         <v>Argentina</v>
       </c>
       <c r="C30" s="7"/>
-      <c r="D30" s="87" t="s">
+      <c r="D30" s="90" t="s">
         <v>25</v>
       </c>
       <c r="E30" s="7"/>
-      <c r="F30" s="89"/>
+      <c r="F30" s="91"/>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
@@ -2362,9 +2362,9 @@
       <c r="K30" s="7"/>
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
-      <c r="N30" s="89"/>
+      <c r="N30" s="91"/>
       <c r="O30" s="7"/>
-      <c r="P30" s="87" t="str">
+      <c r="P30" s="90" t="str">
         <f>R30</f>
         <v>Australia</v>
       </c>
@@ -2387,7 +2387,7 @@
         <v>Denmark</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="89"/>
+      <c r="D31" s="91"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
@@ -2404,7 +2404,7 @@
       <c r="M31" s="7"/>
       <c r="N31" s="7"/>
       <c r="O31" s="7"/>
-      <c r="P31" s="89"/>
+      <c r="P31" s="91"/>
       <c r="Q31" s="7"/>
       <c r="R31" s="15" t="str">
         <f>B9</f>
@@ -2448,7 +2448,7 @@
         <v>Germany</v>
       </c>
       <c r="C33" s="7"/>
-      <c r="D33" s="87" t="s">
+      <c r="D33" s="90" t="s">
         <v>138</v>
       </c>
       <c r="E33" s="7"/>
@@ -2462,7 +2462,7 @@
       <c r="M33" s="7"/>
       <c r="N33" s="7"/>
       <c r="O33" s="7"/>
-      <c r="P33" s="87" t="s">
+      <c r="P33" s="90" t="s">
         <v>14</v>
       </c>
       <c r="Q33" s="7"/>
@@ -2484,9 +2484,9 @@
         <v>Canada</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="89"/>
+      <c r="D34" s="91"/>
       <c r="E34" s="7"/>
-      <c r="F34" s="87" t="s">
+      <c r="F34" s="90" t="s">
         <v>12</v>
       </c>
       <c r="G34" s="7"/>
@@ -2496,11 +2496,11 @@
       <c r="K34" s="7"/>
       <c r="L34" s="7"/>
       <c r="M34" s="7"/>
-      <c r="N34" s="87" t="s">
+      <c r="N34" s="90" t="s">
         <v>14</v>
       </c>
       <c r="O34" s="7"/>
-      <c r="P34" s="89"/>
+      <c r="P34" s="91"/>
       <c r="Q34" s="7"/>
       <c r="R34" s="15" t="str">
         <f>B15</f>
@@ -2517,7 +2517,7 @@
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
-      <c r="F35" s="88"/>
+      <c r="F35" s="92"/>
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
@@ -2525,7 +2525,7 @@
       <c r="K35" s="7"/>
       <c r="L35" s="7"/>
       <c r="M35" s="7"/>
-      <c r="N35" s="88"/>
+      <c r="N35" s="92"/>
       <c r="O35" s="7"/>
       <c r="P35" s="7"/>
       <c r="Q35" s="7"/>
@@ -2542,11 +2542,11 @@
         <v>Brasil</v>
       </c>
       <c r="C36" s="7"/>
-      <c r="D36" s="87" t="s">
+      <c r="D36" s="90" t="s">
         <v>12</v>
       </c>
       <c r="E36" s="7"/>
-      <c r="F36" s="89"/>
+      <c r="F36" s="91"/>
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
       <c r="I36" s="7"/>
@@ -2554,9 +2554,9 @@
       <c r="K36" s="7"/>
       <c r="L36" s="7"/>
       <c r="M36" s="7"/>
-      <c r="N36" s="89"/>
+      <c r="N36" s="91"/>
       <c r="O36" s="7"/>
-      <c r="P36" s="87" t="s">
+      <c r="P36" s="90" t="s">
         <v>136</v>
       </c>
       <c r="Q36" s="7"/>
@@ -2578,7 +2578,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="89"/>
+      <c r="D37" s="91"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
@@ -2590,7 +2590,7 @@
       <c r="M37" s="7"/>
       <c r="N37" s="7"/>
       <c r="O37" s="7"/>
-      <c r="P37" s="89"/>
+      <c r="P37" s="91"/>
       <c r="Q37" s="7"/>
       <c r="R37" s="15" t="str">
         <f>B21</f>
@@ -2625,6 +2625,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="N28:N30"/>
+    <mergeCell ref="N34:N36"/>
+    <mergeCell ref="P27:P28"/>
+    <mergeCell ref="P30:P31"/>
+    <mergeCell ref="P33:P34"/>
+    <mergeCell ref="P36:P37"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="D27:D28"/>
     <mergeCell ref="D30:D31"/>
@@ -2634,12 +2640,6 @@
     <mergeCell ref="F34:F36"/>
     <mergeCell ref="H31:H33"/>
     <mergeCell ref="L31:L33"/>
-    <mergeCell ref="N28:N30"/>
-    <mergeCell ref="N34:N36"/>
-    <mergeCell ref="P27:P28"/>
-    <mergeCell ref="P30:P31"/>
-    <mergeCell ref="P33:P34"/>
-    <mergeCell ref="P36:P37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -2694,7 +2694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86316F4E-9A6C-492E-9EDB-018A26A821E8}">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -2726,26 +2726,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="92"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="89"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="90" t="s">
+      <c r="J1" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="91"/>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="92"/>
-      <c r="P1" s="90" t="s">
+      <c r="K1" s="88"/>
+      <c r="L1" s="88"/>
+      <c r="M1" s="88"/>
+      <c r="N1" s="89"/>
+      <c r="P1" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="91"/>
-      <c r="R1" s="92"/>
+      <c r="Q1" s="88"/>
+      <c r="R1" s="89"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -2948,23 +2948,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="104" t="s">
+      <c r="B8" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="105"/>
-      <c r="D8" s="105"/>
-      <c r="E8" s="105"/>
-      <c r="F8" s="106"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="98"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="104" t="s">
+      <c r="J8" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="105"/>
-      <c r="L8" s="105"/>
-      <c r="M8" s="105"/>
-      <c r="N8" s="106"/>
+      <c r="K8" s="97"/>
+      <c r="L8" s="97"/>
+      <c r="M8" s="97"/>
+      <c r="N8" s="98"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -3154,23 +3154,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="104" t="s">
+      <c r="B15" s="96" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="105"/>
-      <c r="D15" s="105"/>
-      <c r="E15" s="105"/>
-      <c r="F15" s="106"/>
+      <c r="C15" s="97"/>
+      <c r="D15" s="97"/>
+      <c r="E15" s="97"/>
+      <c r="F15" s="98"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="104" t="s">
+      <c r="J15" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="105"/>
-      <c r="L15" s="105"/>
-      <c r="M15" s="105"/>
-      <c r="N15" s="106"/>
+      <c r="K15" s="97"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="98"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -3291,10 +3291,10 @@
         <f t="shared" ref="N19:N20" si="5">IF(J19=L19,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Q19" s="107" t="s">
+      <c r="Q19" s="99" t="s">
         <v>82</v>
       </c>
-      <c r="R19" s="107"/>
+      <c r="R19" s="99"/>
     </row>
     <row r="20" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="27" t="s">
@@ -3349,23 +3349,23 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="104" t="s">
+      <c r="B22" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="105"/>
-      <c r="D22" s="105"/>
-      <c r="E22" s="105"/>
-      <c r="F22" s="106"/>
+      <c r="C22" s="97"/>
+      <c r="D22" s="97"/>
+      <c r="E22" s="97"/>
+      <c r="F22" s="98"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="104" t="s">
+      <c r="J22" s="96" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="105"/>
-      <c r="L22" s="105"/>
-      <c r="M22" s="105"/>
-      <c r="N22" s="106"/>
+      <c r="K22" s="97"/>
+      <c r="L22" s="97"/>
+      <c r="M22" s="97"/>
+      <c r="N22" s="98"/>
       <c r="Q22" s="49"/>
       <c r="R22" s="32" t="s">
         <v>85</v>
@@ -3596,7 +3596,7 @@
         <v>Ecuador</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="99" t="s">
+      <c r="D31" s="103" t="s">
         <v>134</v>
       </c>
       <c r="E31" s="7"/>
@@ -3614,7 +3614,7 @@
         <v>79</v>
       </c>
       <c r="O31" s="7"/>
-      <c r="P31" s="99" t="s">
+      <c r="P31" s="103" t="s">
         <v>41</v>
       </c>
       <c r="Q31" s="7"/>
@@ -3636,12 +3636,12 @@
         <v>Iran</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="100"/>
+      <c r="D32" s="104"/>
       <c r="E32" s="23">
         <f>IF(D31=Master!D27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F32" s="99" t="s">
+      <c r="F32" s="103" t="s">
         <v>25</v>
       </c>
       <c r="G32" s="7"/>
@@ -3651,7 +3651,7 @@
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
-      <c r="N32" s="99" t="str">
+      <c r="N32" s="103" t="str">
         <f>P34</f>
         <v>Australia</v>
       </c>
@@ -3659,7 +3659,7 @@
         <f>IF(P31=Master!P27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P32" s="100"/>
+      <c r="P32" s="104"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="39" t="str">
         <f>D4</f>
@@ -3678,7 +3678,7 @@
         <v>70</v>
       </c>
       <c r="E33" s="7"/>
-      <c r="F33" s="101"/>
+      <c r="F33" s="105"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
@@ -3686,7 +3686,7 @@
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
-      <c r="N33" s="101"/>
+      <c r="N33" s="105"/>
       <c r="O33" s="7"/>
       <c r="P33" s="35" t="s">
         <v>74</v>
@@ -3705,14 +3705,14 @@
         <v>Argentina</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="99" t="s">
+      <c r="D34" s="103" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="23">
         <f>IF(D34=Master!D30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F34" s="100"/>
+      <c r="F34" s="104"/>
       <c r="G34" s="23">
         <f>IF(F32=Master!F28,4,0)</f>
         <v>4</v>
@@ -3730,12 +3730,12 @@
         <f>IF(N32=Master!N28,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N34" s="100"/>
+      <c r="N34" s="104"/>
       <c r="O34" s="23">
         <f>IF(P34=Master!P30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P34" s="99" t="s">
+      <c r="P34" s="103" t="s">
         <v>35</v>
       </c>
       <c r="Q34" s="7"/>
@@ -3757,11 +3757,11 @@
         <v>Denmark</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="100"/>
+      <c r="D35" s="104"/>
       <c r="E35" s="7"/>
       <c r="F35" s="35"/>
       <c r="G35" s="7"/>
-      <c r="H35" s="99" t="s">
+      <c r="H35" s="103" t="s">
         <v>25</v>
       </c>
       <c r="I35" s="7"/>
@@ -3769,14 +3769,14 @@
         <v>81</v>
       </c>
       <c r="K35" s="7"/>
-      <c r="L35" s="99" t="str">
+      <c r="L35" s="103" t="str">
         <f>N32</f>
         <v>Australia</v>
       </c>
       <c r="M35" s="7"/>
       <c r="N35" s="35"/>
       <c r="O35" s="7"/>
-      <c r="P35" s="100"/>
+      <c r="P35" s="104"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="39" t="str">
         <f>D11</f>
@@ -3797,7 +3797,7 @@
       <c r="E36" s="7"/>
       <c r="F36" s="35"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="101"/>
+      <c r="H36" s="105"/>
       <c r="I36" s="24">
         <f>IF(H35=Master!H31,6,0)</f>
         <v>6</v>
@@ -3809,7 +3809,7 @@
         <f>IF(L35=Master!L31,6,0)</f>
         <v>6</v>
       </c>
-      <c r="L36" s="101"/>
+      <c r="L36" s="105"/>
       <c r="M36" s="7"/>
       <c r="N36" s="35"/>
       <c r="O36" s="7"/>
@@ -3830,7 +3830,7 @@
         <v>Germany</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="102" t="s">
+      <c r="D37" s="106" t="s">
         <v>138</v>
       </c>
       <c r="E37" s="7"/>
@@ -3838,17 +3838,17 @@
         <v>78</v>
       </c>
       <c r="G37" s="7"/>
-      <c r="H37" s="100"/>
+      <c r="H37" s="104"/>
       <c r="I37" s="7"/>
       <c r="J37" s="35"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="100"/>
+      <c r="L37" s="104"/>
       <c r="M37" s="7"/>
       <c r="N37" s="35" t="s">
         <v>80</v>
       </c>
       <c r="O37" s="7"/>
-      <c r="P37" s="99" t="s">
+      <c r="P37" s="103" t="s">
         <v>14</v>
       </c>
       <c r="Q37" s="7"/>
@@ -3870,12 +3870,12 @@
         <v>Canada</v>
       </c>
       <c r="C38" s="7"/>
-      <c r="D38" s="103"/>
+      <c r="D38" s="107"/>
       <c r="E38" s="23">
         <f>IF(D37=Master!D33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F38" s="96" t="s">
+      <c r="F38" s="100" t="s">
         <v>12</v>
       </c>
       <c r="G38" s="23">
@@ -3894,14 +3894,14 @@
         <f>IF(N38=Master!N34,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N38" s="99" t="s">
+      <c r="N38" s="103" t="s">
         <v>14</v>
       </c>
       <c r="O38" s="23">
         <f>IF(P37=Master!P33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P38" s="100"/>
+      <c r="P38" s="104"/>
       <c r="Q38" s="7"/>
       <c r="R38" s="39" t="str">
         <f>D18</f>
@@ -3920,7 +3920,7 @@
         <v>72</v>
       </c>
       <c r="E39" s="7"/>
-      <c r="F39" s="97"/>
+      <c r="F39" s="101"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
@@ -3928,7 +3928,7 @@
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
-      <c r="N39" s="101"/>
+      <c r="N39" s="105"/>
       <c r="O39" s="7"/>
       <c r="P39" s="35" t="s">
         <v>76</v>
@@ -3947,14 +3947,14 @@
         <v>Brasil</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="99" t="s">
+      <c r="D40" s="103" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="23">
         <f>IF(D40=Master!D36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F40" s="98"/>
+      <c r="F40" s="102"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
@@ -3962,12 +3962,12 @@
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
-      <c r="N40" s="100"/>
+      <c r="N40" s="104"/>
       <c r="O40" s="23">
         <f>IF(P40=Master!P36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P40" s="99" t="s">
+      <c r="P40" s="103" t="s">
         <v>136</v>
       </c>
       <c r="Q40" s="7"/>
@@ -3989,7 +3989,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="100"/>
+      <c r="D41" s="104"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -4001,7 +4001,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="100"/>
+      <c r="P41" s="104"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="39" t="str">
         <f>D25</f>
@@ -4069,16 +4069,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J22:N22"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="J8:N8"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="Q19:R19"/>
     <mergeCell ref="F38:F40"/>
     <mergeCell ref="P37:P38"/>
     <mergeCell ref="P40:P41"/>
@@ -4093,6 +4083,16 @@
     <mergeCell ref="D37:D38"/>
     <mergeCell ref="H35:H37"/>
     <mergeCell ref="L35:L37"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J22:N22"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="Q19:R19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -4103,7 +4103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69337711-055D-1241-BEB8-C726DCD4CFE4}">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
@@ -4135,26 +4135,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="92"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="89"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="90" t="s">
+      <c r="J1" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="91"/>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="92"/>
-      <c r="P1" s="90" t="s">
+      <c r="K1" s="88"/>
+      <c r="L1" s="88"/>
+      <c r="M1" s="88"/>
+      <c r="N1" s="89"/>
+      <c r="P1" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="91"/>
-      <c r="R1" s="92"/>
+      <c r="Q1" s="88"/>
+      <c r="R1" s="89"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -4357,23 +4357,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="104" t="s">
+      <c r="B8" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="105"/>
-      <c r="D8" s="105"/>
-      <c r="E8" s="105"/>
-      <c r="F8" s="106"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="98"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="104" t="s">
+      <c r="J8" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="105"/>
-      <c r="L8" s="105"/>
-      <c r="M8" s="105"/>
-      <c r="N8" s="106"/>
+      <c r="K8" s="97"/>
+      <c r="L8" s="97"/>
+      <c r="M8" s="97"/>
+      <c r="N8" s="98"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -4563,23 +4563,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="104" t="s">
+      <c r="B15" s="96" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="105"/>
-      <c r="D15" s="105"/>
-      <c r="E15" s="105"/>
-      <c r="F15" s="106"/>
+      <c r="C15" s="97"/>
+      <c r="D15" s="97"/>
+      <c r="E15" s="97"/>
+      <c r="F15" s="98"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="104" t="s">
+      <c r="J15" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="105"/>
-      <c r="L15" s="105"/>
-      <c r="M15" s="105"/>
-      <c r="N15" s="106"/>
+      <c r="K15" s="97"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="98"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -4700,10 +4700,10 @@
         <f t="shared" ref="N19:N20" si="5">IF(J19=L19,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Q19" s="107" t="s">
+      <c r="Q19" s="99" t="s">
         <v>82</v>
       </c>
-      <c r="R19" s="107"/>
+      <c r="R19" s="99"/>
     </row>
     <row r="20" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="27" t="s">
@@ -4758,23 +4758,23 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="104" t="s">
+      <c r="B22" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="105"/>
-      <c r="D22" s="105"/>
-      <c r="E22" s="105"/>
-      <c r="F22" s="106"/>
+      <c r="C22" s="97"/>
+      <c r="D22" s="97"/>
+      <c r="E22" s="97"/>
+      <c r="F22" s="98"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="104" t="s">
+      <c r="J22" s="96" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="105"/>
-      <c r="L22" s="105"/>
-      <c r="M22" s="105"/>
-      <c r="N22" s="106"/>
+      <c r="K22" s="97"/>
+      <c r="L22" s="97"/>
+      <c r="M22" s="97"/>
+      <c r="N22" s="98"/>
       <c r="Q22" s="49"/>
       <c r="R22" s="32" t="s">
         <v>85</v>
@@ -5005,7 +5005,7 @@
         <v>Ecuador</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="99" t="s">
+      <c r="D31" s="103" t="s">
         <v>134</v>
       </c>
       <c r="E31" s="7"/>
@@ -5023,7 +5023,7 @@
         <v>79</v>
       </c>
       <c r="O31" s="7"/>
-      <c r="P31" s="99" t="s">
+      <c r="P31" s="103" t="s">
         <v>41</v>
       </c>
       <c r="Q31" s="7"/>
@@ -5045,12 +5045,12 @@
         <v>Iran</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="100"/>
+      <c r="D32" s="104"/>
       <c r="E32" s="23">
         <f>IF(D31=Master!D27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F32" s="99" t="s">
+      <c r="F32" s="103" t="s">
         <v>25</v>
       </c>
       <c r="G32" s="7"/>
@@ -5060,7 +5060,7 @@
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
-      <c r="N32" s="99" t="str">
+      <c r="N32" s="103" t="str">
         <f>P34</f>
         <v>Australia</v>
       </c>
@@ -5068,7 +5068,7 @@
         <f>IF(P31=Master!P27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P32" s="100"/>
+      <c r="P32" s="104"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="81" t="str">
         <f>D4</f>
@@ -5087,7 +5087,7 @@
         <v>70</v>
       </c>
       <c r="E33" s="7"/>
-      <c r="F33" s="101"/>
+      <c r="F33" s="105"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
@@ -5095,7 +5095,7 @@
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
-      <c r="N33" s="101"/>
+      <c r="N33" s="105"/>
       <c r="O33" s="7"/>
       <c r="P33" s="35"/>
       <c r="Q33" s="7"/>
@@ -5112,14 +5112,14 @@
         <v>Argentina</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="99" t="s">
+      <c r="D34" s="103" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="23">
         <f>IF(D34=Master!D30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F34" s="100"/>
+      <c r="F34" s="104"/>
       <c r="G34" s="23">
         <f>IF(F32=Master!F28,4,0)</f>
         <v>4</v>
@@ -5137,12 +5137,12 @@
         <f>IF(N32=Master!N28,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N34" s="100"/>
+      <c r="N34" s="104"/>
       <c r="O34" s="23">
         <f>IF(P34=Master!P30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P34" s="99" t="s">
+      <c r="P34" s="103" t="s">
         <v>35</v>
       </c>
       <c r="Q34" s="7"/>
@@ -5164,11 +5164,11 @@
         <v>Denmark</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="100"/>
+      <c r="D35" s="104"/>
       <c r="E35" s="7"/>
       <c r="F35" s="35"/>
       <c r="G35" s="7"/>
-      <c r="H35" s="99" t="s">
+      <c r="H35" s="103" t="s">
         <v>25</v>
       </c>
       <c r="I35" s="7"/>
@@ -5176,14 +5176,14 @@
         <v>81</v>
       </c>
       <c r="K35" s="7"/>
-      <c r="L35" s="99" t="str">
+      <c r="L35" s="103" t="str">
         <f>N32</f>
         <v>Australia</v>
       </c>
       <c r="M35" s="7"/>
       <c r="N35" s="35"/>
       <c r="O35" s="7"/>
-      <c r="P35" s="100"/>
+      <c r="P35" s="104"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="81" t="str">
         <f>D11</f>
@@ -5204,7 +5204,7 @@
       <c r="E36" s="7"/>
       <c r="F36" s="35"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="101"/>
+      <c r="H36" s="105"/>
       <c r="I36" s="24">
         <f>IF(H35=Master!H31,6,0)</f>
         <v>6</v>
@@ -5216,7 +5216,7 @@
         <f>IF(L35=Master!L31,6,0)</f>
         <v>6</v>
       </c>
-      <c r="L36" s="101"/>
+      <c r="L36" s="105"/>
       <c r="M36" s="7"/>
       <c r="N36" s="35"/>
       <c r="O36" s="7"/>
@@ -5237,7 +5237,7 @@
         <v>Germany</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="102" t="s">
+      <c r="D37" s="106" t="s">
         <v>138</v>
       </c>
       <c r="E37" s="7"/>
@@ -5245,17 +5245,17 @@
         <v>78</v>
       </c>
       <c r="G37" s="7"/>
-      <c r="H37" s="100"/>
+      <c r="H37" s="104"/>
       <c r="I37" s="7"/>
       <c r="J37" s="35"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="100"/>
+      <c r="L37" s="104"/>
       <c r="M37" s="7"/>
       <c r="N37" s="35" t="s">
         <v>80</v>
       </c>
       <c r="O37" s="7"/>
-      <c r="P37" s="99" t="s">
+      <c r="P37" s="103" t="s">
         <v>14</v>
       </c>
       <c r="Q37" s="7"/>
@@ -5277,12 +5277,12 @@
         <v>Canada</v>
       </c>
       <c r="C38" s="7"/>
-      <c r="D38" s="103"/>
+      <c r="D38" s="107"/>
       <c r="E38" s="23">
         <f>IF(D37=Master!D33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F38" s="96" t="s">
+      <c r="F38" s="100" t="s">
         <v>12</v>
       </c>
       <c r="G38" s="23">
@@ -5301,14 +5301,14 @@
         <f>IF(N38=Master!N34,4,0)</f>
         <v>4</v>
       </c>
-      <c r="N38" s="99" t="s">
+      <c r="N38" s="103" t="s">
         <v>14</v>
       </c>
       <c r="O38" s="23">
         <f>IF(P37=Master!P33,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P38" s="100"/>
+      <c r="P38" s="104"/>
       <c r="Q38" s="7"/>
       <c r="R38" s="81" t="str">
         <f>D18</f>
@@ -5327,7 +5327,7 @@
         <v>72</v>
       </c>
       <c r="E39" s="7"/>
-      <c r="F39" s="97"/>
+      <c r="F39" s="101"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
@@ -5335,7 +5335,7 @@
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
-      <c r="N39" s="101"/>
+      <c r="N39" s="105"/>
       <c r="O39" s="7"/>
       <c r="P39" s="35" t="s">
         <v>76</v>
@@ -5354,14 +5354,14 @@
         <v>Brasil</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="99" t="s">
+      <c r="D40" s="103" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="23">
         <f>IF(D40=Master!D36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F40" s="98"/>
+      <c r="F40" s="102"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
@@ -5369,12 +5369,12 @@
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
-      <c r="N40" s="100"/>
+      <c r="N40" s="104"/>
       <c r="O40" s="23">
         <f>IF(P40=Master!P36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P40" s="99" t="s">
+      <c r="P40" s="103" t="s">
         <v>136</v>
       </c>
       <c r="Q40" s="7"/>
@@ -5396,7 +5396,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="100"/>
+      <c r="D41" s="104"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -5408,7 +5408,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="100"/>
+      <c r="P41" s="104"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="81" t="str">
         <f>D25</f>
@@ -5476,14 +5476,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="P34:P35"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="L35:L37"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="P37:P38"/>
-    <mergeCell ref="F38:F40"/>
-    <mergeCell ref="N38:N40"/>
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="J8:N8"/>
@@ -5500,6 +5492,14 @@
     <mergeCell ref="P31:P32"/>
     <mergeCell ref="F32:F34"/>
     <mergeCell ref="N32:N34"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="P34:P35"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="L35:L37"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="P37:P38"/>
+    <mergeCell ref="F38:F40"/>
+    <mergeCell ref="N38:N40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -5510,7 +5510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C64DF09A-2D3C-4C49-8B16-319C8D3CEDC7}">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
@@ -5539,26 +5539,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="92"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="89"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="90" t="s">
+      <c r="J1" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="91"/>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="92"/>
-      <c r="P1" s="90" t="s">
+      <c r="K1" s="88"/>
+      <c r="L1" s="88"/>
+      <c r="M1" s="88"/>
+      <c r="N1" s="89"/>
+      <c r="P1" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="91"/>
-      <c r="R1" s="92"/>
+      <c r="Q1" s="88"/>
+      <c r="R1" s="89"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -5761,23 +5761,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="104" t="s">
+      <c r="B8" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="105"/>
-      <c r="D8" s="105"/>
-      <c r="E8" s="105"/>
-      <c r="F8" s="106"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="98"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="104" t="s">
+      <c r="J8" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="105"/>
-      <c r="L8" s="105"/>
-      <c r="M8" s="105"/>
-      <c r="N8" s="106"/>
+      <c r="K8" s="97"/>
+      <c r="L8" s="97"/>
+      <c r="M8" s="97"/>
+      <c r="N8" s="98"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -5967,23 +5967,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="104" t="s">
+      <c r="B15" s="96" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="105"/>
-      <c r="D15" s="105"/>
-      <c r="E15" s="105"/>
-      <c r="F15" s="106"/>
+      <c r="C15" s="97"/>
+      <c r="D15" s="97"/>
+      <c r="E15" s="97"/>
+      <c r="F15" s="98"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="104" t="s">
+      <c r="J15" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="105"/>
-      <c r="L15" s="105"/>
-      <c r="M15" s="105"/>
-      <c r="N15" s="106"/>
+      <c r="K15" s="97"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="98"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -6148,23 +6148,23 @@
       <c r="N21" s="52"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="104" t="s">
+      <c r="B22" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="105"/>
-      <c r="D22" s="105"/>
-      <c r="E22" s="105"/>
-      <c r="F22" s="106"/>
+      <c r="C22" s="97"/>
+      <c r="D22" s="97"/>
+      <c r="E22" s="97"/>
+      <c r="F22" s="98"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="104" t="s">
+      <c r="J22" s="96" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="105"/>
-      <c r="L22" s="105"/>
-      <c r="M22" s="105"/>
-      <c r="N22" s="106"/>
+      <c r="K22" s="97"/>
+      <c r="L22" s="97"/>
+      <c r="M22" s="97"/>
+      <c r="N22" s="98"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B23" s="56" t="s">
@@ -6403,7 +6403,7 @@
         <v>79</v>
       </c>
       <c r="O31" s="7"/>
-      <c r="P31" s="99" t="s">
+      <c r="P31" s="103" t="s">
         <v>41</v>
       </c>
       <c r="Q31" s="7"/>
@@ -6447,7 +6447,7 @@
         <f>IF(P31=Master!P27,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P32" s="100"/>
+      <c r="P32" s="104"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="39" t="str">
         <f>D4</f>
@@ -6493,7 +6493,7 @@
         <v>Argentina</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="99" t="s">
+      <c r="D34" s="103" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="23">
@@ -6523,7 +6523,7 @@
         <f>IF(P34=Master!P30,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P34" s="99" t="s">
+      <c r="P34" s="103" t="s">
         <v>35</v>
       </c>
       <c r="Q34" s="7"/>
@@ -6545,7 +6545,7 @@
         <v>Denmark</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="100"/>
+      <c r="D35" s="104"/>
       <c r="E35" s="7"/>
       <c r="F35" s="35"/>
       <c r="G35" s="7"/>
@@ -6564,7 +6564,7 @@
       <c r="M35" s="7"/>
       <c r="N35" s="35"/>
       <c r="O35" s="7"/>
-      <c r="P35" s="100"/>
+      <c r="P35" s="104"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="39" t="str">
         <f>D11</f>
@@ -6618,7 +6618,7 @@
         <v>Germany</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="102" t="s">
+      <c r="D37" s="106" t="s">
         <v>138</v>
       </c>
       <c r="E37" s="7"/>
@@ -6658,7 +6658,7 @@
         <v>Canada</v>
       </c>
       <c r="C38" s="7"/>
-      <c r="D38" s="103"/>
+      <c r="D38" s="107"/>
       <c r="E38" s="23">
         <f>IF(D37=Master!D33,2,0)</f>
         <v>2</v>
@@ -6736,7 +6736,7 @@
         <v>Brasil</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="99" t="s">
+      <c r="D40" s="103" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="23">
@@ -6756,7 +6756,7 @@
         <f>IF(P40=Master!P36,2,0)</f>
         <v>2</v>
       </c>
-      <c r="P40" s="99" t="s">
+      <c r="P40" s="103" t="s">
         <v>136</v>
       </c>
       <c r="Q40" s="7"/>
@@ -6778,7 +6778,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="100"/>
+      <c r="D41" s="104"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -6790,7 +6790,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="100"/>
+      <c r="P41" s="104"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="39" t="str">
         <f>D25</f>
@@ -6858,6 +6858,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="J8:N8"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="D31:D32"/>
@@ -6874,13 +6881,6 @@
     <mergeCell ref="N38:N40"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="P40:P41"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="J8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -6891,7 +6891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB731263-BF9E-B94A-B168-4AE30BA7699C}">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
@@ -6920,26 +6920,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="92"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="89"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="90" t="s">
+      <c r="J1" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="91"/>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="92"/>
-      <c r="P1" s="90" t="s">
+      <c r="K1" s="88"/>
+      <c r="L1" s="88"/>
+      <c r="M1" s="88"/>
+      <c r="N1" s="89"/>
+      <c r="P1" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="91"/>
-      <c r="R1" s="92"/>
+      <c r="Q1" s="88"/>
+      <c r="R1" s="89"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -7142,23 +7142,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="104" t="s">
+      <c r="B8" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="105"/>
-      <c r="D8" s="105"/>
-      <c r="E8" s="105"/>
-      <c r="F8" s="106"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="98"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="104" t="s">
+      <c r="J8" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="105"/>
-      <c r="L8" s="105"/>
-      <c r="M8" s="105"/>
-      <c r="N8" s="106"/>
+      <c r="K8" s="97"/>
+      <c r="L8" s="97"/>
+      <c r="M8" s="97"/>
+      <c r="N8" s="98"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -7348,23 +7348,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="104" t="s">
+      <c r="B15" s="96" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="105"/>
-      <c r="D15" s="105"/>
-      <c r="E15" s="105"/>
-      <c r="F15" s="106"/>
+      <c r="C15" s="97"/>
+      <c r="D15" s="97"/>
+      <c r="E15" s="97"/>
+      <c r="F15" s="98"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="104" t="s">
+      <c r="J15" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="105"/>
-      <c r="L15" s="105"/>
-      <c r="M15" s="105"/>
-      <c r="N15" s="106"/>
+      <c r="K15" s="97"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="98"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -7531,23 +7531,23 @@
       <c r="N21" s="52"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="104" t="s">
+      <c r="B22" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="105"/>
-      <c r="D22" s="105"/>
-      <c r="E22" s="105"/>
-      <c r="F22" s="106"/>
+      <c r="C22" s="97"/>
+      <c r="D22" s="97"/>
+      <c r="E22" s="97"/>
+      <c r="F22" s="98"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="104" t="s">
+      <c r="J22" s="96" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="105"/>
-      <c r="L22" s="105"/>
-      <c r="M22" s="105"/>
-      <c r="N22" s="106"/>
+      <c r="K22" s="97"/>
+      <c r="L22" s="97"/>
+      <c r="M22" s="97"/>
+      <c r="N22" s="98"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B23" s="56" t="s">
@@ -8119,7 +8119,7 @@
         <v>Brasil</v>
       </c>
       <c r="C40" s="7"/>
-      <c r="D40" s="99" t="s">
+      <c r="D40" s="103" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="23">
@@ -8161,7 +8161,7 @@
         <v>Korea Republic</v>
       </c>
       <c r="C41" s="7"/>
-      <c r="D41" s="100"/>
+      <c r="D41" s="104"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -8241,6 +8241,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="J8:N8"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="D31:D32"/>
@@ -8257,13 +8264,6 @@
     <mergeCell ref="N38:N40"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="P40:P41"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="J8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -8303,26 +8303,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="92"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="89"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="90" t="s">
+      <c r="J1" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="91"/>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="92"/>
-      <c r="P1" s="90" t="s">
+      <c r="K1" s="88"/>
+      <c r="L1" s="88"/>
+      <c r="M1" s="88"/>
+      <c r="N1" s="89"/>
+      <c r="P1" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="91"/>
-      <c r="R1" s="92"/>
+      <c r="Q1" s="88"/>
+      <c r="R1" s="89"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="56" t="s">
@@ -8525,23 +8525,23 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B8" s="104" t="s">
+      <c r="B8" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="105"/>
-      <c r="D8" s="105"/>
-      <c r="E8" s="105"/>
-      <c r="F8" s="106"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="98"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="104" t="s">
+      <c r="J8" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="105"/>
-      <c r="L8" s="105"/>
-      <c r="M8" s="105"/>
-      <c r="N8" s="106"/>
+      <c r="K8" s="97"/>
+      <c r="L8" s="97"/>
+      <c r="M8" s="97"/>
+      <c r="N8" s="98"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -8731,23 +8731,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="104" t="s">
+      <c r="B15" s="96" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="105"/>
-      <c r="D15" s="105"/>
-      <c r="E15" s="105"/>
-      <c r="F15" s="106"/>
+      <c r="C15" s="97"/>
+      <c r="D15" s="97"/>
+      <c r="E15" s="97"/>
+      <c r="F15" s="98"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="104" t="s">
+      <c r="J15" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="105"/>
-      <c r="L15" s="105"/>
-      <c r="M15" s="105"/>
-      <c r="N15" s="106"/>
+      <c r="K15" s="97"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="98"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -8918,23 +8918,23 @@
       <c r="N21" s="52"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="104" t="s">
+      <c r="B22" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="105"/>
-      <c r="D22" s="105"/>
-      <c r="E22" s="105"/>
-      <c r="F22" s="106"/>
+      <c r="C22" s="97"/>
+      <c r="D22" s="97"/>
+      <c r="E22" s="97"/>
+      <c r="F22" s="98"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="104" t="s">
+      <c r="J22" s="96" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="105"/>
-      <c r="L22" s="105"/>
-      <c r="M22" s="105"/>
-      <c r="N22" s="106"/>
+      <c r="K22" s="97"/>
+      <c r="L22" s="97"/>
+      <c r="M22" s="97"/>
+      <c r="N22" s="98"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B23" s="56" t="s">
@@ -9631,6 +9631,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="J8:N8"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="D31:D32"/>
@@ -9647,13 +9654,6 @@
     <mergeCell ref="N38:N40"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="P40:P41"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="J8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -9771,26 +9771,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="92"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="89"/>
       <c r="H1" s="7"/>
-      <c r="J1" s="90" t="s">
+      <c r="J1" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="91"/>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="92"/>
-      <c r="P1" s="90" t="s">
+      <c r="K1" s="88"/>
+      <c r="L1" s="88"/>
+      <c r="M1" s="88"/>
+      <c r="N1" s="89"/>
+      <c r="P1" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="91"/>
-      <c r="R1" s="92"/>
+      <c r="Q1" s="88"/>
+      <c r="R1" s="89"/>
       <c r="W1" s="1" t="s">
         <v>92</v>
       </c>
@@ -10098,23 +10098,23 @@
       </c>
     </row>
     <row r="8" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B8" s="104" t="s">
+      <c r="B8" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="105"/>
-      <c r="D8" s="105"/>
-      <c r="E8" s="105"/>
-      <c r="F8" s="106"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="98"/>
       <c r="G8" s="52"/>
       <c r="H8" s="55"/>
       <c r="I8" s="52"/>
-      <c r="J8" s="104" t="s">
+      <c r="J8" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="105"/>
-      <c r="L8" s="105"/>
-      <c r="M8" s="105"/>
-      <c r="N8" s="106"/>
+      <c r="K8" s="97"/>
+      <c r="L8" s="97"/>
+      <c r="M8" s="97"/>
+      <c r="N8" s="98"/>
       <c r="P8" s="16" t="s">
         <v>59</v>
       </c>
@@ -10402,23 +10402,23 @@
       <c r="N14" s="52"/>
     </row>
     <row r="15" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B15" s="104" t="s">
+      <c r="B15" s="96" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="105"/>
-      <c r="D15" s="105"/>
-      <c r="E15" s="105"/>
-      <c r="F15" s="106"/>
+      <c r="C15" s="97"/>
+      <c r="D15" s="97"/>
+      <c r="E15" s="97"/>
+      <c r="F15" s="98"/>
       <c r="G15" s="52"/>
       <c r="H15" s="35"/>
       <c r="I15" s="52"/>
-      <c r="J15" s="104" t="s">
+      <c r="J15" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="105"/>
-      <c r="L15" s="105"/>
-      <c r="M15" s="105"/>
-      <c r="N15" s="106"/>
+      <c r="K15" s="97"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="98"/>
     </row>
     <row r="16" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B16" s="56" t="s">
@@ -10683,23 +10683,23 @@
       <c r="N21" s="52"/>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B22" s="104" t="s">
+      <c r="B22" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="105"/>
-      <c r="D22" s="105"/>
-      <c r="E22" s="105"/>
-      <c r="F22" s="106"/>
+      <c r="C22" s="97"/>
+      <c r="D22" s="97"/>
+      <c r="E22" s="97"/>
+      <c r="F22" s="98"/>
       <c r="G22" s="52"/>
       <c r="H22" s="35"/>
       <c r="I22" s="52"/>
-      <c r="J22" s="104" t="s">
+      <c r="J22" s="96" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="105"/>
-      <c r="L22" s="105"/>
-      <c r="M22" s="105"/>
-      <c r="N22" s="106"/>
+      <c r="K22" s="97"/>
+      <c r="L22" s="97"/>
+      <c r="M22" s="97"/>
+      <c r="N22" s="98"/>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B23" s="56" t="s">
@@ -11473,13 +11473,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="J8:N8"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="D31:D32"/>
@@ -11496,6 +11489,13 @@
     <mergeCell ref="N38:N40"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="P40:P41"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="J8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -11506,7 +11506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12EDD3BB-E2B5-AA49-89B4-1F42796E5997}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
+    <sheetView zoomScale="132" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>